<commit_message>
Atualização da tabela de buscas locais
</commit_message>
<xml_diff>
--- a/Comparaçoes/BuscasLocais.xlsx
+++ b/Comparaçoes/BuscasLocais.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="0" userName="pdezi"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="2" xWindow="240" yWindow="60" windowWidth="9570" windowHeight="8265" tabRatio="500"/>
+    <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="9570" windowHeight="8265" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="k = n|4" sheetId="1" r:id="rId4"/>
@@ -15,17 +15,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1643199832" val="1042" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1643199832" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1643199832" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1643199832"/>
+      <pm:revision xmlns:pm="smNativeData" day="1643203916" val="1042" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1643203916" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1643203916" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1643203916"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="86">
   <si>
     <t>Solução original</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>pr152</t>
+  </si>
+  <si>
+    <t>15403.26</t>
   </si>
   <si>
     <t>berlin52</t>
@@ -278,6 +281,9 @@
   <si>
     <t>k = 3n/4</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
@@ -307,7 +313,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643199832" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -322,7 +328,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643199832" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -337,7 +343,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643199832" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -352,7 +358,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643199832" fgClr="FFFFFF" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="FFFFFF" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -368,7 +374,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643199832" fgClr="FFFFFF" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="FFFFFF" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
@@ -384,7 +390,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643199832" fgClr="FA7D00" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="FA7D00" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
@@ -399,7 +405,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643199832" fgClr="FA7D00" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="FA7D00" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -415,7 +421,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643199832" fgClr="800080" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="800080" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -431,7 +437,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643199832" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -447,7 +453,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643199832" fgClr="7F7F7F" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="7F7F7F" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" i="1"/>
             <pm:cs face="Times New Roman" sz="220" lang="default" i="1"/>
             <pm:ea face="SimSun" sz="220" lang="default" i="1"/>
@@ -462,7 +468,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643199832" fgClr="FF0000" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="FF0000" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -478,7 +484,7 @@
       <sz val="18"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643199832" fgClr="44546A" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="44546A" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="360" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="360" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="360" lang="default" weight="bold"/>
@@ -493,7 +499,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643199832" fgClr="9C6500" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="9C6500" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -509,7 +515,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643199832" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
@@ -525,7 +531,7 @@
       <sz val="15"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643199832" fgClr="44546A" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="44546A" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="300" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="300" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="300" lang="default" weight="bold"/>
@@ -541,7 +547,7 @@
       <sz val="13"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643199832" fgClr="44546A" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="44546A" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="260" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="260" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="260" lang="default" weight="bold"/>
@@ -557,7 +563,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643199832" fgClr="44546A" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="44546A" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
@@ -573,7 +579,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643199832" fgClr="3F3F3F" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="3F3F3F" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
@@ -588,7 +594,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643199832" fgClr="3F3F76" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="3F3F76" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -603,7 +609,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643199832" fgClr="006100" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="006100" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -618,7 +624,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643199832" fgClr="9C0006" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="9C0006" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -640,7 +646,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00FFE697" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00FFE697" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -654,7 +660,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00A5A5A5" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00A5A5A5" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -665,7 +671,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00EBEBEB" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00EBEBEB" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -676,7 +682,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00F8CAAB" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00F8CAAB" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -687,7 +693,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -698,7 +704,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00C5DFB3" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00C5DFB3" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -709,7 +715,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00A5A5A5" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00A5A5A5" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -723,7 +729,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00FFC000" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00FFC000" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -734,7 +740,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="004472C4" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="004472C4" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -748,7 +754,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="0070AD47" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="0070AD47" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -759,7 +765,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00FFCC99" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00FFCC99" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -770,7 +776,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00F2F2F2" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00F2F2F2" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -781,7 +787,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00F2F2F2" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00F2F2F2" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -795,7 +801,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00BDD7EE" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00BDD7EE" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -806,7 +812,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00C6EFCE" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00C6EFCE" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -817,7 +823,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00FFC7CE" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00FFC7CE" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -828,7 +834,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00FFEB9C" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00FFEB9C" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -839,7 +845,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00D9E1F2" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00D9E1F2" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -850,7 +856,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="005B9BD5" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="005B9BD5" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -861,7 +867,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00DDEBF7" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00DDEBF7" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -872,7 +878,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="009BC2E6" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="009BC2E6" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -883,7 +889,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00E1EFD8" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00E1EFD8" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -894,7 +900,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00ED7D31" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00ED7D31" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -905,7 +911,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00FBE3D5" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00FBE3D5" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -916,7 +922,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00F4AF82" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00F4AF82" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -927,7 +933,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00D9D9D9" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00D9D9D9" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -938,7 +944,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00C7C7C7" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00C7C7C7" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -949,7 +955,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00FFF2CA" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00FFF2CA" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -960,7 +966,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00FFD964" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00FFD964" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -971,7 +977,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00B4C6E7" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00B4C6E7" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -982,7 +988,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="008EA9DB" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="008EA9DB" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -993,7 +999,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00A8D08C" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00A8D08C" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1007,7 +1013,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1018,7 +1024,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643199832" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1040,7 +1046,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1059,7 +1065,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1078,7 +1084,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832">
+          <pm:border xmlns:pm="smNativeData" id="1643203916">
             <pm:line position="bottom" type="2" style="0" width="20" dist="20" width2="20" rgb="FF8001"/>
           </pm:border>
         </ext>
@@ -1099,7 +1105,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832">
+          <pm:border xmlns:pm="smNativeData" id="1643203916">
             <pm:line position="top" type="2" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
             <pm:line position="bottom" type="2" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
             <pm:line position="left" type="2" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
@@ -1123,7 +1129,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1142,7 +1148,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1161,7 +1167,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832">
+          <pm:border xmlns:pm="smNativeData" id="1643203916">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
@@ -1185,7 +1191,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1204,7 +1210,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1223,7 +1229,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832">
+          <pm:border xmlns:pm="smNativeData" id="1643203916">
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="5B9BD5"/>
           </pm:border>
         </ext>
@@ -1244,7 +1250,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1263,7 +1269,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1282,7 +1288,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832">
+          <pm:border xmlns:pm="smNativeData" id="1643203916">
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="ACCCEA"/>
           </pm:border>
         </ext>
@@ -1303,7 +1309,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1322,7 +1328,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832">
+          <pm:border xmlns:pm="smNativeData" id="1643203916">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
@@ -1346,7 +1352,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832">
+          <pm:border xmlns:pm="smNativeData" id="1643203916">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
@@ -1370,7 +1376,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832">
+          <pm:border xmlns:pm="smNativeData" id="1643203916">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
@@ -1394,7 +1400,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832">
+          <pm:border xmlns:pm="smNativeData" id="1643203916">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="5B9BD5"/>
             <pm:line position="bottom" type="2" style="0" width="20" dist="20" width2="20" rgb="5B9BD5"/>
           </pm:border>
@@ -1416,7 +1422,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1435,7 +1441,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1454,7 +1460,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1473,7 +1479,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1492,7 +1498,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1511,7 +1517,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1530,7 +1536,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1549,7 +1555,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1568,7 +1574,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1587,7 +1593,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1606,7 +1612,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1625,7 +1631,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1644,7 +1650,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1663,7 +1669,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1682,7 +1688,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1701,7 +1707,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1720,7 +1726,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1739,7 +1745,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1758,7 +1764,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -1777,7 +1783,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832">
+          <pm:border xmlns:pm="smNativeData" id="1643203916">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1801,7 +1807,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832">
+          <pm:border xmlns:pm="smNativeData" id="1643203916">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1825,7 +1831,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643199832"/>
+          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
         </ext>
       </extLst>
     </border>
@@ -2203,10 +2209,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1643199832" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1643203916" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1643199832" count="41">
+      <pm:colors xmlns:pm="smNativeData" id="1643203916" count="41">
         <pm:color name="Cor 24" rgb="FA7D00"/>
         <pm:color name="Cor 25" rgb="800080"/>
         <pm:color name="Cor 26" rgb="44546A"/>
@@ -2512,8 +2518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AJ28"/>
   <sheetViews>
-    <sheetView view="normal" topLeftCell="N4" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="Z4" zoomScale="90" workbookViewId="0">
+      <selection activeCell="AH29" sqref="AH29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.20"/>
@@ -2764,7 +2770,9 @@
       <c r="I5" s="55" t="n">
         <v>683.649999999999977</v>
       </c>
-      <c r="J5" s="55"/>
+      <c r="J5" s="55" t="n">
+        <v>707.340000000000032</v>
+      </c>
       <c r="K5" s="55"/>
       <c r="L5" s="55"/>
       <c r="N5" s="51" t="s">
@@ -2791,7 +2799,9 @@
       <c r="U5" s="55" t="n">
         <v>558</v>
       </c>
-      <c r="V5" s="55"/>
+      <c r="V5" s="55" t="n">
+        <v>582</v>
+      </c>
       <c r="W5" s="55"/>
       <c r="X5" s="55"/>
       <c r="Z5" s="51" t="s">
@@ -2818,7 +2828,9 @@
       <c r="AG5" s="55" t="n">
         <v>25126.8400000000001</v>
       </c>
-      <c r="AH5" s="55"/>
+      <c r="AH5" s="55" t="n">
+        <v>25126.8400000000001</v>
+      </c>
       <c r="AI5" s="55"/>
       <c r="AJ5" s="55"/>
     </row>
@@ -2862,7 +2874,9 @@
       <c r="U6" s="55" t="n">
         <v>9818.95000000000073</v>
       </c>
-      <c r="V6" s="55"/>
+      <c r="V6" s="55" t="n">
+        <v>10082.9699999999993</v>
+      </c>
       <c r="W6" s="55"/>
       <c r="X6" s="55"/>
       <c r="Z6" s="51" t="s">
@@ -2889,7 +2903,9 @@
       <c r="AG6" s="55" t="n">
         <v>7165.82999999999993</v>
       </c>
-      <c r="AH6" s="55"/>
+      <c r="AH6" s="55" t="n">
+        <v>7537.28999999999996</v>
+      </c>
       <c r="AI6" s="55"/>
       <c r="AJ6" s="55"/>
     </row>
@@ -2918,7 +2934,9 @@
       <c r="I7" s="55" t="n">
         <v>1373</v>
       </c>
-      <c r="J7" s="55"/>
+      <c r="J7" s="55" t="n">
+        <v>1373</v>
+      </c>
       <c r="K7" s="55"/>
       <c r="L7" s="55"/>
       <c r="N7" s="51" t="s">
@@ -2945,7 +2963,9 @@
       <c r="U7" s="55" t="n">
         <v>1404</v>
       </c>
-      <c r="V7" s="55"/>
+      <c r="V7" s="55" t="n">
+        <v>1356</v>
+      </c>
       <c r="W7" s="55"/>
       <c r="X7" s="55"/>
       <c r="Z7" s="51" t="s">
@@ -2972,7 +2992,9 @@
       <c r="AG7" s="55" t="n">
         <v>13755.2299999999996</v>
       </c>
-      <c r="AH7" s="55"/>
+      <c r="AH7" s="55" t="n">
+        <v>14065.4400000000005</v>
+      </c>
       <c r="AI7" s="55"/>
       <c r="AJ7" s="55"/>
     </row>
@@ -3001,7 +3023,9 @@
       <c r="I8" s="55" t="n">
         <v>4334</v>
       </c>
-      <c r="J8" s="55"/>
+      <c r="J8" s="55" t="n">
+        <v>4532</v>
+      </c>
       <c r="K8" s="55"/>
       <c r="L8" s="55"/>
       <c r="N8" s="51" t="s">
@@ -3043,7 +3067,9 @@
       <c r="AG8" s="55" t="n">
         <v>23341.4599999999991</v>
       </c>
-      <c r="AH8" s="55"/>
+      <c r="AH8" s="55" t="n">
+        <v>23147.119999999999</v>
+      </c>
       <c r="AI8" s="55"/>
       <c r="AJ8" s="55"/>
     </row>
@@ -3072,7 +3098,9 @@
       <c r="I9" s="55" t="n">
         <v>292</v>
       </c>
-      <c r="J9" s="55"/>
+      <c r="J9" s="55" t="n">
+        <v>292</v>
+      </c>
       <c r="K9" s="55"/>
       <c r="L9" s="55"/>
       <c r="N9" s="51" t="s">
@@ -3114,7 +3142,9 @@
       <c r="AG9" s="55" t="n">
         <v>12001.0300000000007</v>
       </c>
-      <c r="AH9" s="55"/>
+      <c r="AH9" s="55" t="n">
+        <v>11480.7299999999996</v>
+      </c>
       <c r="AI9" s="55"/>
       <c r="AJ9" s="55"/>
     </row>
@@ -3143,7 +3173,9 @@
       <c r="I10" s="55" t="n">
         <v>352</v>
       </c>
-      <c r="J10" s="55"/>
+      <c r="J10" s="55" t="n">
+        <v>352</v>
+      </c>
       <c r="K10" s="55"/>
       <c r="L10" s="55"/>
       <c r="N10" s="51" t="s">
@@ -3185,13 +3217,15 @@
       <c r="AG10" s="55" t="n">
         <v>15403.25</v>
       </c>
-      <c r="AH10" s="55"/>
+      <c r="AH10" s="55" t="s">
+        <v>28</v>
+      </c>
       <c r="AI10" s="55"/>
       <c r="AJ10" s="55"/>
     </row>
     <row r="11" spans="2:36">
       <c r="B11" s="50" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="50" t="n">
         <v>13</v>
@@ -3214,11 +3248,13 @@
       <c r="I11" s="55" t="n">
         <v>556.809999999999945</v>
       </c>
-      <c r="J11" s="55"/>
+      <c r="J11" s="55" t="n">
+        <v>556.809999999999945</v>
+      </c>
       <c r="K11" s="55"/>
       <c r="L11" s="55"/>
       <c r="N11" s="51" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O11" s="51" t="n">
         <v>107</v>
@@ -3233,7 +3269,7 @@
       <c r="W11" s="55"/>
       <c r="X11" s="55"/>
       <c r="Z11" s="51" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AA11" s="51" t="n">
         <v>56</v>
@@ -3256,13 +3292,15 @@
       <c r="AG11" s="55" t="n">
         <v>23231.1899999999987</v>
       </c>
-      <c r="AH11" s="55"/>
+      <c r="AH11" s="55" t="n">
+        <v>23231.1899999999987</v>
+      </c>
       <c r="AI11" s="55"/>
       <c r="AJ11" s="55"/>
     </row>
     <row r="12" spans="2:36">
       <c r="B12" s="50" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" s="50" t="n">
         <v>31</v>
@@ -3285,11 +3323,13 @@
       <c r="I12" s="55" t="n">
         <v>11580.3199999999997</v>
       </c>
-      <c r="J12" s="55"/>
+      <c r="J12" s="55" t="n">
+        <v>12834.5799999999999</v>
+      </c>
       <c r="K12" s="55"/>
       <c r="L12" s="55"/>
       <c r="N12" s="51" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O12" s="51" t="n">
         <v>166</v>
@@ -3304,7 +3344,7 @@
       <c r="W12" s="55"/>
       <c r="X12" s="55"/>
       <c r="Z12" s="51" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AA12" s="51" t="n">
         <v>66</v>
@@ -3327,13 +3367,15 @@
       <c r="AG12" s="55" t="n">
         <v>8023.60999999999876</v>
       </c>
-      <c r="AH12" s="55"/>
+      <c r="AH12" s="55" t="n">
+        <v>8023.60999999999967</v>
+      </c>
       <c r="AI12" s="55"/>
       <c r="AJ12" s="55"/>
     </row>
     <row r="13" spans="2:36">
       <c r="B13" s="50" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" s="50" t="n">
         <v>14</v>
@@ -3356,11 +3398,13 @@
       <c r="I13" s="55" t="n">
         <v>4607</v>
       </c>
-      <c r="J13" s="55"/>
+      <c r="J13" s="55" t="n">
+        <v>4607</v>
+      </c>
       <c r="K13" s="55"/>
       <c r="L13" s="55"/>
       <c r="N13" s="51" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O13" s="51" t="n">
         <v>12</v>
@@ -3383,11 +3427,13 @@
       <c r="U13" s="55" t="n">
         <v>3155</v>
       </c>
-      <c r="V13" s="55"/>
+      <c r="V13" s="55" t="n">
+        <v>3155</v>
+      </c>
       <c r="W13" s="55"/>
       <c r="X13" s="55"/>
       <c r="Z13" s="51" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AA13" s="51" t="n">
         <v>74</v>
@@ -3410,13 +3456,15 @@
       <c r="AG13" s="55" t="n">
         <v>11699.6600000000017</v>
       </c>
-      <c r="AH13" s="55"/>
+      <c r="AH13" s="55" t="n">
+        <v>10546.9599999999991</v>
+      </c>
       <c r="AI13" s="55"/>
       <c r="AJ13" s="55"/>
     </row>
     <row r="14" spans="2:36">
       <c r="B14" s="50" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" s="50" t="n">
         <v>45</v>
@@ -3439,11 +3487,13 @@
       <c r="I14" s="55" t="n">
         <v>480</v>
       </c>
-      <c r="J14" s="55"/>
+      <c r="J14" s="55" t="n">
+        <v>570</v>
+      </c>
       <c r="K14" s="55"/>
       <c r="L14" s="55"/>
       <c r="N14" s="51" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O14" s="51" t="n">
         <v>25</v>
@@ -3466,11 +3516,13 @@
       <c r="U14" s="55" t="n">
         <v>4792.3100000000004</v>
       </c>
-      <c r="V14" s="55"/>
+      <c r="V14" s="55" t="n">
+        <v>4788.84000000000015</v>
+      </c>
       <c r="W14" s="55"/>
       <c r="X14" s="55"/>
       <c r="Z14" s="51" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AA14" s="51" t="n">
         <v>109</v>
@@ -3493,13 +3545,15 @@
       <c r="AG14" s="55" t="n">
         <v>22573.2900000000009</v>
       </c>
-      <c r="AH14" s="55"/>
+      <c r="AH14" s="55" t="n">
+        <v>21586.4500000000007</v>
+      </c>
       <c r="AI14" s="55"/>
       <c r="AJ14" s="55"/>
     </row>
     <row r="15" spans="2:36">
       <c r="B15" s="50" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C15" s="50" t="n">
         <v>3</v>
@@ -3522,11 +3576,13 @@
       <c r="I15" s="55" t="n">
         <v>249.879999999999995</v>
       </c>
-      <c r="J15" s="55"/>
+      <c r="J15" s="55" t="n">
+        <v>249.879999999999995</v>
+      </c>
       <c r="K15" s="55"/>
       <c r="L15" s="55"/>
       <c r="N15" s="51" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O15" s="51" t="n">
         <v>37</v>
@@ -3549,11 +3605,13 @@
       <c r="U15" s="55" t="n">
         <v>7222.10000000000036</v>
       </c>
-      <c r="V15" s="55"/>
+      <c r="V15" s="55" t="n">
+        <v>7646.89999999999964</v>
+      </c>
       <c r="W15" s="55"/>
       <c r="X15" s="55"/>
       <c r="Z15" s="51" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AA15" s="51" t="n">
         <v>250</v>
@@ -3576,7 +3634,7 @@
     </row>
     <row r="16" spans="2:36">
       <c r="B16" s="50" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C16" s="50" t="n">
         <v>32</v>
@@ -3599,11 +3657,13 @@
       <c r="I16" s="55" t="n">
         <v>1215.96000000000004</v>
       </c>
-      <c r="J16" s="55"/>
+      <c r="J16" s="55" t="n">
+        <v>1215.96000000000004</v>
+      </c>
       <c r="K16" s="55"/>
       <c r="L16" s="55"/>
       <c r="N16" s="51" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="O16" s="51" t="n">
         <v>50</v>
@@ -3626,11 +3686,13 @@
       <c r="U16" s="55" t="n">
         <v>6846.38000000000011</v>
       </c>
-      <c r="V16" s="55"/>
+      <c r="V16" s="55" t="n">
+        <v>6741.10999999999967</v>
+      </c>
       <c r="W16" s="55"/>
       <c r="X16" s="55"/>
       <c r="Z16" s="51" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AA16" s="51" t="n">
         <v>24</v>
@@ -3653,13 +3715,15 @@
       <c r="AG16" s="55" t="n">
         <v>306.990000000000009</v>
       </c>
-      <c r="AH16" s="55"/>
+      <c r="AH16" s="55" t="n">
+        <v>292.550000000000011</v>
+      </c>
       <c r="AI16" s="55"/>
       <c r="AJ16" s="55"/>
     </row>
     <row r="17" spans="2:36">
       <c r="B17" s="50" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C17" s="50" t="n">
         <v>37</v>
@@ -3682,11 +3746,13 @@
       <c r="I17" s="55" t="n">
         <v>1381.34999999999991</v>
       </c>
-      <c r="J17" s="55"/>
+      <c r="J17" s="55" t="n">
+        <v>1245.96000000000004</v>
+      </c>
       <c r="K17" s="55"/>
       <c r="L17" s="55"/>
       <c r="N17" s="51" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O17" s="51" t="n">
         <v>25</v>
@@ -3709,11 +3775,13 @@
       <c r="U17" s="55" t="n">
         <v>4469.8100000000004</v>
       </c>
-      <c r="V17" s="55"/>
+      <c r="V17" s="55" t="n">
+        <v>5384.90999999999985</v>
+      </c>
       <c r="W17" s="55"/>
       <c r="X17" s="55"/>
       <c r="Z17" s="51" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AA17" s="51" t="n">
         <v>48</v>
@@ -3736,13 +3804,15 @@
       <c r="AG17" s="55" t="n">
         <v>593.080000000000041</v>
       </c>
-      <c r="AH17" s="55"/>
+      <c r="AH17" s="55" t="n">
+        <v>546.129999999999995</v>
+      </c>
       <c r="AI17" s="55"/>
       <c r="AJ17" s="55"/>
     </row>
     <row r="18" spans="2:36">
       <c r="B18" s="50" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" s="50" t="n">
         <v>10</v>
@@ -3765,11 +3835,13 @@
       <c r="I18" s="55" t="n">
         <v>100</v>
       </c>
-      <c r="J18" s="55"/>
+      <c r="J18" s="55" t="n">
+        <v>100</v>
+      </c>
       <c r="K18" s="55"/>
       <c r="L18" s="55"/>
       <c r="N18" s="51" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O18" s="51" t="n">
         <v>37</v>
@@ -3792,11 +3864,13 @@
       <c r="U18" s="55" t="n">
         <v>5396.32999999999993</v>
       </c>
-      <c r="V18" s="55"/>
+      <c r="V18" s="55" t="n">
+        <v>5396.32999999999993</v>
+      </c>
       <c r="W18" s="55"/>
       <c r="X18" s="55"/>
       <c r="Z18" s="51" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AA18" s="51" t="n">
         <v>143</v>
@@ -3819,13 +3893,15 @@
       <c r="AG18" s="55" t="n">
         <v>1696.54999999999995</v>
       </c>
-      <c r="AH18" s="55"/>
+      <c r="AH18" s="55" t="n">
+        <v>1700.80999999999995</v>
+      </c>
       <c r="AI18" s="55"/>
       <c r="AJ18" s="55"/>
     </row>
     <row r="19" spans="2:36">
       <c r="B19" s="50" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C19" s="50" t="n">
         <v>12</v>
@@ -3848,17 +3924,19 @@
       <c r="I19" s="55" t="n">
         <v>77.0400000000000063</v>
       </c>
-      <c r="J19" s="55"/>
+      <c r="J19" s="55" t="n">
+        <v>77.0400000000000063</v>
+      </c>
       <c r="K19" s="55"/>
       <c r="L19" s="55"/>
       <c r="N19" s="51" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="O19" s="51" t="n">
         <v>50</v>
       </c>
       <c r="P19" s="53" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Q19" s="53" t="n">
         <v>6789.90999999999985</v>
@@ -3875,11 +3953,13 @@
       <c r="U19" s="55" t="n">
         <v>8120.14000000000033</v>
       </c>
-      <c r="V19" s="55"/>
+      <c r="V19" s="55" t="n">
+        <v>7231.97999999999956</v>
+      </c>
       <c r="W19" s="55"/>
       <c r="X19" s="55"/>
       <c r="Z19" s="51" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AA19" s="51" t="n">
         <v>195</v>
@@ -3898,13 +3978,15 @@
       <c r="AG19" s="55" t="n">
         <v>2352.71000000000004</v>
       </c>
-      <c r="AH19" s="55"/>
+      <c r="AH19" s="55" t="n">
+        <v>2218.15999999999985</v>
+      </c>
       <c r="AI19" s="55"/>
       <c r="AJ19" s="55"/>
     </row>
     <row r="20" spans="2:36">
       <c r="B20" s="50" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C20" s="50" t="n">
         <v>19</v>
@@ -3927,11 +4009,13 @@
       <c r="I20" s="55" t="n">
         <v>99.4500000000000028</v>
       </c>
-      <c r="J20" s="55"/>
+      <c r="J20" s="55" t="n">
+        <v>99.4500000000000028</v>
+      </c>
       <c r="K20" s="55"/>
       <c r="L20" s="55"/>
       <c r="N20" s="51" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O20" s="51" t="n">
         <v>25</v>
@@ -3954,11 +4038,13 @@
       <c r="U20" s="55" t="n">
         <v>5775.96000000000004</v>
       </c>
-      <c r="V20" s="55"/>
+      <c r="V20" s="55" t="n">
+        <v>4293.02000000000044</v>
+      </c>
       <c r="W20" s="55"/>
       <c r="X20" s="55"/>
       <c r="Z20" s="51" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AA20" s="51" t="n">
         <v>43</v>
@@ -3981,13 +4067,15 @@
       <c r="AG20" s="55" t="n">
         <v>5476</v>
       </c>
-      <c r="AH20" s="55"/>
+      <c r="AH20" s="55" t="n">
+        <v>5420</v>
+      </c>
       <c r="AI20" s="55"/>
       <c r="AJ20" s="55"/>
     </row>
     <row r="21" spans="2:36">
       <c r="B21" s="50" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C21" s="50" t="n">
         <v>25</v>
@@ -4010,11 +4098,13 @@
       <c r="I21" s="55" t="n">
         <v>132.75</v>
       </c>
-      <c r="J21" s="55"/>
+      <c r="J21" s="55" t="n">
+        <v>139.620000000000005</v>
+      </c>
       <c r="K21" s="55"/>
       <c r="L21" s="55"/>
       <c r="N21" s="51" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="O21" s="51" t="n">
         <v>25</v>
@@ -4037,11 +4127,13 @@
       <c r="U21" s="55" t="n">
         <v>5246.27999999999975</v>
       </c>
-      <c r="V21" s="55"/>
+      <c r="V21" s="55" t="n">
+        <v>5246.27999999999975</v>
+      </c>
       <c r="W21" s="55"/>
       <c r="X21" s="55"/>
       <c r="Z21" s="51" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA21" s="51" t="n">
         <v>133</v>
@@ -4064,13 +4156,15 @@
       <c r="AG21" s="55" t="n">
         <v>12012</v>
       </c>
-      <c r="AH21" s="55"/>
+      <c r="AH21" s="55" t="n">
+        <v>12196</v>
+      </c>
       <c r="AI21" s="55"/>
       <c r="AJ21" s="55"/>
     </row>
     <row r="22" spans="2:36">
       <c r="B22" s="50" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C22" s="50" t="n">
         <v>6</v>
@@ -4093,11 +4187,13 @@
       <c r="I22" s="55" t="n">
         <v>147</v>
       </c>
-      <c r="J22" s="55"/>
+      <c r="J22" s="55" t="n">
+        <v>147</v>
+      </c>
       <c r="K22" s="55"/>
       <c r="L22" s="55"/>
       <c r="N22" s="51" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O22" s="51" t="n">
         <v>25</v>
@@ -4120,11 +4216,13 @@
       <c r="U22" s="55" t="n">
         <v>3842.76000000000022</v>
       </c>
-      <c r="V22" s="55"/>
+      <c r="V22" s="55" t="n">
+        <v>3919.57999999999993</v>
+      </c>
       <c r="W22" s="55"/>
       <c r="X22" s="55"/>
       <c r="Z22" s="51" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AA22" s="51" t="n">
         <v>258</v>
@@ -4151,7 +4249,7 @@
     </row>
     <row r="23" spans="2:36">
       <c r="B23" s="50" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C23" s="50" t="n">
         <v>65</v>
@@ -4174,11 +4272,13 @@
       <c r="I23" s="55" t="n">
         <v>652.590000000000032</v>
       </c>
-      <c r="J23" s="55"/>
+      <c r="J23" s="55" t="n">
+        <v>655.799999999999955</v>
+      </c>
       <c r="K23" s="55"/>
       <c r="L23" s="55"/>
       <c r="N23" s="51" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O23" s="51" t="n">
         <v>26</v>
@@ -4201,11 +4301,13 @@
       <c r="U23" s="55" t="n">
         <v>2033.3599999999999</v>
       </c>
-      <c r="V23" s="55"/>
+      <c r="V23" s="55" t="n">
+        <v>2002.98000000000002</v>
+      </c>
       <c r="W23" s="55"/>
       <c r="X23" s="55"/>
       <c r="Z23" s="50" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AA23" s="50" t="n">
         <v>17</v>
@@ -4228,13 +4330,15 @@
       <c r="AG23" s="55" t="n">
         <v>127.180000000000007</v>
       </c>
-      <c r="AH23" s="55"/>
+      <c r="AH23" s="55" t="n">
+        <v>127.180000000000007</v>
+      </c>
       <c r="AI23" s="55"/>
       <c r="AJ23" s="55"/>
     </row>
     <row r="24" spans="2:36">
       <c r="B24" s="50" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C24" s="50" t="n">
         <v>4</v>
@@ -4257,11 +4361,13 @@
       <c r="I24" s="55" t="n">
         <v>154</v>
       </c>
-      <c r="J24" s="55"/>
+      <c r="J24" s="55" t="n">
+        <v>154</v>
+      </c>
       <c r="K24" s="55"/>
       <c r="L24" s="55"/>
       <c r="N24" s="51" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O24" s="51" t="n">
         <v>79</v>
@@ -4284,11 +4390,13 @@
       <c r="U24" s="55" t="n">
         <v>8969.48999999999796</v>
       </c>
-      <c r="V24" s="55"/>
+      <c r="V24" s="55" t="n">
+        <v>9406.35000000000036</v>
+      </c>
       <c r="W24" s="55"/>
       <c r="X24" s="55"/>
       <c r="Z24" s="51" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AA24" s="51" t="n">
         <v>10</v>
@@ -4311,13 +4419,15 @@
       <c r="AG24" s="55" t="n">
         <v>146</v>
       </c>
-      <c r="AH24" s="55"/>
+      <c r="AH24" s="55" t="n">
+        <v>146</v>
+      </c>
       <c r="AI24" s="55"/>
       <c r="AJ24" s="55"/>
     </row>
     <row r="25" spans="2:36">
       <c r="B25" s="50" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C25" s="50" t="n">
         <v>5</v>
@@ -4340,11 +4450,13 @@
       <c r="I25" s="55" t="n">
         <v>248</v>
       </c>
-      <c r="J25" s="55"/>
+      <c r="J25" s="55" t="n">
+        <v>248</v>
+      </c>
       <c r="K25" s="55"/>
       <c r="L25" s="55"/>
       <c r="N25" s="51" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="O25" s="51" t="n">
         <v>344</v>
@@ -4365,7 +4477,7 @@
       <c r="W25" s="55"/>
       <c r="X25" s="55"/>
       <c r="Z25" s="51" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA25" s="51" t="n">
         <v>56</v>
@@ -4388,13 +4500,15 @@
       <c r="AG25" s="55" t="n">
         <v>27500</v>
       </c>
-      <c r="AH25" s="55"/>
+      <c r="AH25" s="55" t="n">
+        <v>27500</v>
+      </c>
       <c r="AI25" s="55"/>
       <c r="AJ25" s="55"/>
     </row>
     <row r="26" spans="2:36">
       <c r="B26" s="50" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C26" s="50" t="n">
         <v>6</v>
@@ -4417,11 +4531,13 @@
       <c r="I26" s="55" t="n">
         <v>162</v>
       </c>
-      <c r="J26" s="55"/>
+      <c r="J26" s="55" t="n">
+        <v>162</v>
+      </c>
       <c r="K26" s="55"/>
       <c r="L26" s="55"/>
       <c r="N26" s="51" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="O26" s="51" t="n">
         <v>140</v>
@@ -4444,11 +4560,13 @@
       <c r="U26" s="55" t="n">
         <v>535</v>
       </c>
-      <c r="V26" s="55"/>
+      <c r="V26" s="55" t="n">
+        <v>640</v>
+      </c>
       <c r="W26" s="55"/>
       <c r="X26" s="55"/>
       <c r="Z26" s="51" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AA26" s="51" t="n">
         <v>56</v>
@@ -4471,13 +4589,15 @@
       <c r="AG26" s="55" t="n">
         <v>1038.02999999999997</v>
       </c>
-      <c r="AH26" s="55"/>
+      <c r="AH26" s="55" t="n">
+        <v>1094.8900000000001</v>
+      </c>
       <c r="AI26" s="55"/>
       <c r="AJ26" s="55"/>
     </row>
     <row r="27" spans="26:36">
       <c r="Z27" s="50" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AA27" s="50" t="n">
         <v>4</v>
@@ -4500,13 +4620,15 @@
       <c r="AG27" s="55" t="n">
         <v>751.059999999999832</v>
       </c>
-      <c r="AH27" s="55"/>
+      <c r="AH27" s="55" t="n">
+        <v>751.059999999999945</v>
+      </c>
       <c r="AI27" s="55"/>
       <c r="AJ27" s="55"/>
     </row>
     <row r="28" spans="26:36">
       <c r="Z28" s="50" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AA28" s="50" t="n">
         <v>5</v>
@@ -4529,7 +4651,9 @@
       <c r="AG28" s="55" t="n">
         <v>456.579999999999984</v>
       </c>
-      <c r="AH28" s="55"/>
+      <c r="AH28" s="55" t="n">
+        <v>456.579999999999984</v>
+      </c>
       <c r="AI28" s="55"/>
       <c r="AJ28" s="55"/>
     </row>
@@ -4551,7 +4675,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1643199832" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1643203916" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -4560,16 +4684,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1643199832" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1643199832" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1643199832" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1643199832" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1643203916" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1643203916" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1643203916" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1643203916" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1643199832" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1643203916" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -4582,8 +4706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AJ28"/>
   <sheetViews>
-    <sheetView view="normal" topLeftCell="AC4" workbookViewId="0">
-      <selection activeCell="Z29" sqref="Z29"/>
+    <sheetView view="normal" topLeftCell="Z4" zoomScale="90" workbookViewId="0">
+      <selection activeCell="AH28" sqref="AH28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.20"/>
@@ -4645,7 +4769,7 @@
     <row r="3" spans="2:36">
       <c r="B3" s="51"/>
       <c r="C3" s="51" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D3" s="49" t="s">
         <v>2</v>
@@ -4664,7 +4788,7 @@
       <c r="L3" s="49"/>
       <c r="N3" s="51"/>
       <c r="O3" s="51" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="P3" s="49" t="s">
         <v>2</v>
@@ -4683,7 +4807,7 @@
       <c r="X3" s="49"/>
       <c r="Z3" s="51"/>
       <c r="AA3" s="51" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AB3" s="49" t="s">
         <v>2</v>
@@ -4827,7 +4951,9 @@
       <c r="I5" s="55" t="n">
         <v>1425.65000000000009</v>
       </c>
-      <c r="J5" s="55"/>
+      <c r="J5" s="55" t="n">
+        <v>1328.53999999999996</v>
+      </c>
       <c r="K5" s="55"/>
       <c r="L5" s="55"/>
       <c r="N5" s="51" t="s">
@@ -4854,7 +4980,9 @@
       <c r="U5" s="55" t="n">
         <v>1691</v>
       </c>
-      <c r="V5" s="55"/>
+      <c r="V5" s="55" t="n">
+        <v>1691</v>
+      </c>
       <c r="W5" s="55"/>
       <c r="X5" s="55"/>
       <c r="Z5" s="51" t="s">
@@ -4881,7 +5009,9 @@
       <c r="AG5" s="55" t="n">
         <v>44106.739999999998</v>
       </c>
-      <c r="AH5" s="55"/>
+      <c r="AH5" s="55" t="n">
+        <v>44106.739999999998</v>
+      </c>
       <c r="AI5" s="55"/>
       <c r="AJ5" s="55"/>
     </row>
@@ -4925,7 +5055,9 @@
       <c r="U6" s="55" t="n">
         <v>22425.0299999999988</v>
       </c>
-      <c r="V6" s="55"/>
+      <c r="V6" s="55" t="n">
+        <v>26964.5200000000004</v>
+      </c>
       <c r="W6" s="55"/>
       <c r="X6" s="55"/>
       <c r="Z6" s="51" t="s">
@@ -4952,7 +5084,9 @@
       <c r="AG6" s="55" t="n">
         <v>15274.4300000000003</v>
       </c>
-      <c r="AH6" s="55"/>
+      <c r="AH6" s="55" t="n">
+        <v>16472.9799999999996</v>
+      </c>
       <c r="AI6" s="55"/>
       <c r="AJ6" s="55"/>
     </row>
@@ -4981,7 +5115,9 @@
       <c r="I7" s="55" t="n">
         <v>3674</v>
       </c>
-      <c r="J7" s="55"/>
+      <c r="J7" s="55" t="n">
+        <v>3674</v>
+      </c>
       <c r="K7" s="55"/>
       <c r="L7" s="55"/>
       <c r="N7" s="51" t="s">
@@ -5008,7 +5144,9 @@
       <c r="U7" s="55" t="n">
         <v>3062</v>
       </c>
-      <c r="V7" s="55"/>
+      <c r="V7" s="55" t="n">
+        <v>2950</v>
+      </c>
       <c r="W7" s="55"/>
       <c r="X7" s="55"/>
       <c r="Z7" s="51" t="s">
@@ -5035,7 +5173,9 @@
       <c r="AG7" s="55" t="n">
         <v>22298.2299999999996</v>
       </c>
-      <c r="AH7" s="55"/>
+      <c r="AH7" s="55" t="n">
+        <v>21887.8899999999994</v>
+      </c>
       <c r="AI7" s="55"/>
       <c r="AJ7" s="55"/>
     </row>
@@ -5064,7 +5204,9 @@
       <c r="I8" s="55" t="n">
         <v>9700</v>
       </c>
-      <c r="J8" s="55"/>
+      <c r="J8" s="55" t="n">
+        <v>11824</v>
+      </c>
       <c r="K8" s="55"/>
       <c r="L8" s="55"/>
       <c r="N8" s="51" t="s">
@@ -5106,7 +5248,9 @@
       <c r="AG8" s="55" t="n">
         <v>49348.6699999999983</v>
       </c>
-      <c r="AH8" s="55"/>
+      <c r="AH8" s="55" t="n">
+        <v>48383.8099999999977</v>
+      </c>
       <c r="AI8" s="55"/>
       <c r="AJ8" s="55"/>
     </row>
@@ -5135,7 +5279,9 @@
       <c r="I9" s="55" t="n">
         <v>581</v>
       </c>
-      <c r="J9" s="55"/>
+      <c r="J9" s="55" t="n">
+        <v>581</v>
+      </c>
       <c r="K9" s="55"/>
       <c r="L9" s="55"/>
       <c r="N9" s="51" t="s">
@@ -5177,7 +5323,9 @@
       <c r="AG9" s="55" t="n">
         <v>28343.3400000000001</v>
       </c>
-      <c r="AH9" s="55"/>
+      <c r="AH9" s="55" t="n">
+        <v>26341.8199999999997</v>
+      </c>
       <c r="AI9" s="55"/>
       <c r="AJ9" s="55"/>
     </row>
@@ -5206,7 +5354,9 @@
       <c r="I10" s="55" t="n">
         <v>818</v>
       </c>
-      <c r="J10" s="55"/>
+      <c r="J10" s="55" t="n">
+        <v>818</v>
+      </c>
       <c r="K10" s="55"/>
       <c r="L10" s="55"/>
       <c r="N10" s="51" t="s">
@@ -5248,13 +5398,15 @@
       <c r="AG10" s="55" t="n">
         <v>34036.7300000000032</v>
       </c>
-      <c r="AH10" s="55"/>
+      <c r="AH10" s="55" t="n">
+        <v>34036.7300000000032</v>
+      </c>
       <c r="AI10" s="55"/>
       <c r="AJ10" s="55"/>
     </row>
     <row r="11" spans="2:36">
       <c r="B11" s="50" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="50" t="n">
         <v>26</v>
@@ -5277,11 +5429,13 @@
       <c r="I11" s="55" t="n">
         <v>1813.95000000000005</v>
       </c>
-      <c r="J11" s="55"/>
+      <c r="J11" s="55" t="n">
+        <v>1813.95000000000005</v>
+      </c>
       <c r="K11" s="55"/>
       <c r="L11" s="55"/>
       <c r="N11" s="51" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O11" s="51" t="n">
         <v>215</v>
@@ -5296,7 +5450,7 @@
       <c r="W11" s="55"/>
       <c r="X11" s="55"/>
       <c r="Z11" s="51" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AA11" s="51" t="n">
         <v>113</v>
@@ -5319,13 +5473,15 @@
       <c r="AG11" s="55" t="n">
         <v>52534.3300000000017</v>
       </c>
-      <c r="AH11" s="55"/>
+      <c r="AH11" s="55" t="n">
+        <v>52927.2699999999968</v>
+      </c>
       <c r="AI11" s="55"/>
       <c r="AJ11" s="55"/>
     </row>
     <row r="12" spans="2:36">
       <c r="B12" s="50" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" s="50" t="n">
         <v>63</v>
@@ -5348,11 +5504,13 @@
       <c r="I12" s="55" t="n">
         <v>29059.75</v>
       </c>
-      <c r="J12" s="55"/>
+      <c r="J12" s="55" t="n">
+        <v>27954.9900000000016</v>
+      </c>
       <c r="K12" s="55"/>
       <c r="L12" s="55"/>
       <c r="N12" s="51" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O12" s="51" t="n">
         <v>333</v>
@@ -5367,7 +5525,7 @@
       <c r="W12" s="55"/>
       <c r="X12" s="55"/>
       <c r="Z12" s="51" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AA12" s="51" t="n">
         <v>132</v>
@@ -5390,13 +5548,15 @@
       <c r="AG12" s="55" t="n">
         <v>21514.7599999999984</v>
       </c>
-      <c r="AH12" s="55"/>
+      <c r="AH12" s="55" t="n">
+        <v>21495.7599999999984</v>
+      </c>
       <c r="AI12" s="55"/>
       <c r="AJ12" s="55"/>
     </row>
     <row r="13" spans="2:36">
       <c r="B13" s="50" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" s="50" t="n">
         <v>29</v>
@@ -5419,11 +5579,13 @@
       <c r="I13" s="55" t="n">
         <v>9455</v>
       </c>
-      <c r="J13" s="55"/>
+      <c r="J13" s="55" t="n">
+        <v>9812</v>
+      </c>
       <c r="K13" s="55"/>
       <c r="L13" s="55"/>
       <c r="N13" s="51" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O13" s="51" t="n">
         <v>24</v>
@@ -5446,11 +5608,13 @@
       <c r="U13" s="55" t="n">
         <v>5381</v>
       </c>
-      <c r="V13" s="55"/>
+      <c r="V13" s="55" t="n">
+        <v>6289</v>
+      </c>
       <c r="W13" s="55"/>
       <c r="X13" s="55"/>
       <c r="Z13" s="51" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AA13" s="51" t="n">
         <v>149</v>
@@ -5473,13 +5637,15 @@
       <c r="AG13" s="55" t="n">
         <v>24326.7099999999991</v>
       </c>
-      <c r="AH13" s="55"/>
+      <c r="AH13" s="55" t="n">
+        <v>24783.4700000000012</v>
+      </c>
       <c r="AI13" s="55"/>
       <c r="AJ13" s="55"/>
     </row>
     <row r="14" spans="2:36">
       <c r="B14" s="50" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" s="50" t="n">
         <v>90</v>
@@ -5502,11 +5668,13 @@
       <c r="I14" s="55" t="n">
         <v>980</v>
       </c>
-      <c r="J14" s="55"/>
+      <c r="J14" s="55" t="n">
+        <v>1090</v>
+      </c>
       <c r="K14" s="55"/>
       <c r="L14" s="55"/>
       <c r="N14" s="51" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O14" s="51" t="n">
         <v>50</v>
@@ -5529,11 +5697,13 @@
       <c r="U14" s="55" t="n">
         <v>9744.28000000000065</v>
       </c>
-      <c r="V14" s="55"/>
+      <c r="V14" s="55" t="n">
+        <v>10444.8999999999996</v>
+      </c>
       <c r="W14" s="55"/>
       <c r="X14" s="55"/>
       <c r="Z14" s="51" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AA14" s="51" t="n">
         <v>219</v>
@@ -5556,13 +5726,15 @@
       <c r="AG14" s="55" t="n">
         <v>42428.8499999999985</v>
       </c>
-      <c r="AH14" s="55"/>
+      <c r="AH14" s="55" t="n">
+        <v>42621.9499999999971</v>
+      </c>
       <c r="AI14" s="55"/>
       <c r="AJ14" s="55"/>
     </row>
     <row r="15" spans="2:36">
       <c r="B15" s="50" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C15" s="50" t="n">
         <v>7</v>
@@ -5585,11 +5757,13 @@
       <c r="I15" s="55" t="n">
         <v>1339.11999999999989</v>
       </c>
-      <c r="J15" s="55"/>
+      <c r="J15" s="55" t="n">
+        <v>1339.11999999999989</v>
+      </c>
       <c r="K15" s="55"/>
       <c r="L15" s="55"/>
       <c r="N15" s="51" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O15" s="51" t="n">
         <v>75</v>
@@ -5612,11 +5786,13 @@
       <c r="U15" s="55" t="n">
         <v>14150.0800000000017</v>
       </c>
-      <c r="V15" s="55"/>
+      <c r="V15" s="55" t="n">
+        <v>13836.7999999999993</v>
+      </c>
       <c r="W15" s="55"/>
       <c r="X15" s="55"/>
       <c r="Z15" s="51" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AA15" s="51" t="n">
         <v>501</v>
@@ -5639,7 +5815,7 @@
     </row>
     <row r="16" spans="2:36">
       <c r="B16" s="50" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C16" s="50" t="n">
         <v>65</v>
@@ -5662,11 +5838,13 @@
       <c r="I16" s="55" t="n">
         <v>2726.80000000000018</v>
       </c>
-      <c r="J16" s="55"/>
+      <c r="J16" s="55" t="n">
+        <v>2565.23000000000002</v>
+      </c>
       <c r="K16" s="55"/>
       <c r="L16" s="55"/>
       <c r="N16" s="51" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="O16" s="51" t="n">
         <v>100</v>
@@ -5689,11 +5867,13 @@
       <c r="U16" s="55" t="n">
         <v>15446.0200000000004</v>
       </c>
-      <c r="V16" s="55"/>
+      <c r="V16" s="55" t="n">
+        <v>15428.7999999999993</v>
+      </c>
       <c r="W16" s="55"/>
       <c r="X16" s="55"/>
       <c r="Z16" s="51" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AA16" s="51" t="n">
         <v>49</v>
@@ -5716,13 +5896,15 @@
       <c r="AG16" s="55" t="n">
         <v>599.440000000000168</v>
       </c>
-      <c r="AH16" s="55"/>
+      <c r="AH16" s="55" t="n">
+        <v>600.549999999999955</v>
+      </c>
       <c r="AI16" s="55"/>
       <c r="AJ16" s="55"/>
     </row>
     <row r="17" spans="2:36">
       <c r="B17" s="50" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C17" s="50" t="n">
         <v>75</v>
@@ -5745,11 +5927,13 @@
       <c r="I17" s="55" t="n">
         <v>3345.19999999999982</v>
       </c>
-      <c r="J17" s="55"/>
+      <c r="J17" s="55" t="n">
+        <v>3089.53999999999996</v>
+      </c>
       <c r="K17" s="55"/>
       <c r="L17" s="55"/>
       <c r="N17" s="51" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O17" s="51" t="n">
         <v>50</v>
@@ -5772,11 +5956,13 @@
       <c r="U17" s="55" t="n">
         <v>11037.6000000000004</v>
       </c>
-      <c r="V17" s="55"/>
+      <c r="V17" s="55" t="n">
+        <v>10913.6100000000006</v>
+      </c>
       <c r="W17" s="55"/>
       <c r="X17" s="55"/>
       <c r="Z17" s="51" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AA17" s="51" t="n">
         <v>97</v>
@@ -5799,13 +5985,15 @@
       <c r="AG17" s="55" t="n">
         <v>1253.26999999999998</v>
       </c>
-      <c r="AH17" s="55"/>
+      <c r="AH17" s="55" t="n">
+        <v>1158.97000000000003</v>
+      </c>
       <c r="AI17" s="55"/>
       <c r="AJ17" s="55"/>
     </row>
     <row r="18" spans="2:36">
       <c r="B18" s="50" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" s="50" t="n">
         <v>21</v>
@@ -5828,11 +6016,13 @@
       <c r="I18" s="55" t="n">
         <v>248</v>
       </c>
-      <c r="J18" s="55"/>
+      <c r="J18" s="55" t="n">
+        <v>248</v>
+      </c>
       <c r="K18" s="55"/>
       <c r="L18" s="55"/>
       <c r="N18" s="51" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O18" s="51" t="n">
         <v>75</v>
@@ -5855,11 +6045,13 @@
       <c r="U18" s="55" t="n">
         <v>12931.0400000000009</v>
       </c>
-      <c r="V18" s="55"/>
+      <c r="V18" s="55" t="n">
+        <v>11828.9599999999991</v>
+      </c>
       <c r="W18" s="55"/>
       <c r="X18" s="55"/>
       <c r="Z18" s="51" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AA18" s="51" t="n">
         <v>287</v>
@@ -5882,13 +6074,15 @@
       <c r="AG18" s="55" t="n">
         <v>3569.88000000000011</v>
       </c>
-      <c r="AH18" s="55"/>
+      <c r="AH18" s="55" t="n">
+        <v>3574.94999999999982</v>
+      </c>
       <c r="AI18" s="55"/>
       <c r="AJ18" s="55"/>
     </row>
     <row r="19" spans="2:36">
       <c r="B19" s="50" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C19" s="50" t="n">
         <v>25</v>
@@ -5911,11 +6105,13 @@
       <c r="I19" s="55" t="n">
         <v>190.340000000000003</v>
       </c>
-      <c r="J19" s="55"/>
+      <c r="J19" s="55" t="n">
+        <v>190.340000000000003</v>
+      </c>
       <c r="K19" s="55"/>
       <c r="L19" s="55"/>
       <c r="N19" s="51" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="O19" s="51" t="n">
         <v>100</v>
@@ -5938,11 +6134,13 @@
       <c r="U19" s="55" t="n">
         <v>16340.7299999999996</v>
       </c>
-      <c r="V19" s="55"/>
+      <c r="V19" s="55" t="n">
+        <v>15996.6100000000006</v>
+      </c>
       <c r="W19" s="55"/>
       <c r="X19" s="55"/>
       <c r="Z19" s="51" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AA19" s="51" t="n">
         <v>391</v>
@@ -5965,7 +6163,7 @@
     </row>
     <row r="20" spans="2:36">
       <c r="B20" s="50" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C20" s="50" t="n">
         <v>38</v>
@@ -5988,11 +6186,13 @@
       <c r="I20" s="55" t="n">
         <v>240.5</v>
       </c>
-      <c r="J20" s="55"/>
+      <c r="J20" s="55" t="n">
+        <v>224.719999999999999</v>
+      </c>
       <c r="K20" s="55"/>
       <c r="L20" s="55"/>
       <c r="N20" s="51" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O20" s="51" t="n">
         <v>50</v>
@@ -6015,11 +6215,13 @@
       <c r="U20" s="55" t="n">
         <v>11626.2099999999991</v>
       </c>
-      <c r="V20" s="55"/>
+      <c r="V20" s="55" t="n">
+        <v>10824.7399999999998</v>
+      </c>
       <c r="W20" s="55"/>
       <c r="X20" s="55"/>
       <c r="Z20" s="51" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AA20" s="51" t="n">
         <v>87</v>
@@ -6042,13 +6244,15 @@
       <c r="AG20" s="55" t="n">
         <v>10488</v>
       </c>
-      <c r="AH20" s="55"/>
+      <c r="AH20" s="55" t="n">
+        <v>10384</v>
+      </c>
       <c r="AI20" s="55"/>
       <c r="AJ20" s="55"/>
     </row>
     <row r="21" spans="2:36">
       <c r="B21" s="50" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C21" s="50" t="n">
         <v>50</v>
@@ -6071,11 +6275,13 @@
       <c r="I21" s="55" t="n">
         <v>266.889999999999986</v>
       </c>
-      <c r="J21" s="55"/>
+      <c r="J21" s="55" t="n">
+        <v>313.779999999999973</v>
+      </c>
       <c r="K21" s="55"/>
       <c r="L21" s="55"/>
       <c r="N21" s="51" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="O21" s="51" t="n">
         <v>50</v>
@@ -6098,11 +6304,13 @@
       <c r="U21" s="55" t="n">
         <v>11210.2600000000002</v>
       </c>
-      <c r="V21" s="55"/>
+      <c r="V21" s="55" t="n">
+        <v>11197.7299999999996</v>
+      </c>
       <c r="W21" s="55"/>
       <c r="X21" s="55"/>
       <c r="Z21" s="51" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA21" s="51" t="n">
         <v>267</v>
@@ -6125,13 +6333,15 @@
       <c r="AG21" s="55" t="n">
         <v>23179</v>
       </c>
-      <c r="AH21" s="55"/>
+      <c r="AH21" s="55" t="n">
+        <v>23486</v>
+      </c>
       <c r="AI21" s="55"/>
       <c r="AJ21" s="55"/>
     </row>
     <row r="22" spans="2:36">
       <c r="B22" s="50" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C22" s="50" t="n">
         <v>13</v>
@@ -6154,11 +6364,13 @@
       <c r="I22" s="55" t="n">
         <v>391</v>
       </c>
-      <c r="J22" s="55"/>
+      <c r="J22" s="55" t="n">
+        <v>391</v>
+      </c>
       <c r="K22" s="55"/>
       <c r="L22" s="55"/>
       <c r="N22" s="51" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O22" s="51" t="n">
         <v>50</v>
@@ -6181,11 +6393,13 @@
       <c r="U22" s="55" t="n">
         <v>9883.1299999999992</v>
       </c>
-      <c r="V22" s="55"/>
+      <c r="V22" s="55" t="n">
+        <v>9449.57999999999993</v>
+      </c>
       <c r="W22" s="55"/>
       <c r="X22" s="55"/>
       <c r="Z22" s="51" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AA22" s="51" t="n">
         <v>516</v>
@@ -6208,7 +6422,7 @@
     </row>
     <row r="23" spans="2:36">
       <c r="B23" s="50" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C23" s="50" t="n">
         <v>131</v>
@@ -6231,11 +6445,13 @@
       <c r="I23" s="55" t="n">
         <v>1350.29999999999995</v>
       </c>
-      <c r="J23" s="55"/>
+      <c r="J23" s="55" t="n">
+        <v>1205.59999999999991</v>
+      </c>
       <c r="K23" s="55"/>
       <c r="L23" s="55"/>
       <c r="N23" s="51" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O23" s="51" t="n">
         <v>52</v>
@@ -6258,11 +6474,13 @@
       <c r="U23" s="55" t="n">
         <v>5255.48999999999978</v>
       </c>
-      <c r="V23" s="55"/>
+      <c r="V23" s="55" t="n">
+        <v>5838.61999999999989</v>
+      </c>
       <c r="W23" s="55"/>
       <c r="X23" s="55"/>
       <c r="Z23" s="50" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AA23" s="50" t="n">
         <v>35</v>
@@ -6285,13 +6503,15 @@
       <c r="AG23" s="55" t="n">
         <v>248.689999999999998</v>
       </c>
-      <c r="AH23" s="55"/>
+      <c r="AH23" s="55" t="n">
+        <v>282.180000000000007</v>
+      </c>
       <c r="AI23" s="55"/>
       <c r="AJ23" s="55"/>
     </row>
     <row r="24" spans="2:36">
       <c r="B24" s="50" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C24" s="50" t="n">
         <v>8</v>
@@ -6314,11 +6534,13 @@
       <c r="I24" s="55" t="n">
         <v>426</v>
       </c>
-      <c r="J24" s="55"/>
+      <c r="J24" s="55" t="n">
+        <v>359</v>
+      </c>
       <c r="K24" s="55"/>
       <c r="L24" s="55"/>
       <c r="N24" s="51" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O24" s="51" t="n">
         <v>159</v>
@@ -6341,11 +6563,13 @@
       <c r="U24" s="55" t="n">
         <v>20147.5999999999985</v>
       </c>
-      <c r="V24" s="55"/>
+      <c r="V24" s="55" t="n">
+        <v>21122.4700000000012</v>
+      </c>
       <c r="W24" s="55"/>
       <c r="X24" s="55"/>
       <c r="Z24" s="51" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AA24" s="51" t="n">
         <v>21</v>
@@ -6368,13 +6592,15 @@
       <c r="AG24" s="55" t="n">
         <v>425</v>
       </c>
-      <c r="AH24" s="55"/>
+      <c r="AH24" s="55" t="n">
+        <v>485</v>
+      </c>
       <c r="AI24" s="55"/>
       <c r="AJ24" s="55"/>
     </row>
     <row r="25" spans="2:36">
       <c r="B25" s="50" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C25" s="50" t="n">
         <v>10</v>
@@ -6397,11 +6623,13 @@
       <c r="I25" s="55" t="n">
         <v>683</v>
       </c>
-      <c r="J25" s="55"/>
+      <c r="J25" s="55" t="n">
+        <v>732</v>
+      </c>
       <c r="K25" s="55"/>
       <c r="L25" s="55"/>
       <c r="N25" s="51" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="O25" s="51" t="n">
         <v>689</v>
@@ -6422,7 +6650,7 @@
       <c r="W25" s="55"/>
       <c r="X25" s="55"/>
       <c r="Z25" s="51" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA25" s="51" t="n">
         <v>112</v>
@@ -6445,13 +6673,15 @@
       <c r="AG25" s="55" t="n">
         <v>69730.6699999999983</v>
       </c>
-      <c r="AH25" s="55"/>
+      <c r="AH25" s="55" t="n">
+        <v>73643.8600000000006</v>
+      </c>
       <c r="AI25" s="55"/>
       <c r="AJ25" s="55"/>
     </row>
     <row r="26" spans="2:36">
       <c r="B26" s="50" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C26" s="50" t="n">
         <v>12</v>
@@ -6474,11 +6704,13 @@
       <c r="I26" s="55" t="n">
         <v>413</v>
       </c>
-      <c r="J26" s="55"/>
+      <c r="J26" s="55" t="n">
+        <v>413</v>
+      </c>
       <c r="K26" s="55"/>
       <c r="L26" s="55"/>
       <c r="N26" s="51" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="O26" s="51" t="n">
         <v>280</v>
@@ -6501,11 +6733,13 @@
       <c r="U26" s="55" t="n">
         <v>1161</v>
       </c>
-      <c r="V26" s="55"/>
+      <c r="V26" s="55" t="n">
+        <v>1298</v>
+      </c>
       <c r="W26" s="55"/>
       <c r="X26" s="55"/>
       <c r="Z26" s="51" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AA26" s="51" t="n">
         <v>112</v>
@@ -6526,15 +6760,17 @@
         <v>2049.57000000000016</v>
       </c>
       <c r="AG26" s="55" t="s">
-        <v>80</v>
-      </c>
-      <c r="AH26" s="55"/>
+        <v>81</v>
+      </c>
+      <c r="AH26" s="55" t="n">
+        <v>2166.09999999999991</v>
+      </c>
       <c r="AI26" s="55"/>
       <c r="AJ26" s="55"/>
     </row>
     <row r="27" spans="26:36">
       <c r="Z27" s="50" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AA27" s="50" t="n">
         <v>8</v>
@@ -6555,15 +6791,17 @@
         <v>1981.15000000000009</v>
       </c>
       <c r="AG27" s="55" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH27" s="55"/>
+        <v>82</v>
+      </c>
+      <c r="AH27" s="55" t="n">
+        <v>1981.15000000000009</v>
+      </c>
       <c r="AI27" s="55"/>
       <c r="AJ27" s="55"/>
     </row>
     <row r="28" spans="26:36">
       <c r="Z28" s="50" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AA28" s="50" t="n">
         <v>11</v>
@@ -6584,9 +6822,11 @@
         <v>2062.34999999999991</v>
       </c>
       <c r="AG28" s="55" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH28" s="55"/>
+        <v>83</v>
+      </c>
+      <c r="AH28" s="55" t="n">
+        <v>2062.34999999999991</v>
+      </c>
       <c r="AI28" s="55"/>
       <c r="AJ28" s="55"/>
     </row>
@@ -6608,7 +6848,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1643199832" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1643203916" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -6617,16 +6857,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1643199832" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1643199832" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1643199832" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1643199832" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1643203916" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1643203916" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1643203916" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1643203916" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1643199832" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1643203916" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -6637,10 +6877,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:AJ28"/>
+  <dimension ref="B2:AJ29"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="Z6" workbookViewId="0">
-      <selection activeCell="AG29" sqref="AG29"/>
+    <sheetView view="normal" topLeftCell="Z4" zoomScale="90" workbookViewId="0">
+      <selection activeCell="AH29" sqref="AH29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.20"/>
@@ -6702,7 +6942,7 @@
     <row r="3" spans="2:36">
       <c r="B3" s="50"/>
       <c r="C3" s="50" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D3" s="49" t="s">
         <v>2</v>
@@ -6721,7 +6961,7 @@
       <c r="L3" s="49"/>
       <c r="N3" s="51"/>
       <c r="O3" s="51" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="P3" s="49" t="s">
         <v>2</v>
@@ -6740,7 +6980,7 @@
       <c r="X3" s="49"/>
       <c r="Z3" s="50"/>
       <c r="AA3" s="50" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AB3" s="49" t="s">
         <v>2</v>
@@ -6884,7 +7124,9 @@
       <c r="I5" s="55" t="n">
         <v>2149.65000000000009</v>
       </c>
-      <c r="J5" s="55"/>
+      <c r="J5" s="55" t="n">
+        <v>1986.15000000000009</v>
+      </c>
       <c r="K5" s="55"/>
       <c r="L5" s="55"/>
       <c r="N5" s="51" t="s">
@@ -6911,7 +7153,9 @@
       <c r="U5" s="55" t="n">
         <v>3311</v>
       </c>
-      <c r="V5" s="55"/>
+      <c r="V5" s="55" t="n">
+        <v>3439</v>
+      </c>
       <c r="W5" s="55"/>
       <c r="X5" s="55"/>
       <c r="Z5" s="50" t="s">
@@ -6938,7 +7182,9 @@
       <c r="AG5" s="55" t="n">
         <v>69677.3399999999965</v>
       </c>
-      <c r="AH5" s="55"/>
+      <c r="AH5" s="55" t="n">
+        <v>62006.8099999999977</v>
+      </c>
       <c r="AI5" s="55"/>
       <c r="AJ5" s="55"/>
     </row>
@@ -6982,7 +7228,9 @@
       <c r="U6" s="55" t="n">
         <v>36870.5899999999965</v>
       </c>
-      <c r="V6" s="55"/>
+      <c r="V6" s="55" t="n">
+        <v>39977.8199999999997</v>
+      </c>
       <c r="W6" s="55"/>
       <c r="X6" s="55"/>
       <c r="Z6" s="50" t="s">
@@ -7009,7 +7257,9 @@
       <c r="AG6" s="55" t="n">
         <v>31079.4199999999983</v>
       </c>
-      <c r="AH6" s="55"/>
+      <c r="AH6" s="55" t="n">
+        <v>32380.7000000000007</v>
+      </c>
       <c r="AI6" s="55"/>
       <c r="AJ6" s="55"/>
     </row>
@@ -7038,7 +7288,9 @@
       <c r="I7" s="55" t="n">
         <v>6635</v>
       </c>
-      <c r="J7" s="55"/>
+      <c r="J7" s="55" t="n">
+        <v>6635</v>
+      </c>
       <c r="K7" s="55"/>
       <c r="L7" s="55"/>
       <c r="N7" s="51" t="s">
@@ -7065,7 +7317,9 @@
       <c r="U7" s="55" t="n">
         <v>4810</v>
       </c>
-      <c r="V7" s="55"/>
+      <c r="V7" s="55" t="n">
+        <v>4797</v>
+      </c>
       <c r="W7" s="55"/>
       <c r="X7" s="55"/>
       <c r="Z7" s="50" t="s">
@@ -7092,7 +7346,9 @@
       <c r="AG7" s="55" t="n">
         <v>39439.8899999999994</v>
       </c>
-      <c r="AH7" s="55"/>
+      <c r="AH7" s="55" t="n">
+        <v>40887.3000000000029</v>
+      </c>
       <c r="AI7" s="55"/>
       <c r="AJ7" s="55"/>
     </row>
@@ -7121,7 +7377,9 @@
       <c r="I8" s="55" t="n">
         <v>17882</v>
       </c>
-      <c r="J8" s="55"/>
+      <c r="J8" s="55" t="n">
+        <v>19769</v>
+      </c>
       <c r="K8" s="55"/>
       <c r="L8" s="55"/>
       <c r="N8" s="51" t="s">
@@ -7163,7 +7421,9 @@
       <c r="AG8" s="55" t="n">
         <v>78690.7200000000012</v>
       </c>
-      <c r="AH8" s="55"/>
+      <c r="AH8" s="55" t="n">
+        <v>82166.3800000000047</v>
+      </c>
       <c r="AI8" s="55"/>
       <c r="AJ8" s="55"/>
     </row>
@@ -7192,7 +7452,9 @@
       <c r="I9" s="55" t="n">
         <v>1068</v>
       </c>
-      <c r="J9" s="55"/>
+      <c r="J9" s="55" t="n">
+        <v>1068</v>
+      </c>
       <c r="K9" s="55"/>
       <c r="L9" s="55"/>
       <c r="N9" s="51" t="s">
@@ -7234,7 +7496,9 @@
       <c r="AG9" s="55" t="n">
         <v>42908.7900000000009</v>
       </c>
-      <c r="AH9" s="55"/>
+      <c r="AH9" s="55" t="n">
+        <v>42507.9499999999971</v>
+      </c>
       <c r="AI9" s="55"/>
       <c r="AJ9" s="55"/>
     </row>
@@ -7263,7 +7527,9 @@
       <c r="I10" s="55" t="n">
         <v>1174</v>
       </c>
-      <c r="J10" s="55"/>
+      <c r="J10" s="55" t="n">
+        <v>1174</v>
+      </c>
       <c r="K10" s="55"/>
       <c r="L10" s="55"/>
       <c r="N10" s="51" t="s">
@@ -7305,13 +7571,15 @@
       <c r="AG10" s="55" t="n">
         <v>49587.010000000002</v>
       </c>
-      <c r="AH10" s="55"/>
+      <c r="AH10" s="55" t="n">
+        <v>50601.8799999999974</v>
+      </c>
       <c r="AI10" s="55"/>
       <c r="AJ10" s="55"/>
     </row>
     <row r="11" spans="2:36">
       <c r="B11" s="50" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" s="50" t="n">
         <v>39</v>
@@ -7334,11 +7602,13 @@
       <c r="I11" s="55" t="n">
         <v>4586.39999999999964</v>
       </c>
-      <c r="J11" s="55"/>
+      <c r="J11" s="55" t="n">
+        <v>4324.48999999999978</v>
+      </c>
       <c r="K11" s="55"/>
       <c r="L11" s="55"/>
       <c r="N11" s="51" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O11" s="51" t="n">
         <v>323</v>
@@ -7353,7 +7623,7 @@
       <c r="W11" s="55"/>
       <c r="X11" s="55"/>
       <c r="Z11" s="50" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AA11" s="50" t="n">
         <v>169</v>
@@ -7376,13 +7646,15 @@
       <c r="AG11" s="55" t="n">
         <v>69909.4400000000023</v>
       </c>
-      <c r="AH11" s="55"/>
+      <c r="AH11" s="55" t="n">
+        <v>72191.5500000000029</v>
+      </c>
       <c r="AI11" s="55"/>
       <c r="AJ11" s="55"/>
     </row>
     <row r="12" spans="2:36">
       <c r="B12" s="50" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" s="50" t="n">
         <v>95</v>
@@ -7405,11 +7677,13 @@
       <c r="I12" s="55" t="n">
         <v>50245.0699999999997</v>
       </c>
-      <c r="J12" s="55"/>
+      <c r="J12" s="55" t="n">
+        <v>53622.8899999999994</v>
+      </c>
       <c r="K12" s="55"/>
       <c r="L12" s="55"/>
       <c r="N12" s="51" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="O12" s="51" t="n">
         <v>499</v>
@@ -7424,7 +7698,7 @@
       <c r="W12" s="55"/>
       <c r="X12" s="55"/>
       <c r="Z12" s="50" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AA12" s="50" t="n">
         <v>198</v>
@@ -7447,13 +7721,15 @@
       <c r="AG12" s="55" t="n">
         <v>34202.9599999999991</v>
       </c>
-      <c r="AH12" s="55"/>
+      <c r="AH12" s="55" t="n">
+        <v>39882.4300000000003</v>
+      </c>
       <c r="AI12" s="55"/>
       <c r="AJ12" s="55"/>
     </row>
     <row r="13" spans="2:36">
       <c r="B13" s="50" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" s="50" t="n">
         <v>43</v>
@@ -7476,11 +7752,13 @@
       <c r="I13" s="55" t="n">
         <v>12573</v>
       </c>
-      <c r="J13" s="55"/>
+      <c r="J13" s="55" t="n">
+        <v>13041</v>
+      </c>
       <c r="K13" s="55"/>
       <c r="L13" s="55"/>
       <c r="N13" s="51" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O13" s="51" t="n">
         <v>36</v>
@@ -7503,11 +7781,13 @@
       <c r="U13" s="55" t="n">
         <v>7839</v>
       </c>
-      <c r="V13" s="55"/>
+      <c r="V13" s="55" t="n">
+        <v>8281</v>
+      </c>
       <c r="W13" s="55"/>
       <c r="X13" s="55"/>
       <c r="Z13" s="50" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AA13" s="50" t="n">
         <v>224</v>
@@ -7530,13 +7810,15 @@
       <c r="AG13" s="55" t="n">
         <v>38200.6500000000015</v>
       </c>
-      <c r="AH13" s="55"/>
+      <c r="AH13" s="55" t="n">
+        <v>38509.5299999999988</v>
+      </c>
       <c r="AI13" s="55"/>
       <c r="AJ13" s="55"/>
     </row>
     <row r="14" spans="2:36">
       <c r="B14" s="50" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" s="50" t="n">
         <v>135</v>
@@ -7559,11 +7841,13 @@
       <c r="I14" s="55" t="n">
         <v>1490</v>
       </c>
-      <c r="J14" s="55"/>
+      <c r="J14" s="55" t="n">
+        <v>1884.68000000000006</v>
+      </c>
       <c r="K14" s="55"/>
       <c r="L14" s="55"/>
       <c r="N14" s="51" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O14" s="51" t="n">
         <v>75</v>
@@ -7586,11 +7870,13 @@
       <c r="U14" s="55" t="n">
         <v>15712.9599999999991</v>
       </c>
-      <c r="V14" s="55"/>
+      <c r="V14" s="55" t="n">
+        <v>16197.6200000000008</v>
+      </c>
       <c r="W14" s="55"/>
       <c r="X14" s="55"/>
       <c r="Z14" s="50" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AA14" s="50" t="n">
         <v>329</v>
@@ -7613,13 +7899,15 @@
       <c r="AG14" s="55" t="n">
         <v>67419.5899999999965</v>
       </c>
-      <c r="AH14" s="55"/>
+      <c r="AH14" s="55" t="n">
+        <v>62172.2799999999988</v>
+      </c>
       <c r="AI14" s="55"/>
       <c r="AJ14" s="55"/>
     </row>
     <row r="15" spans="2:36">
       <c r="B15" s="50" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C15" s="50" t="n">
         <v>10</v>
@@ -7642,11 +7930,13 @@
       <c r="I15" s="55" t="n">
         <v>1884.68000000000006</v>
       </c>
-      <c r="J15" s="55"/>
+      <c r="J15" s="55" t="n">
+        <v>1884.68000000000006</v>
+      </c>
       <c r="K15" s="55"/>
       <c r="L15" s="55"/>
       <c r="N15" s="51" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O15" s="51" t="n">
         <v>112</v>
@@ -7669,11 +7959,13 @@
       <c r="U15" s="55" t="n">
         <v>20666.0699999999997</v>
       </c>
-      <c r="V15" s="55"/>
+      <c r="V15" s="55" t="n">
+        <v>20349.9199999999983</v>
+      </c>
       <c r="W15" s="55"/>
       <c r="X15" s="55"/>
       <c r="Z15" s="50" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AA15" s="50" t="n">
         <v>751</v>
@@ -7696,7 +7988,7 @@
     </row>
     <row r="16" spans="2:36">
       <c r="B16" s="50" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C16" s="50" t="n">
         <v>97</v>
@@ -7719,11 +8011,13 @@
       <c r="I16" s="55" t="n">
         <v>4633.18000000000029</v>
       </c>
-      <c r="J16" s="55"/>
+      <c r="J16" s="55" t="n">
+        <v>4510.59000000000015</v>
+      </c>
       <c r="K16" s="55"/>
       <c r="L16" s="55"/>
       <c r="N16" s="51" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="O16" s="51" t="n">
         <v>150</v>
@@ -7746,11 +8040,13 @@
       <c r="U16" s="55" t="n">
         <v>23526.0600000000013</v>
       </c>
-      <c r="V16" s="55"/>
+      <c r="V16" s="55" t="n">
+        <v>21685.4900000000016</v>
+      </c>
       <c r="W16" s="55"/>
       <c r="X16" s="55"/>
       <c r="Z16" s="50" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AA16" s="50" t="n">
         <v>74</v>
@@ -7773,13 +8069,15 @@
       <c r="AG16" s="55" t="n">
         <v>923.110000000000014</v>
       </c>
-      <c r="AH16" s="55"/>
+      <c r="AH16" s="55" t="n">
+        <v>946.850000000000023</v>
+      </c>
       <c r="AI16" s="55"/>
       <c r="AJ16" s="55"/>
     </row>
     <row r="17" spans="2:36">
       <c r="B17" s="50" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C17" s="50" t="n">
         <v>112</v>
@@ -7802,11 +8100,13 @@
       <c r="I17" s="55" t="n">
         <v>4874.36999999999989</v>
       </c>
-      <c r="J17" s="55"/>
+      <c r="J17" s="55" t="n">
+        <v>4972.60000000000036</v>
+      </c>
       <c r="K17" s="55"/>
       <c r="L17" s="55"/>
       <c r="N17" s="51" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O17" s="51" t="n">
         <v>75</v>
@@ -7829,11 +8129,13 @@
       <c r="U17" s="55" t="n">
         <v>18160.3199999999997</v>
       </c>
-      <c r="V17" s="55"/>
+      <c r="V17" s="55" t="n">
+        <v>17264.5499999999993</v>
+      </c>
       <c r="W17" s="55"/>
       <c r="X17" s="55"/>
       <c r="Z17" s="50" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AA17" s="50" t="n">
         <v>146</v>
@@ -7856,13 +8158,15 @@
       <c r="AG17" s="55" t="n">
         <v>1867.75</v>
       </c>
-      <c r="AH17" s="55"/>
+      <c r="AH17" s="55" t="n">
+        <v>1804.08999999999992</v>
+      </c>
       <c r="AI17" s="55"/>
       <c r="AJ17" s="55"/>
     </row>
     <row r="18" spans="2:36">
       <c r="B18" s="50" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" s="50" t="n">
         <v>31</v>
@@ -7885,11 +8189,13 @@
       <c r="I18" s="55" t="n">
         <v>390</v>
       </c>
-      <c r="J18" s="55"/>
+      <c r="J18" s="55" t="n">
+        <v>390</v>
+      </c>
       <c r="K18" s="55"/>
       <c r="L18" s="55"/>
       <c r="N18" s="51" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O18" s="51" t="n">
         <v>112</v>
@@ -7912,11 +8218,13 @@
       <c r="U18" s="55" t="n">
         <v>19505.7599999999984</v>
       </c>
-      <c r="V18" s="55"/>
+      <c r="V18" s="55" t="n">
+        <v>19459.4000000000015</v>
+      </c>
       <c r="W18" s="55"/>
       <c r="X18" s="55"/>
       <c r="Z18" s="50" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AA18" s="50" t="n">
         <v>431</v>
@@ -7937,13 +8245,15 @@
         <v>5334.69999999999982</v>
       </c>
       <c r="AG18" s="55"/>
-      <c r="AH18" s="55"/>
+      <c r="AH18" s="55" t="n">
+        <v>5421.56999999999971</v>
+      </c>
       <c r="AI18" s="55"/>
       <c r="AJ18" s="55"/>
     </row>
     <row r="19" spans="2:36">
       <c r="B19" s="50" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C19" s="50" t="n">
         <v>38</v>
@@ -7966,11 +8276,13 @@
       <c r="I19" s="55" t="n">
         <v>318.279999999999973</v>
       </c>
-      <c r="J19" s="55"/>
+      <c r="J19" s="55" t="n">
+        <v>286.550000000000011</v>
+      </c>
       <c r="K19" s="55"/>
       <c r="L19" s="55"/>
       <c r="N19" s="51" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="O19" s="51" t="n">
         <v>150</v>
@@ -7993,11 +8305,13 @@
       <c r="U19" s="55" t="n">
         <v>23838.380000000001</v>
       </c>
-      <c r="V19" s="55"/>
+      <c r="V19" s="55" t="n">
+        <v>24834.4300000000003</v>
+      </c>
       <c r="W19" s="55"/>
       <c r="X19" s="55"/>
       <c r="Z19" s="50" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AA19" s="50" t="n">
         <v>587</v>
@@ -8020,7 +8334,7 @@
     </row>
     <row r="20" spans="2:36">
       <c r="B20" s="50" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C20" s="50" t="n">
         <v>57</v>
@@ -8043,11 +8357,13 @@
       <c r="I20" s="55" t="n">
         <v>373.069999999999993</v>
       </c>
-      <c r="J20" s="55"/>
+      <c r="J20" s="55" t="n">
+        <v>365.110000000000014</v>
+      </c>
       <c r="K20" s="55"/>
       <c r="L20" s="55"/>
       <c r="N20" s="51" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O20" s="51" t="n">
         <v>75</v>
@@ -8070,11 +8386,13 @@
       <c r="U20" s="55" t="n">
         <v>18188.3199999999997</v>
       </c>
-      <c r="V20" s="55"/>
+      <c r="V20" s="55" t="n">
+        <v>17267.5800000000017</v>
+      </c>
       <c r="W20" s="55"/>
       <c r="X20" s="55"/>
       <c r="Z20" s="50" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AA20" s="50" t="n">
         <v>131</v>
@@ -8097,13 +8415,15 @@
       <c r="AG20" s="55" t="n">
         <v>16073</v>
       </c>
-      <c r="AH20" s="55"/>
+      <c r="AH20" s="55" t="n">
+        <v>16124</v>
+      </c>
       <c r="AI20" s="55"/>
       <c r="AJ20" s="55"/>
     </row>
     <row r="21" spans="2:36">
       <c r="B21" s="50" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C21" s="50" t="n">
         <v>75</v>
@@ -8126,11 +8446,13 @@
       <c r="I21" s="55" t="n">
         <v>444.620000000000005</v>
       </c>
-      <c r="J21" s="55"/>
+      <c r="J21" s="55" t="n">
+        <v>447.649999999999977</v>
+      </c>
       <c r="K21" s="55"/>
       <c r="L21" s="55"/>
       <c r="N21" s="51" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="O21" s="51" t="n">
         <v>75</v>
@@ -8153,11 +8475,13 @@
       <c r="U21" s="55" t="n">
         <v>16911.5200000000004</v>
       </c>
-      <c r="V21" s="55"/>
+      <c r="V21" s="55" t="n">
+        <v>16977.3499999999985</v>
+      </c>
       <c r="W21" s="55"/>
       <c r="X21" s="55"/>
       <c r="Z21" s="50" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA21" s="50" t="n">
         <v>401</v>
@@ -8180,13 +8504,15 @@
       <c r="AG21" s="55" t="n">
         <v>35323</v>
       </c>
-      <c r="AH21" s="55"/>
+      <c r="AH21" s="55" t="n">
+        <v>35918</v>
+      </c>
       <c r="AI21" s="55"/>
       <c r="AJ21" s="55"/>
     </row>
     <row r="22" spans="2:36">
       <c r="B22" s="50" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C22" s="50" t="n">
         <v>19</v>
@@ -8209,11 +8535,13 @@
       <c r="I22" s="55" t="n">
         <v>528</v>
       </c>
-      <c r="J22" s="55"/>
+      <c r="J22" s="55" t="n">
+        <v>553</v>
+      </c>
       <c r="K22" s="55"/>
       <c r="L22" s="55"/>
       <c r="N22" s="51" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O22" s="51" t="n">
         <v>75</v>
@@ -8236,11 +8564,13 @@
       <c r="U22" s="55" t="n">
         <v>16746.6899999999987</v>
       </c>
-      <c r="V22" s="55"/>
+      <c r="V22" s="55" t="n">
+        <v>16892.0299999999988</v>
+      </c>
       <c r="W22" s="55"/>
       <c r="X22" s="55"/>
       <c r="Z22" s="50" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AA22" s="50" t="n">
         <v>774</v>
@@ -8263,7 +8593,7 @@
     </row>
     <row r="23" spans="2:36">
       <c r="B23" s="50" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C23" s="50" t="n">
         <v>196</v>
@@ -8286,11 +8616,13 @@
       <c r="I23" s="55" t="n">
         <v>1907.04999999999995</v>
       </c>
-      <c r="J23" s="55"/>
+      <c r="J23" s="55" t="n">
+        <v>1852.1099999999999</v>
+      </c>
       <c r="K23" s="55"/>
       <c r="L23" s="55"/>
       <c r="N23" s="51" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O23" s="51" t="n">
         <v>78</v>
@@ -8313,11 +8645,13 @@
       <c r="U23" s="55" t="n">
         <v>8672.70999999999913</v>
       </c>
-      <c r="V23" s="55"/>
+      <c r="V23" s="55" t="n">
+        <v>9242.6200000000008</v>
+      </c>
       <c r="W23" s="55"/>
       <c r="X23" s="55"/>
       <c r="Z23" s="50" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AA23" s="50" t="n">
         <v>52</v>
@@ -8340,13 +8674,15 @@
       <c r="AG23" s="55" t="n">
         <v>433.589999999999975</v>
       </c>
-      <c r="AH23" s="55"/>
+      <c r="AH23" s="55" t="n">
+        <v>510.810000000000002</v>
+      </c>
       <c r="AI23" s="55"/>
       <c r="AJ23" s="55"/>
     </row>
     <row r="24" spans="2:36">
       <c r="B24" s="50" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C24" s="50" t="n">
         <v>12</v>
@@ -8369,11 +8705,13 @@
       <c r="I24" s="55" t="n">
         <v>813</v>
       </c>
-      <c r="J24" s="55"/>
+      <c r="J24" s="55" t="n">
+        <v>640</v>
+      </c>
       <c r="K24" s="55"/>
       <c r="L24" s="55"/>
       <c r="N24" s="51" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O24" s="51" t="n">
         <v>238</v>
@@ -8396,11 +8734,13 @@
       <c r="U24" s="55" t="n">
         <v>32866.010000000002</v>
       </c>
-      <c r="V24" s="55"/>
+      <c r="V24" s="55" t="n">
+        <v>34393.5999999999985</v>
+      </c>
       <c r="W24" s="55"/>
       <c r="X24" s="55"/>
       <c r="Z24" s="50" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AA24" s="50" t="n">
         <v>31</v>
@@ -8423,13 +8763,15 @@
       <c r="AG24" s="55" t="n">
         <v>727</v>
       </c>
-      <c r="AH24" s="55"/>
+      <c r="AH24" s="55" t="n">
+        <v>719</v>
+      </c>
       <c r="AI24" s="55"/>
       <c r="AJ24" s="55"/>
     </row>
     <row r="25" spans="2:36">
       <c r="B25" s="50" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C25" s="50" t="n">
         <v>15</v>
@@ -8452,11 +8794,13 @@
       <c r="I25" s="55" t="n">
         <v>1276</v>
       </c>
-      <c r="J25" s="55"/>
+      <c r="J25" s="55" t="n">
+        <v>1276</v>
+      </c>
       <c r="K25" s="55"/>
       <c r="L25" s="55"/>
       <c r="N25" s="51" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="O25" s="51" t="n">
         <v>1034</v>
@@ -8477,7 +8821,7 @@
       <c r="W25" s="55"/>
       <c r="X25" s="55"/>
       <c r="Z25" s="50" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AA25" s="50" t="n">
         <v>168</v>
@@ -8500,13 +8844,15 @@
       <c r="AG25" s="55" t="n">
         <v>102850.229999999996</v>
       </c>
-      <c r="AH25" s="55"/>
+      <c r="AH25" s="55" t="n">
+        <v>87227.9199999999983</v>
+      </c>
       <c r="AI25" s="55"/>
       <c r="AJ25" s="55"/>
     </row>
     <row r="26" spans="2:36">
       <c r="B26" s="50" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C26" s="50" t="n">
         <v>18</v>
@@ -8529,11 +8875,13 @@
       <c r="I26" s="55" t="n">
         <v>802</v>
       </c>
-      <c r="J26" s="55"/>
+      <c r="J26" s="55" t="n">
+        <v>802</v>
+      </c>
       <c r="K26" s="55"/>
       <c r="L26" s="55"/>
       <c r="N26" s="51" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="O26" s="51" t="n">
         <v>420</v>
@@ -8556,11 +8904,13 @@
       <c r="U26" s="55" t="n">
         <v>2012</v>
       </c>
-      <c r="V26" s="55"/>
+      <c r="V26" s="55" t="n">
+        <v>2114</v>
+      </c>
       <c r="W26" s="55"/>
       <c r="X26" s="55"/>
       <c r="Z26" s="50" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AA26" s="50" t="n">
         <v>168</v>
@@ -8583,13 +8933,15 @@
       <c r="AG26" s="55" t="n">
         <v>3123.67000000000007</v>
       </c>
-      <c r="AH26" s="55"/>
+      <c r="AH26" s="55" t="n">
+        <v>2844.80999999999995</v>
+      </c>
       <c r="AI26" s="55"/>
       <c r="AJ26" s="55"/>
     </row>
     <row r="27" spans="26:36">
       <c r="Z27" s="50" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AA27" s="50" t="n">
         <v>12</v>
@@ -8612,13 +8964,15 @@
       <c r="AG27" s="55" t="n">
         <v>2852.11000000000013</v>
       </c>
-      <c r="AH27" s="55"/>
+      <c r="AH27" s="55" t="n">
+        <v>2852.11000000000013</v>
+      </c>
       <c r="AI27" s="55"/>
       <c r="AJ27" s="55"/>
     </row>
     <row r="28" spans="26:36">
       <c r="Z28" s="50" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AA28" s="50" t="n">
         <v>16</v>
@@ -8641,9 +8995,16 @@
       <c r="AG28" s="55" t="n">
         <v>2936.28999999999996</v>
       </c>
-      <c r="AH28" s="55"/>
+      <c r="AH28" s="55" t="n">
+        <v>2936.28999999999996</v>
+      </c>
       <c r="AI28" s="55"/>
       <c r="AJ28" s="55"/>
+    </row>
+    <row r="29" spans="34:34">
+      <c r="AH29" s="54" t="s">
+        <v>85</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -8663,7 +9024,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1643199832" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1643203916" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -8672,16 +9033,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1643199832" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1643199832" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1643199832" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1643199832" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1643203916" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1643203916" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1643203916" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1643203916" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1643199832" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1643203916" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Atualização tabela de buscas locais
</commit_message>
<xml_diff>
--- a/Comparaçoes/BuscasLocais.xlsx
+++ b/Comparaçoes/BuscasLocais.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="0" userName="pdezi"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="9570" windowHeight="8265" tabRatio="500"/>
+    <workbookView activeTab="2" xWindow="240" yWindow="60" windowWidth="9570" windowHeight="8265" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="k = n|4" sheetId="1" r:id="rId4"/>
@@ -15,10 +15,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1643203916" val="1042" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1643203916" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1643203916" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1643203916"/>
+      <pm:revision xmlns:pm="smNativeData" day="1643288762" val="1042" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1643288762" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1643288762" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1643288762"/>
     </ext>
   </extLst>
 </workbook>
@@ -198,6 +198,9 @@
     <t>rat783</t>
   </si>
   <si>
+    <t>2207.6</t>
+  </si>
+  <si>
     <t>eil76</t>
   </si>
   <si>
@@ -270,16 +273,13 @@
     <t>k = n/2</t>
   </si>
   <si>
-    <t>2092.28</t>
+    <t>k = 3n/4</t>
   </si>
   <si>
-    <t>1981.15</t>
+    <t>37162.88</t>
   </si>
   <si>
-    <t>2062.35</t>
-  </si>
-  <si>
-    <t>k = 3n/4</t>
+    <t>802C:\Users\pdezi\Desktop\Iniciação Científica\GitHub\Instâncias\</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -313,7 +313,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643288762" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -328,7 +328,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643288762" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -343,7 +343,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643288762" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -358,7 +358,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="FFFFFF" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643288762" fgClr="FFFFFF" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -374,7 +374,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="FFFFFF" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643288762" fgClr="FFFFFF" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
@@ -390,7 +390,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="FA7D00" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643288762" fgClr="FA7D00" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
@@ -405,7 +405,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="FA7D00" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643288762" fgClr="FA7D00" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -421,7 +421,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="800080" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643288762" fgClr="800080" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -437,7 +437,7 @@
       <u val="single"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="0000FF" ulstyle="single" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643288762" fgClr="0000FF" ulstyle="single" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -453,7 +453,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="7F7F7F" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643288762" fgClr="7F7F7F" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" i="1"/>
             <pm:cs face="Times New Roman" sz="220" lang="default" i="1"/>
             <pm:ea face="SimSun" sz="220" lang="default" i="1"/>
@@ -468,7 +468,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="FF0000" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643288762" fgClr="FF0000" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -484,7 +484,7 @@
       <sz val="18"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="44546A" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643288762" fgClr="44546A" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="360" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="360" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="360" lang="default" weight="bold"/>
@@ -499,7 +499,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="9C6500" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643288762" fgClr="9C6500" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -515,7 +515,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643288762" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
@@ -531,7 +531,7 @@
       <sz val="15"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="44546A" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643288762" fgClr="44546A" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="300" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="300" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="300" lang="default" weight="bold"/>
@@ -547,7 +547,7 @@
       <sz val="13"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="44546A" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643288762" fgClr="44546A" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="260" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="260" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="260" lang="default" weight="bold"/>
@@ -563,7 +563,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="44546A" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643288762" fgClr="44546A" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
@@ -579,7 +579,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="3F3F3F" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643288762" fgClr="3F3F3F" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="220" lang="default" weight="bold"/>
             <pm:ea face="SimSun" sz="220" lang="default" weight="bold"/>
@@ -594,7 +594,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="3F3F76" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643288762" fgClr="3F3F76" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -609,7 +609,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="006100" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643288762" fgClr="006100" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -624,7 +624,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1643203916" fgClr="9C0006" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1643288762" fgClr="9C0006" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Times New Roman" sz="220" lang="default"/>
             <pm:ea face="SimSun" sz="220" lang="default"/>
@@ -646,7 +646,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00FFE697" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00FFE697" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -660,7 +660,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00A5A5A5" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00A5A5A5" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -671,7 +671,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00EBEBEB" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00EBEBEB" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -682,7 +682,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00F8CAAB" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00F8CAAB" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -693,7 +693,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00FFFFCC" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -704,7 +704,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00C5DFB3" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00C5DFB3" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -715,7 +715,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00A5A5A5" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00A5A5A5" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -729,7 +729,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00FFC000" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00FFC000" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -740,7 +740,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="004472C4" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="004472C4" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -754,7 +754,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="0070AD47" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="0070AD47" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -765,7 +765,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00FFCC99" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00FFCC99" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -776,7 +776,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00F2F2F2" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00F2F2F2" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -787,7 +787,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00F2F2F2" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00F2F2F2" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -801,7 +801,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00BDD7EE" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00BDD7EE" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -812,7 +812,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00C6EFCE" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00C6EFCE" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -823,7 +823,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00FFC7CE" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00FFC7CE" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -834,7 +834,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00FFEB9C" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00FFEB9C" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -845,7 +845,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00D9E1F2" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00D9E1F2" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -856,7 +856,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="005B9BD5" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="005B9BD5" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -867,7 +867,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00DDEBF7" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00DDEBF7" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -878,7 +878,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="009BC2E6" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="009BC2E6" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -889,7 +889,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00E1EFD8" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00E1EFD8" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -900,7 +900,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00ED7D31" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00ED7D31" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -911,7 +911,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00FBE3D5" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00FBE3D5" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -922,7 +922,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00F4AF82" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00F4AF82" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -933,7 +933,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00D9D9D9" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00D9D9D9" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -944,7 +944,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00C7C7C7" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00C7C7C7" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -955,7 +955,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00FFF2CA" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00FFF2CA" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -966,7 +966,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00FFD964" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00FFD964" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -977,7 +977,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00B4C6E7" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00B4C6E7" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -988,7 +988,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="008EA9DB" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="008EA9DB" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -999,7 +999,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00A8D08C" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00A8D08C" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1013,7 +1013,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="0" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1024,7 +1024,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1643203916" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1643288762" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -1046,7 +1046,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1065,7 +1065,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1084,7 +1084,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916">
+          <pm:border xmlns:pm="smNativeData" id="1643288762">
             <pm:line position="bottom" type="2" style="0" width="20" dist="20" width2="20" rgb="FF8001"/>
           </pm:border>
         </ext>
@@ -1105,7 +1105,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916">
+          <pm:border xmlns:pm="smNativeData" id="1643288762">
             <pm:line position="top" type="2" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
             <pm:line position="bottom" type="2" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
             <pm:line position="left" type="2" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
@@ -1129,7 +1129,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1148,7 +1148,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1167,7 +1167,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916">
+          <pm:border xmlns:pm="smNativeData" id="1643288762">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="B2B2B2"/>
@@ -1191,7 +1191,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1210,7 +1210,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1229,7 +1229,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916">
+          <pm:border xmlns:pm="smNativeData" id="1643288762">
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="5B9BD5"/>
           </pm:border>
         </ext>
@@ -1250,7 +1250,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1269,7 +1269,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1288,7 +1288,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916">
+          <pm:border xmlns:pm="smNativeData" id="1643288762">
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="ACCCEA"/>
           </pm:border>
         </ext>
@@ -1309,7 +1309,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1328,7 +1328,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916">
+          <pm:border xmlns:pm="smNativeData" id="1643288762">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
@@ -1352,7 +1352,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916">
+          <pm:border xmlns:pm="smNativeData" id="1643288762">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="3F3F3F"/>
@@ -1376,7 +1376,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916">
+          <pm:border xmlns:pm="smNativeData" id="1643288762">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="7F7F7F"/>
@@ -1400,7 +1400,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916">
+          <pm:border xmlns:pm="smNativeData" id="1643288762">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="5B9BD5"/>
             <pm:line position="bottom" type="2" style="0" width="20" dist="20" width2="20" rgb="5B9BD5"/>
           </pm:border>
@@ -1422,7 +1422,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1441,7 +1441,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1460,7 +1460,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1479,7 +1479,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1498,7 +1498,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1517,7 +1517,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1536,7 +1536,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1555,7 +1555,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1574,7 +1574,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1593,7 +1593,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1612,7 +1612,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1631,7 +1631,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1650,7 +1650,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1669,7 +1669,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1688,7 +1688,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1707,7 +1707,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1726,7 +1726,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1745,7 +1745,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1764,7 +1764,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -1783,7 +1783,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916">
+          <pm:border xmlns:pm="smNativeData" id="1643288762">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1807,7 +1807,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916">
+          <pm:border xmlns:pm="smNativeData" id="1643288762">
             <pm:line position="top" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="20" dist="20" width2="20" rgb="000000"/>
@@ -1831,7 +1831,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1643203916"/>
+          <pm:border xmlns:pm="smNativeData" id="1643288762"/>
         </ext>
       </extLst>
     </border>
@@ -2209,10 +2209,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1643203916" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1643288762" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1643203916" count="41">
+      <pm:colors xmlns:pm="smNativeData" id="1643288762" count="41">
         <pm:color name="Cor 24" rgb="FA7D00"/>
         <pm:color name="Cor 25" rgb="800080"/>
         <pm:color name="Cor 26" rgb="44546A"/>
@@ -2518,8 +2518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AJ28"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="Z4" zoomScale="90" workbookViewId="0">
-      <selection activeCell="AH29" sqref="AH29"/>
+    <sheetView view="normal" topLeftCell="Z4" zoomScale="90" workbookViewId="0">
+      <selection activeCell="AI29" sqref="AI29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.20"/>
@@ -2773,7 +2773,9 @@
       <c r="J5" s="55" t="n">
         <v>707.340000000000032</v>
       </c>
-      <c r="K5" s="55"/>
+      <c r="K5" s="55" t="n">
+        <v>678.440000000000055</v>
+      </c>
       <c r="L5" s="55"/>
       <c r="N5" s="51" t="s">
         <v>11</v>
@@ -2802,7 +2804,9 @@
       <c r="V5" s="55" t="n">
         <v>582</v>
       </c>
-      <c r="W5" s="55"/>
+      <c r="W5" s="55" t="n">
+        <v>582</v>
+      </c>
       <c r="X5" s="55"/>
       <c r="Z5" s="51" t="s">
         <v>12</v>
@@ -2831,7 +2835,9 @@
       <c r="AH5" s="55" t="n">
         <v>25126.8400000000001</v>
       </c>
-      <c r="AI5" s="55"/>
+      <c r="AI5" s="55" t="n">
+        <v>25126.8400000000001</v>
+      </c>
       <c r="AJ5" s="55"/>
     </row>
     <row r="6" spans="2:36">
@@ -2877,7 +2883,9 @@
       <c r="V6" s="55" t="n">
         <v>10082.9699999999993</v>
       </c>
-      <c r="W6" s="55"/>
+      <c r="W6" s="55" t="n">
+        <v>10082.9699999999993</v>
+      </c>
       <c r="X6" s="55"/>
       <c r="Z6" s="51" t="s">
         <v>15</v>
@@ -2886,7 +2894,7 @@
         <v>26</v>
       </c>
       <c r="AB6" s="53" t="n">
-        <v>7769.73999999999887</v>
+        <v>7769.73999999999978</v>
       </c>
       <c r="AC6" s="53" t="n">
         <v>7564.93999999999869</v>
@@ -2906,7 +2914,9 @@
       <c r="AH6" s="55" t="n">
         <v>7537.28999999999996</v>
       </c>
-      <c r="AI6" s="55"/>
+      <c r="AI6" s="55" t="n">
+        <v>7305.55000000000018</v>
+      </c>
       <c r="AJ6" s="55"/>
     </row>
     <row r="7" spans="2:36">
@@ -2937,7 +2947,9 @@
       <c r="J7" s="55" t="n">
         <v>1373</v>
       </c>
-      <c r="K7" s="55"/>
+      <c r="K7" s="55" t="n">
+        <v>1373</v>
+      </c>
       <c r="L7" s="55"/>
       <c r="N7" s="51" t="s">
         <v>17</v>
@@ -2966,7 +2978,9 @@
       <c r="V7" s="55" t="n">
         <v>1356</v>
       </c>
-      <c r="W7" s="55"/>
+      <c r="W7" s="55" t="n">
+        <v>1356</v>
+      </c>
       <c r="X7" s="55"/>
       <c r="Z7" s="51" t="s">
         <v>18</v>
@@ -2995,7 +3009,9 @@
       <c r="AH7" s="55" t="n">
         <v>14065.4400000000005</v>
       </c>
-      <c r="AI7" s="55"/>
+      <c r="AI7" s="55" t="n">
+        <v>14065.4400000000005</v>
+      </c>
       <c r="AJ7" s="55"/>
     </row>
     <row r="8" spans="2:36">
@@ -3026,7 +3042,9 @@
       <c r="J8" s="55" t="n">
         <v>4532</v>
       </c>
-      <c r="K8" s="55"/>
+      <c r="K8" s="55" t="n">
+        <v>4397</v>
+      </c>
       <c r="L8" s="55"/>
       <c r="N8" s="51" t="s">
         <v>20</v>
@@ -3070,7 +3088,9 @@
       <c r="AH8" s="55" t="n">
         <v>23147.119999999999</v>
       </c>
-      <c r="AI8" s="55"/>
+      <c r="AI8" s="55" t="n">
+        <v>22717.369999999999</v>
+      </c>
       <c r="AJ8" s="55"/>
     </row>
     <row r="9" spans="2:36">
@@ -3101,7 +3121,9 @@
       <c r="J9" s="55" t="n">
         <v>292</v>
       </c>
-      <c r="K9" s="55"/>
+      <c r="K9" s="55" t="n">
+        <v>292</v>
+      </c>
       <c r="L9" s="55"/>
       <c r="N9" s="51" t="s">
         <v>23</v>
@@ -3145,7 +3167,9 @@
       <c r="AH9" s="55" t="n">
         <v>11480.7299999999996</v>
       </c>
-      <c r="AI9" s="55"/>
+      <c r="AI9" s="55" t="n">
+        <v>11325.3299999999999</v>
+      </c>
       <c r="AJ9" s="55"/>
     </row>
     <row r="10" spans="2:36">
@@ -3176,7 +3200,9 @@
       <c r="J10" s="55" t="n">
         <v>352</v>
       </c>
-      <c r="K10" s="55"/>
+      <c r="K10" s="55" t="n">
+        <v>352</v>
+      </c>
       <c r="L10" s="55"/>
       <c r="N10" s="51" t="s">
         <v>26</v>
@@ -3220,7 +3246,9 @@
       <c r="AH10" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="AI10" s="55"/>
+      <c r="AI10" s="55" t="n">
+        <v>15403.2600000000002</v>
+      </c>
       <c r="AJ10" s="55"/>
     </row>
     <row r="11" spans="2:36">
@@ -3251,7 +3279,9 @@
       <c r="J11" s="55" t="n">
         <v>556.809999999999945</v>
       </c>
-      <c r="K11" s="55"/>
+      <c r="K11" s="55" t="n">
+        <v>556.809999999999945</v>
+      </c>
       <c r="L11" s="55"/>
       <c r="N11" s="51" t="s">
         <v>30</v>
@@ -3295,7 +3325,9 @@
       <c r="AH11" s="55" t="n">
         <v>23231.1899999999987</v>
       </c>
-      <c r="AI11" s="55"/>
+      <c r="AI11" s="55" t="n">
+        <v>22003.0400000000009</v>
+      </c>
       <c r="AJ11" s="55"/>
     </row>
     <row r="12" spans="2:36">
@@ -3324,9 +3356,11 @@
         <v>11580.3199999999997</v>
       </c>
       <c r="J12" s="55" t="n">
-        <v>12834.5799999999999</v>
-      </c>
-      <c r="K12" s="55"/>
+        <v>12834.5800000000017</v>
+      </c>
+      <c r="K12" s="55" t="n">
+        <v>12805.7199999999993</v>
+      </c>
       <c r="L12" s="55"/>
       <c r="N12" s="51" t="s">
         <v>33</v>
@@ -3368,9 +3402,11 @@
         <v>8023.60999999999876</v>
       </c>
       <c r="AH12" s="55" t="n">
+        <v>8023.60999999999876</v>
+      </c>
+      <c r="AI12" s="55" t="n">
         <v>8023.60999999999967</v>
       </c>
-      <c r="AI12" s="55"/>
       <c r="AJ12" s="55"/>
     </row>
     <row r="13" spans="2:36">
@@ -3401,7 +3437,9 @@
       <c r="J13" s="55" t="n">
         <v>4607</v>
       </c>
-      <c r="K13" s="55"/>
+      <c r="K13" s="55" t="n">
+        <v>4607</v>
+      </c>
       <c r="L13" s="55"/>
       <c r="N13" s="51" t="s">
         <v>36</v>
@@ -3430,7 +3468,9 @@
       <c r="V13" s="55" t="n">
         <v>3155</v>
       </c>
-      <c r="W13" s="55"/>
+      <c r="W13" s="55" t="n">
+        <v>3155</v>
+      </c>
       <c r="X13" s="55"/>
       <c r="Z13" s="51" t="s">
         <v>37</v>
@@ -3451,15 +3491,17 @@
         <v>12127.2900000000009</v>
       </c>
       <c r="AF13" s="55" t="n">
-        <v>11699.6600000000017</v>
+        <v>11699.6599999999999</v>
       </c>
       <c r="AG13" s="55" t="n">
-        <v>11699.6600000000017</v>
+        <v>11699.6599999999999</v>
       </c>
       <c r="AH13" s="55" t="n">
         <v>10546.9599999999991</v>
       </c>
-      <c r="AI13" s="55"/>
+      <c r="AI13" s="55" t="n">
+        <v>10546.9599999999991</v>
+      </c>
       <c r="AJ13" s="55"/>
     </row>
     <row r="14" spans="2:36">
@@ -3490,7 +3532,9 @@
       <c r="J14" s="55" t="n">
         <v>570</v>
       </c>
-      <c r="K14" s="55"/>
+      <c r="K14" s="55" t="n">
+        <v>530</v>
+      </c>
       <c r="L14" s="55"/>
       <c r="N14" s="51" t="s">
         <v>39</v>
@@ -3519,7 +3563,9 @@
       <c r="V14" s="55" t="n">
         <v>4788.84000000000015</v>
       </c>
-      <c r="W14" s="55"/>
+      <c r="W14" s="55" t="n">
+        <v>4753.67000000000007</v>
+      </c>
       <c r="X14" s="55"/>
       <c r="Z14" s="51" t="s">
         <v>40</v>
@@ -3548,7 +3594,9 @@
       <c r="AH14" s="55" t="n">
         <v>21586.4500000000007</v>
       </c>
-      <c r="AI14" s="55"/>
+      <c r="AI14" s="55" t="n">
+        <v>21338.0400000000009</v>
+      </c>
       <c r="AJ14" s="55"/>
     </row>
     <row r="15" spans="2:36">
@@ -3579,7 +3627,9 @@
       <c r="J15" s="55" t="n">
         <v>249.879999999999995</v>
       </c>
-      <c r="K15" s="55"/>
+      <c r="K15" s="55" t="n">
+        <v>249.879999999999995</v>
+      </c>
       <c r="L15" s="55"/>
       <c r="N15" s="51" t="s">
         <v>42</v>
@@ -3606,9 +3656,11 @@
         <v>7222.10000000000036</v>
       </c>
       <c r="V15" s="55" t="n">
-        <v>7646.89999999999964</v>
-      </c>
-      <c r="W15" s="55"/>
+        <v>7646.89999999999873</v>
+      </c>
+      <c r="W15" s="55" t="n">
+        <v>7538.64999999999964</v>
+      </c>
       <c r="X15" s="55"/>
       <c r="Z15" s="51" t="s">
         <v>43</v>
@@ -3660,7 +3712,9 @@
       <c r="J16" s="55" t="n">
         <v>1215.96000000000004</v>
       </c>
-      <c r="K16" s="55"/>
+      <c r="K16" s="55" t="n">
+        <v>1154.49000000000001</v>
+      </c>
       <c r="L16" s="55"/>
       <c r="N16" s="51" t="s">
         <v>45</v>
@@ -3689,7 +3743,9 @@
       <c r="V16" s="55" t="n">
         <v>6741.10999999999967</v>
       </c>
-      <c r="W16" s="55"/>
+      <c r="W16" s="55" t="n">
+        <v>6821.1899999999996</v>
+      </c>
       <c r="X16" s="55"/>
       <c r="Z16" s="51" t="s">
         <v>46</v>
@@ -3718,7 +3774,9 @@
       <c r="AH16" s="55" t="n">
         <v>292.550000000000011</v>
       </c>
-      <c r="AI16" s="55"/>
+      <c r="AI16" s="55" t="n">
+        <v>272.980000000000018</v>
+      </c>
       <c r="AJ16" s="55"/>
     </row>
     <row r="17" spans="2:36">
@@ -3749,7 +3807,9 @@
       <c r="J17" s="55" t="n">
         <v>1245.96000000000004</v>
       </c>
-      <c r="K17" s="55"/>
+      <c r="K17" s="55" t="n">
+        <v>1245.96000000000004</v>
+      </c>
       <c r="L17" s="55"/>
       <c r="N17" s="51" t="s">
         <v>48</v>
@@ -3778,7 +3838,9 @@
       <c r="V17" s="55" t="n">
         <v>5384.90999999999985</v>
       </c>
-      <c r="W17" s="55"/>
+      <c r="W17" s="55" t="n">
+        <v>5384.90999999999985</v>
+      </c>
       <c r="X17" s="55"/>
       <c r="Z17" s="51" t="s">
         <v>49</v>
@@ -3807,7 +3869,9 @@
       <c r="AH17" s="55" t="n">
         <v>546.129999999999995</v>
       </c>
-      <c r="AI17" s="55"/>
+      <c r="AI17" s="55" t="n">
+        <v>546.129999999999995</v>
+      </c>
       <c r="AJ17" s="55"/>
     </row>
     <row r="18" spans="2:36">
@@ -3838,7 +3902,9 @@
       <c r="J18" s="55" t="n">
         <v>100</v>
       </c>
-      <c r="K18" s="55"/>
+      <c r="K18" s="55" t="n">
+        <v>100</v>
+      </c>
       <c r="L18" s="55"/>
       <c r="N18" s="51" t="s">
         <v>51</v>
@@ -3867,7 +3933,9 @@
       <c r="V18" s="55" t="n">
         <v>5396.32999999999993</v>
       </c>
-      <c r="W18" s="55"/>
+      <c r="W18" s="55" t="n">
+        <v>5396.32999999999993</v>
+      </c>
       <c r="X18" s="55"/>
       <c r="Z18" s="51" t="s">
         <v>52</v>
@@ -3896,7 +3964,9 @@
       <c r="AH18" s="55" t="n">
         <v>1700.80999999999995</v>
       </c>
-      <c r="AI18" s="55"/>
+      <c r="AI18" s="55" t="n">
+        <v>1698.68000000000006</v>
+      </c>
       <c r="AJ18" s="55"/>
     </row>
     <row r="19" spans="2:36">
@@ -3927,7 +3997,9 @@
       <c r="J19" s="55" t="n">
         <v>77.0400000000000063</v>
       </c>
-      <c r="K19" s="55"/>
+      <c r="K19" s="55" t="n">
+        <v>77.0400000000000063</v>
+      </c>
       <c r="L19" s="55"/>
       <c r="N19" s="51" t="s">
         <v>54</v>
@@ -3954,9 +4026,11 @@
         <v>8120.14000000000033</v>
       </c>
       <c r="V19" s="55" t="n">
-        <v>7231.97999999999956</v>
-      </c>
-      <c r="W19" s="55"/>
+        <v>7231.97999999999865</v>
+      </c>
+      <c r="W19" s="55" t="n">
+        <v>7202.14000000000033</v>
+      </c>
       <c r="X19" s="55"/>
       <c r="Z19" s="51" t="s">
         <v>56</v>
@@ -3981,12 +4055,14 @@
       <c r="AH19" s="55" t="n">
         <v>2218.15999999999985</v>
       </c>
-      <c r="AI19" s="55"/>
+      <c r="AI19" s="55" t="s">
+        <v>57</v>
+      </c>
       <c r="AJ19" s="55"/>
     </row>
     <row r="20" spans="2:36">
       <c r="B20" s="50" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C20" s="50" t="n">
         <v>19</v>
@@ -4012,10 +4088,12 @@
       <c r="J20" s="55" t="n">
         <v>99.4500000000000028</v>
       </c>
-      <c r="K20" s="55"/>
+      <c r="K20" s="55" t="n">
+        <v>99.4500000000000028</v>
+      </c>
       <c r="L20" s="55"/>
       <c r="N20" s="51" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O20" s="51" t="n">
         <v>25</v>
@@ -4041,10 +4119,12 @@
       <c r="V20" s="55" t="n">
         <v>4293.02000000000044</v>
       </c>
-      <c r="W20" s="55"/>
+      <c r="W20" s="55" t="n">
+        <v>4293.02000000000044</v>
+      </c>
       <c r="X20" s="55"/>
       <c r="Z20" s="51" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA20" s="51" t="n">
         <v>43</v>
@@ -4070,12 +4150,14 @@
       <c r="AH20" s="55" t="n">
         <v>5420</v>
       </c>
-      <c r="AI20" s="55"/>
+      <c r="AI20" s="55" t="n">
+        <v>5382</v>
+      </c>
       <c r="AJ20" s="55"/>
     </row>
     <row r="21" spans="2:36">
       <c r="B21" s="50" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C21" s="50" t="n">
         <v>25</v>
@@ -4101,10 +4183,12 @@
       <c r="J21" s="55" t="n">
         <v>139.620000000000005</v>
       </c>
-      <c r="K21" s="55"/>
+      <c r="K21" s="55" t="n">
+        <v>139.330000000000013</v>
+      </c>
       <c r="L21" s="55"/>
       <c r="N21" s="51" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O21" s="51" t="n">
         <v>25</v>
@@ -4130,10 +4214,12 @@
       <c r="V21" s="55" t="n">
         <v>5246.27999999999975</v>
       </c>
-      <c r="W21" s="55"/>
+      <c r="W21" s="55" t="n">
+        <v>5246.27999999999975</v>
+      </c>
       <c r="X21" s="55"/>
       <c r="Z21" s="51" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AA21" s="51" t="n">
         <v>133</v>
@@ -4159,12 +4245,14 @@
       <c r="AH21" s="55" t="n">
         <v>12196</v>
       </c>
-      <c r="AI21" s="55"/>
+      <c r="AI21" s="55" t="n">
+        <v>12194</v>
+      </c>
       <c r="AJ21" s="55"/>
     </row>
     <row r="22" spans="2:36">
       <c r="B22" s="50" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C22" s="50" t="n">
         <v>6</v>
@@ -4190,10 +4278,12 @@
       <c r="J22" s="55" t="n">
         <v>147</v>
       </c>
-      <c r="K22" s="55"/>
+      <c r="K22" s="55" t="n">
+        <v>147</v>
+      </c>
       <c r="L22" s="55"/>
       <c r="N22" s="51" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="O22" s="51" t="n">
         <v>25</v>
@@ -4219,10 +4309,12 @@
       <c r="V22" s="55" t="n">
         <v>3919.57999999999993</v>
       </c>
-      <c r="W22" s="55"/>
+      <c r="W22" s="55" t="n">
+        <v>3919.59000000000015</v>
+      </c>
       <c r="X22" s="55"/>
       <c r="Z22" s="51" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AA22" s="51" t="n">
         <v>258</v>
@@ -4249,7 +4341,7 @@
     </row>
     <row r="23" spans="2:36">
       <c r="B23" s="50" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C23" s="50" t="n">
         <v>65</v>
@@ -4275,10 +4367,12 @@
       <c r="J23" s="55" t="n">
         <v>655.799999999999955</v>
       </c>
-      <c r="K23" s="55"/>
+      <c r="K23" s="55" t="n">
+        <v>633.590000000000032</v>
+      </c>
       <c r="L23" s="55"/>
       <c r="N23" s="51" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="O23" s="51" t="n">
         <v>26</v>
@@ -4304,10 +4398,12 @@
       <c r="V23" s="55" t="n">
         <v>2002.98000000000002</v>
       </c>
-      <c r="W23" s="55"/>
+      <c r="W23" s="55" t="n">
+        <v>2002.98000000000002</v>
+      </c>
       <c r="X23" s="55"/>
       <c r="Z23" s="50" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AA23" s="50" t="n">
         <v>17</v>
@@ -4333,12 +4429,14 @@
       <c r="AH23" s="55" t="n">
         <v>127.180000000000007</v>
       </c>
-      <c r="AI23" s="55"/>
+      <c r="AI23" s="55" t="n">
+        <v>127.180000000000007</v>
+      </c>
       <c r="AJ23" s="55"/>
     </row>
     <row r="24" spans="2:36">
       <c r="B24" s="50" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C24" s="50" t="n">
         <v>4</v>
@@ -4364,10 +4462,12 @@
       <c r="J24" s="55" t="n">
         <v>154</v>
       </c>
-      <c r="K24" s="55"/>
+      <c r="K24" s="55" t="n">
+        <v>154</v>
+      </c>
       <c r="L24" s="55"/>
       <c r="N24" s="51" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O24" s="51" t="n">
         <v>79</v>
@@ -4393,10 +4493,12 @@
       <c r="V24" s="55" t="n">
         <v>9406.35000000000036</v>
       </c>
-      <c r="W24" s="55"/>
+      <c r="W24" s="55" t="n">
+        <v>9133.8799999999992</v>
+      </c>
       <c r="X24" s="55"/>
       <c r="Z24" s="51" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AA24" s="51" t="n">
         <v>10</v>
@@ -4422,12 +4524,14 @@
       <c r="AH24" s="55" t="n">
         <v>146</v>
       </c>
-      <c r="AI24" s="55"/>
+      <c r="AI24" s="55" t="n">
+        <v>146</v>
+      </c>
       <c r="AJ24" s="55"/>
     </row>
     <row r="25" spans="2:36">
       <c r="B25" s="50" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C25" s="50" t="n">
         <v>5</v>
@@ -4453,10 +4557,12 @@
       <c r="J25" s="55" t="n">
         <v>248</v>
       </c>
-      <c r="K25" s="55"/>
+      <c r="K25" s="55" t="n">
+        <v>248</v>
+      </c>
       <c r="L25" s="55"/>
       <c r="N25" s="51" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O25" s="51" t="n">
         <v>344</v>
@@ -4477,7 +4583,7 @@
       <c r="W25" s="55"/>
       <c r="X25" s="55"/>
       <c r="Z25" s="51" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AA25" s="51" t="n">
         <v>56</v>
@@ -4503,12 +4609,14 @@
       <c r="AH25" s="55" t="n">
         <v>27500</v>
       </c>
-      <c r="AI25" s="55"/>
+      <c r="AI25" s="55" t="n">
+        <v>27500</v>
+      </c>
       <c r="AJ25" s="55"/>
     </row>
     <row r="26" spans="2:36">
       <c r="B26" s="50" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C26" s="50" t="n">
         <v>6</v>
@@ -4534,10 +4642,12 @@
       <c r="J26" s="55" t="n">
         <v>162</v>
       </c>
-      <c r="K26" s="55"/>
+      <c r="K26" s="55" t="n">
+        <v>162</v>
+      </c>
       <c r="L26" s="55"/>
       <c r="N26" s="51" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="O26" s="51" t="n">
         <v>140</v>
@@ -4563,22 +4673,24 @@
       <c r="V26" s="55" t="n">
         <v>640</v>
       </c>
-      <c r="W26" s="55"/>
+      <c r="W26" s="55" t="n">
+        <v>636</v>
+      </c>
       <c r="X26" s="55"/>
       <c r="Z26" s="51" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AA26" s="51" t="n">
         <v>56</v>
       </c>
       <c r="AB26" s="53" t="n">
-        <v>964.260000000000105</v>
+        <v>964.259999999999991</v>
       </c>
       <c r="AC26" s="53" t="n">
-        <v>964.260000000000105</v>
+        <v>964.259999999999991</v>
       </c>
       <c r="AD26" s="53" t="n">
-        <v>996.510000000000105</v>
+        <v>996.509999999999991</v>
       </c>
       <c r="AE26" s="55" t="n">
         <v>1038.02999999999997</v>
@@ -4592,12 +4704,14 @@
       <c r="AH26" s="55" t="n">
         <v>1094.8900000000001</v>
       </c>
-      <c r="AI26" s="55"/>
+      <c r="AI26" s="55" t="n">
+        <v>1081.51999999999998</v>
+      </c>
       <c r="AJ26" s="55"/>
     </row>
     <row r="27" spans="26:36">
       <c r="Z27" s="50" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AA27" s="50" t="n">
         <v>4</v>
@@ -4621,14 +4735,16 @@
         <v>751.059999999999832</v>
       </c>
       <c r="AH27" s="55" t="n">
+        <v>751.059999999999832</v>
+      </c>
+      <c r="AI27" s="55" t="n">
         <v>751.059999999999945</v>
       </c>
-      <c r="AI27" s="55"/>
       <c r="AJ27" s="55"/>
     </row>
     <row r="28" spans="26:36">
       <c r="Z28" s="50" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AA28" s="50" t="n">
         <v>5</v>
@@ -4654,7 +4770,9 @@
       <c r="AH28" s="55" t="n">
         <v>456.579999999999984</v>
       </c>
-      <c r="AI28" s="55"/>
+      <c r="AI28" s="55" t="n">
+        <v>456.579999999999984</v>
+      </c>
       <c r="AJ28" s="55"/>
     </row>
   </sheetData>
@@ -4675,7 +4793,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1643203916" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1643288762" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -4684,16 +4802,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1643203916" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1643203916" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1643203916" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1643203916" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1643288762" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1643288762" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1643288762" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1643288762" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1643203916" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1643288762" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -4707,7 +4825,7 @@
   <dimension ref="B2:AJ28"/>
   <sheetViews>
     <sheetView view="normal" topLeftCell="Z4" zoomScale="90" workbookViewId="0">
-      <selection activeCell="AH28" sqref="AH28"/>
+      <selection activeCell="AG29" sqref="AG29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.20"/>
@@ -4725,7 +4843,7 @@
     <col min="18" max="18" width="9.752475" customWidth="1" style="54"/>
     <col min="19" max="20" width="9.574257" customWidth="1" style="54"/>
     <col min="21" max="26" width="9.138614" customWidth="1" style="54"/>
-    <col min="27" max="27" width="19.138614" customWidth="1" style="54"/>
+    <col min="27" max="27" width="13.524752" customWidth="1" style="54"/>
     <col min="28" max="30" width="10.861386" customWidth="1" style="54"/>
     <col min="31" max="32" width="9.574257" customWidth="1" style="54"/>
     <col min="33" max="16384" width="9.138614" customWidth="1" style="54"/>
@@ -4769,7 +4887,7 @@
     <row r="3" spans="2:36">
       <c r="B3" s="51"/>
       <c r="C3" s="51" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D3" s="49" t="s">
         <v>2</v>
@@ -4788,7 +4906,7 @@
       <c r="L3" s="49"/>
       <c r="N3" s="51"/>
       <c r="O3" s="51" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="P3" s="49" t="s">
         <v>2</v>
@@ -4807,7 +4925,7 @@
       <c r="X3" s="49"/>
       <c r="Z3" s="51"/>
       <c r="AA3" s="51" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AB3" s="49" t="s">
         <v>2</v>
@@ -4954,7 +5072,9 @@
       <c r="J5" s="55" t="n">
         <v>1328.53999999999996</v>
       </c>
-      <c r="K5" s="55"/>
+      <c r="K5" s="55" t="n">
+        <v>1289.93000000000006</v>
+      </c>
       <c r="L5" s="55"/>
       <c r="N5" s="51" t="s">
         <v>11</v>
@@ -4983,7 +5103,9 @@
       <c r="V5" s="55" t="n">
         <v>1691</v>
       </c>
-      <c r="W5" s="55"/>
+      <c r="W5" s="55" t="n">
+        <v>1691</v>
+      </c>
       <c r="X5" s="55"/>
       <c r="Z5" s="51" t="s">
         <v>12</v>
@@ -5012,7 +5134,9 @@
       <c r="AH5" s="55" t="n">
         <v>44106.739999999998</v>
       </c>
-      <c r="AI5" s="55"/>
+      <c r="AI5" s="55" t="n">
+        <v>43770.4100000000035</v>
+      </c>
       <c r="AJ5" s="55"/>
     </row>
     <row r="6" spans="2:36">
@@ -5058,7 +5182,9 @@
       <c r="V6" s="55" t="n">
         <v>26964.5200000000004</v>
       </c>
-      <c r="W6" s="55"/>
+      <c r="W6" s="55" t="n">
+        <v>26610.1599999999999</v>
+      </c>
       <c r="X6" s="55"/>
       <c r="Z6" s="51" t="s">
         <v>15</v>
@@ -5087,7 +5213,9 @@
       <c r="AH6" s="55" t="n">
         <v>16472.9799999999996</v>
       </c>
-      <c r="AI6" s="55"/>
+      <c r="AI6" s="55" t="n">
+        <v>15831.6499999999996</v>
+      </c>
       <c r="AJ6" s="55"/>
     </row>
     <row r="7" spans="2:36">
@@ -5118,7 +5246,9 @@
       <c r="J7" s="55" t="n">
         <v>3674</v>
       </c>
-      <c r="K7" s="55"/>
+      <c r="K7" s="55" t="n">
+        <v>3452</v>
+      </c>
       <c r="L7" s="55"/>
       <c r="N7" s="51" t="s">
         <v>17</v>
@@ -5147,7 +5277,9 @@
       <c r="V7" s="55" t="n">
         <v>2950</v>
       </c>
-      <c r="W7" s="55"/>
+      <c r="W7" s="55" t="n">
+        <v>2950</v>
+      </c>
       <c r="X7" s="55"/>
       <c r="Z7" s="51" t="s">
         <v>18</v>
@@ -5176,7 +5308,9 @@
       <c r="AH7" s="55" t="n">
         <v>21887.8899999999994</v>
       </c>
-      <c r="AI7" s="55"/>
+      <c r="AI7" s="55" t="n">
+        <v>21887.8899999999994</v>
+      </c>
       <c r="AJ7" s="55"/>
     </row>
     <row r="8" spans="2:36">
@@ -5207,7 +5341,9 @@
       <c r="J8" s="55" t="n">
         <v>11824</v>
       </c>
-      <c r="K8" s="55"/>
+      <c r="K8" s="55" t="n">
+        <v>11686</v>
+      </c>
       <c r="L8" s="55"/>
       <c r="N8" s="51" t="s">
         <v>20</v>
@@ -5251,7 +5387,9 @@
       <c r="AH8" s="55" t="n">
         <v>48383.8099999999977</v>
       </c>
-      <c r="AI8" s="55"/>
+      <c r="AI8" s="55" t="n">
+        <v>47304.6600000000035</v>
+      </c>
       <c r="AJ8" s="55"/>
     </row>
     <row r="9" spans="2:36">
@@ -5282,7 +5420,9 @@
       <c r="J9" s="55" t="n">
         <v>581</v>
       </c>
-      <c r="K9" s="55"/>
+      <c r="K9" s="55" t="n">
+        <v>581</v>
+      </c>
       <c r="L9" s="55"/>
       <c r="N9" s="51" t="s">
         <v>23</v>
@@ -5326,7 +5466,9 @@
       <c r="AH9" s="55" t="n">
         <v>26341.8199999999997</v>
       </c>
-      <c r="AI9" s="55"/>
+      <c r="AI9" s="55" t="n">
+        <v>26306.3400000000001</v>
+      </c>
       <c r="AJ9" s="55"/>
     </row>
     <row r="10" spans="2:36">
@@ -5357,7 +5499,9 @@
       <c r="J10" s="55" t="n">
         <v>818</v>
       </c>
-      <c r="K10" s="55"/>
+      <c r="K10" s="55" t="n">
+        <v>818</v>
+      </c>
       <c r="L10" s="55"/>
       <c r="N10" s="51" t="s">
         <v>26</v>
@@ -5401,7 +5545,9 @@
       <c r="AH10" s="55" t="n">
         <v>34036.7300000000032</v>
       </c>
-      <c r="AI10" s="55"/>
+      <c r="AI10" s="55" t="n">
+        <v>33537.8899999999994</v>
+      </c>
       <c r="AJ10" s="55"/>
     </row>
     <row r="11" spans="2:36">
@@ -5432,7 +5578,9 @@
       <c r="J11" s="55" t="n">
         <v>1813.95000000000005</v>
       </c>
-      <c r="K11" s="55"/>
+      <c r="K11" s="55" t="n">
+        <v>1766.55999999999995</v>
+      </c>
       <c r="L11" s="55"/>
       <c r="N11" s="51" t="s">
         <v>30</v>
@@ -5476,7 +5624,9 @@
       <c r="AH11" s="55" t="n">
         <v>52927.2699999999968</v>
       </c>
-      <c r="AI11" s="55"/>
+      <c r="AI11" s="55" t="n">
+        <v>52745.3600000000006</v>
+      </c>
       <c r="AJ11" s="55"/>
     </row>
     <row r="12" spans="2:36">
@@ -5507,7 +5657,9 @@
       <c r="J12" s="55" t="n">
         <v>27954.9900000000016</v>
       </c>
-      <c r="K12" s="55"/>
+      <c r="K12" s="55" t="n">
+        <v>27447.7099999999991</v>
+      </c>
       <c r="L12" s="55"/>
       <c r="N12" s="51" t="s">
         <v>33</v>
@@ -5551,7 +5703,9 @@
       <c r="AH12" s="55" t="n">
         <v>21495.7599999999984</v>
       </c>
-      <c r="AI12" s="55"/>
+      <c r="AI12" s="55" t="n">
+        <v>21327.2299999999996</v>
+      </c>
       <c r="AJ12" s="55"/>
     </row>
     <row r="13" spans="2:36">
@@ -5582,7 +5736,9 @@
       <c r="J13" s="55" t="n">
         <v>9812</v>
       </c>
-      <c r="K13" s="55"/>
+      <c r="K13" s="55" t="n">
+        <v>9828</v>
+      </c>
       <c r="L13" s="55"/>
       <c r="N13" s="51" t="s">
         <v>36</v>
@@ -5611,7 +5767,9 @@
       <c r="V13" s="55" t="n">
         <v>6289</v>
       </c>
-      <c r="W13" s="55"/>
+      <c r="W13" s="55" t="n">
+        <v>6199</v>
+      </c>
       <c r="X13" s="55"/>
       <c r="Z13" s="51" t="s">
         <v>37</v>
@@ -5640,7 +5798,9 @@
       <c r="AH13" s="55" t="n">
         <v>24783.4700000000012</v>
       </c>
-      <c r="AI13" s="55"/>
+      <c r="AI13" s="55" t="n">
+        <v>24364.1899999999987</v>
+      </c>
       <c r="AJ13" s="55"/>
     </row>
     <row r="14" spans="2:36">
@@ -5671,7 +5831,9 @@
       <c r="J14" s="55" t="n">
         <v>1090</v>
       </c>
-      <c r="K14" s="55"/>
+      <c r="K14" s="55" t="n">
+        <v>1000</v>
+      </c>
       <c r="L14" s="55"/>
       <c r="N14" s="51" t="s">
         <v>39</v>
@@ -5683,7 +5845,7 @@
         <v>11430.2199999999993</v>
       </c>
       <c r="Q14" s="53" t="n">
-        <v>10638.4100000000017</v>
+        <v>10638.4099999999999</v>
       </c>
       <c r="R14" s="53" t="n">
         <v>10809.4699999999993</v>
@@ -5700,7 +5862,9 @@
       <c r="V14" s="55" t="n">
         <v>10444.8999999999996</v>
       </c>
-      <c r="W14" s="55"/>
+      <c r="W14" s="55" t="n">
+        <v>10405.0799999999999</v>
+      </c>
       <c r="X14" s="55"/>
       <c r="Z14" s="51" t="s">
         <v>40</v>
@@ -5729,7 +5893,9 @@
       <c r="AH14" s="55" t="n">
         <v>42621.9499999999971</v>
       </c>
-      <c r="AI14" s="55"/>
+      <c r="AI14" s="55" t="n">
+        <v>40395.7300000000032</v>
+      </c>
       <c r="AJ14" s="55"/>
     </row>
     <row r="15" spans="2:36">
@@ -5760,7 +5926,9 @@
       <c r="J15" s="55" t="n">
         <v>1339.11999999999989</v>
       </c>
-      <c r="K15" s="55"/>
+      <c r="K15" s="55" t="n">
+        <v>1339.11999999999989</v>
+      </c>
       <c r="L15" s="55"/>
       <c r="N15" s="51" t="s">
         <v>42</v>
@@ -5784,12 +5952,14 @@
         <v>14693.2999999999993</v>
       </c>
       <c r="U15" s="55" t="n">
-        <v>14150.0800000000017</v>
+        <v>14150.0799999999999</v>
       </c>
       <c r="V15" s="55" t="n">
         <v>13836.7999999999993</v>
       </c>
-      <c r="W15" s="55"/>
+      <c r="W15" s="55" t="n">
+        <v>13836.7999999999993</v>
+      </c>
       <c r="X15" s="55"/>
       <c r="Z15" s="51" t="s">
         <v>43</v>
@@ -5841,7 +6011,9 @@
       <c r="J16" s="55" t="n">
         <v>2565.23000000000002</v>
       </c>
-      <c r="K16" s="55"/>
+      <c r="K16" s="55" t="n">
+        <v>2563.2800000000002</v>
+      </c>
       <c r="L16" s="55"/>
       <c r="N16" s="51" t="s">
         <v>45</v>
@@ -5870,7 +6042,9 @@
       <c r="V16" s="55" t="n">
         <v>15428.7999999999993</v>
       </c>
-      <c r="W16" s="55"/>
+      <c r="W16" s="55" t="n">
+        <v>15350.3700000000008</v>
+      </c>
       <c r="X16" s="55"/>
       <c r="Z16" s="51" t="s">
         <v>46</v>
@@ -5899,7 +6073,9 @@
       <c r="AH16" s="55" t="n">
         <v>600.549999999999955</v>
       </c>
-      <c r="AI16" s="55"/>
+      <c r="AI16" s="55" t="n">
+        <v>586.059999999999945</v>
+      </c>
       <c r="AJ16" s="55"/>
     </row>
     <row r="17" spans="2:36">
@@ -5930,7 +6106,9 @@
       <c r="J17" s="55" t="n">
         <v>3089.53999999999996</v>
       </c>
-      <c r="K17" s="55"/>
+      <c r="K17" s="55" t="n">
+        <v>3069.09999999999991</v>
+      </c>
       <c r="L17" s="55"/>
       <c r="N17" s="51" t="s">
         <v>48</v>
@@ -5959,7 +6137,9 @@
       <c r="V17" s="55" t="n">
         <v>10913.6100000000006</v>
       </c>
-      <c r="W17" s="55"/>
+      <c r="W17" s="55" t="n">
+        <v>10880.7399999999998</v>
+      </c>
       <c r="X17" s="55"/>
       <c r="Z17" s="51" t="s">
         <v>49</v>
@@ -5988,7 +6168,9 @@
       <c r="AH17" s="55" t="n">
         <v>1158.97000000000003</v>
       </c>
-      <c r="AI17" s="55"/>
+      <c r="AI17" s="55" t="n">
+        <v>1154.55999999999995</v>
+      </c>
       <c r="AJ17" s="55"/>
     </row>
     <row r="18" spans="2:36">
@@ -6019,7 +6201,9 @@
       <c r="J18" s="55" t="n">
         <v>248</v>
       </c>
-      <c r="K18" s="55"/>
+      <c r="K18" s="55" t="n">
+        <v>248</v>
+      </c>
       <c r="L18" s="55"/>
       <c r="N18" s="51" t="s">
         <v>51</v>
@@ -6048,7 +6232,9 @@
       <c r="V18" s="55" t="n">
         <v>11828.9599999999991</v>
       </c>
-      <c r="W18" s="55"/>
+      <c r="W18" s="55" t="n">
+        <v>11639.3999999999996</v>
+      </c>
       <c r="X18" s="55"/>
       <c r="Z18" s="51" t="s">
         <v>52</v>
@@ -6077,7 +6263,9 @@
       <c r="AH18" s="55" t="n">
         <v>3574.94999999999982</v>
       </c>
-      <c r="AI18" s="55"/>
+      <c r="AI18" s="55" t="n">
+        <v>3505.75</v>
+      </c>
       <c r="AJ18" s="55"/>
     </row>
     <row r="19" spans="2:36">
@@ -6108,7 +6296,9 @@
       <c r="J19" s="55" t="n">
         <v>190.340000000000003</v>
       </c>
-      <c r="K19" s="55"/>
+      <c r="K19" s="55" t="n">
+        <v>188.75</v>
+      </c>
       <c r="L19" s="55"/>
       <c r="N19" s="51" t="s">
         <v>54</v>
@@ -6137,7 +6327,9 @@
       <c r="V19" s="55" t="n">
         <v>15996.6100000000006</v>
       </c>
-      <c r="W19" s="55"/>
+      <c r="W19" s="55" t="n">
+        <v>15788.5200000000004</v>
+      </c>
       <c r="X19" s="55"/>
       <c r="Z19" s="51" t="s">
         <v>56</v>
@@ -6158,12 +6350,14 @@
       <c r="AF19" s="55"/>
       <c r="AG19" s="55"/>
       <c r="AH19" s="55"/>
-      <c r="AI19" s="55"/>
+      <c r="AI19" s="55" t="n">
+        <v>4603.60999999999967</v>
+      </c>
       <c r="AJ19" s="55"/>
     </row>
     <row r="20" spans="2:36">
       <c r="B20" s="50" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C20" s="50" t="n">
         <v>38</v>
@@ -6189,10 +6383,12 @@
       <c r="J20" s="55" t="n">
         <v>224.719999999999999</v>
       </c>
-      <c r="K20" s="55"/>
+      <c r="K20" s="55" t="n">
+        <v>224.719999999999999</v>
+      </c>
       <c r="L20" s="55"/>
       <c r="N20" s="51" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O20" s="51" t="n">
         <v>50</v>
@@ -6207,10 +6403,10 @@
         <v>9555.72999999999956</v>
       </c>
       <c r="S20" s="55" t="n">
-        <v>11703.5800000000017</v>
+        <v>11703.5799999999999</v>
       </c>
       <c r="T20" s="55" t="n">
-        <v>11550.1600000000017</v>
+        <v>11550.1599999999999</v>
       </c>
       <c r="U20" s="55" t="n">
         <v>11626.2099999999991</v>
@@ -6218,10 +6414,12 @@
       <c r="V20" s="55" t="n">
         <v>10824.7399999999998</v>
       </c>
-      <c r="W20" s="55"/>
+      <c r="W20" s="55" t="n">
+        <v>10690.6900000000005</v>
+      </c>
       <c r="X20" s="55"/>
       <c r="Z20" s="51" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA20" s="51" t="n">
         <v>87</v>
@@ -6247,12 +6445,14 @@
       <c r="AH20" s="55" t="n">
         <v>10384</v>
       </c>
-      <c r="AI20" s="55"/>
+      <c r="AI20" s="55" t="n">
+        <v>10336</v>
+      </c>
       <c r="AJ20" s="55"/>
     </row>
     <row r="21" spans="2:36">
       <c r="B21" s="50" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C21" s="50" t="n">
         <v>50</v>
@@ -6278,10 +6478,12 @@
       <c r="J21" s="55" t="n">
         <v>313.779999999999973</v>
       </c>
-      <c r="K21" s="55"/>
+      <c r="K21" s="55" t="n">
+        <v>313.490000000000009</v>
+      </c>
       <c r="L21" s="55"/>
       <c r="N21" s="51" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O21" s="51" t="n">
         <v>50</v>
@@ -6307,10 +6509,12 @@
       <c r="V21" s="55" t="n">
         <v>11197.7299999999996</v>
       </c>
-      <c r="W21" s="55"/>
+      <c r="W21" s="55" t="n">
+        <v>11197.7299999999996</v>
+      </c>
       <c r="X21" s="55"/>
       <c r="Z21" s="51" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AA21" s="51" t="n">
         <v>267</v>
@@ -6336,12 +6540,14 @@
       <c r="AH21" s="55" t="n">
         <v>23486</v>
       </c>
-      <c r="AI21" s="55"/>
+      <c r="AI21" s="55" t="n">
+        <v>23426</v>
+      </c>
       <c r="AJ21" s="55"/>
     </row>
     <row r="22" spans="2:36">
       <c r="B22" s="50" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C22" s="50" t="n">
         <v>13</v>
@@ -6367,10 +6573,12 @@
       <c r="J22" s="55" t="n">
         <v>391</v>
       </c>
-      <c r="K22" s="55"/>
+      <c r="K22" s="55" t="n">
+        <v>391</v>
+      </c>
       <c r="L22" s="55"/>
       <c r="N22" s="51" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="O22" s="51" t="n">
         <v>50</v>
@@ -6385,7 +6593,7 @@
         <v>9424.10000000000036</v>
       </c>
       <c r="S22" s="55" t="n">
-        <v>10160.4100000000017</v>
+        <v>10160.4099999999999</v>
       </c>
       <c r="T22" s="55" t="n">
         <v>9777.09000000000015</v>
@@ -6394,12 +6602,14 @@
         <v>9883.1299999999992</v>
       </c>
       <c r="V22" s="55" t="n">
+        <v>9449.58000000000175</v>
+      </c>
+      <c r="W22" s="55" t="n">
         <v>9449.57999999999993</v>
       </c>
-      <c r="W22" s="55"/>
       <c r="X22" s="55"/>
       <c r="Z22" s="51" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AA22" s="51" t="n">
         <v>516</v>
@@ -6422,7 +6632,7 @@
     </row>
     <row r="23" spans="2:36">
       <c r="B23" s="50" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C23" s="50" t="n">
         <v>131</v>
@@ -6448,10 +6658,12 @@
       <c r="J23" s="55" t="n">
         <v>1205.59999999999991</v>
       </c>
-      <c r="K23" s="55"/>
+      <c r="K23" s="55" t="n">
+        <v>1202.25</v>
+      </c>
       <c r="L23" s="55"/>
       <c r="N23" s="51" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="O23" s="51" t="n">
         <v>52</v>
@@ -6477,10 +6689,12 @@
       <c r="V23" s="55" t="n">
         <v>5838.61999999999989</v>
       </c>
-      <c r="W23" s="55"/>
+      <c r="W23" s="55" t="n">
+        <v>5666.11999999999989</v>
+      </c>
       <c r="X23" s="55"/>
       <c r="Z23" s="50" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AA23" s="50" t="n">
         <v>35</v>
@@ -6506,12 +6720,14 @@
       <c r="AH23" s="55" t="n">
         <v>282.180000000000007</v>
       </c>
-      <c r="AI23" s="55"/>
+      <c r="AI23" s="55" t="n">
+        <v>282.180000000000007</v>
+      </c>
       <c r="AJ23" s="55"/>
     </row>
     <row r="24" spans="2:36">
       <c r="B24" s="50" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C24" s="50" t="n">
         <v>8</v>
@@ -6537,10 +6753,12 @@
       <c r="J24" s="55" t="n">
         <v>359</v>
       </c>
-      <c r="K24" s="55"/>
+      <c r="K24" s="55" t="n">
+        <v>359</v>
+      </c>
       <c r="L24" s="55"/>
       <c r="N24" s="51" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O24" s="51" t="n">
         <v>159</v>
@@ -6566,10 +6784,12 @@
       <c r="V24" s="55" t="n">
         <v>21122.4700000000012</v>
       </c>
-      <c r="W24" s="55"/>
+      <c r="W24" s="55" t="n">
+        <v>20261.5299999999988</v>
+      </c>
       <c r="X24" s="55"/>
       <c r="Z24" s="51" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AA24" s="51" t="n">
         <v>21</v>
@@ -6595,12 +6815,14 @@
       <c r="AH24" s="55" t="n">
         <v>485</v>
       </c>
-      <c r="AI24" s="55"/>
+      <c r="AI24" s="55" t="n">
+        <v>483</v>
+      </c>
       <c r="AJ24" s="55"/>
     </row>
     <row r="25" spans="2:36">
       <c r="B25" s="50" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C25" s="50" t="n">
         <v>10</v>
@@ -6626,10 +6848,12 @@
       <c r="J25" s="55" t="n">
         <v>732</v>
       </c>
-      <c r="K25" s="55"/>
+      <c r="K25" s="55" t="n">
+        <v>732</v>
+      </c>
       <c r="L25" s="55"/>
       <c r="N25" s="51" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O25" s="51" t="n">
         <v>689</v>
@@ -6650,7 +6874,7 @@
       <c r="W25" s="55"/>
       <c r="X25" s="55"/>
       <c r="Z25" s="51" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AA25" s="51" t="n">
         <v>112</v>
@@ -6676,12 +6900,14 @@
       <c r="AH25" s="55" t="n">
         <v>73643.8600000000006</v>
       </c>
-      <c r="AI25" s="55"/>
+      <c r="AI25" s="55" t="n">
+        <v>69439.8000000000029</v>
+      </c>
       <c r="AJ25" s="55"/>
     </row>
     <row r="26" spans="2:36">
       <c r="B26" s="50" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C26" s="50" t="n">
         <v>12</v>
@@ -6707,10 +6933,12 @@
       <c r="J26" s="55" t="n">
         <v>413</v>
       </c>
-      <c r="K26" s="55"/>
+      <c r="K26" s="55" t="n">
+        <v>413</v>
+      </c>
       <c r="L26" s="55"/>
       <c r="N26" s="51" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="O26" s="51" t="n">
         <v>280</v>
@@ -6736,10 +6964,12 @@
       <c r="V26" s="55" t="n">
         <v>1298</v>
       </c>
-      <c r="W26" s="55"/>
+      <c r="W26" s="55" t="n">
+        <v>1278</v>
+      </c>
       <c r="X26" s="55"/>
       <c r="Z26" s="51" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AA26" s="51" t="n">
         <v>112</v>
@@ -6759,18 +6989,20 @@
       <c r="AF26" s="55" t="n">
         <v>2049.57000000000016</v>
       </c>
-      <c r="AG26" s="55" t="s">
-        <v>81</v>
+      <c r="AG26" s="55" t="n">
+        <v>2092.80000000000018</v>
       </c>
       <c r="AH26" s="55" t="n">
         <v>2166.09999999999991</v>
       </c>
-      <c r="AI26" s="55"/>
+      <c r="AI26" s="55" t="n">
+        <v>2093.96000000000004</v>
+      </c>
       <c r="AJ26" s="55"/>
     </row>
     <row r="27" spans="26:36">
       <c r="Z27" s="50" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AA27" s="50" t="n">
         <v>8</v>
@@ -6790,18 +7022,20 @@
       <c r="AF27" s="55" t="n">
         <v>1981.15000000000009</v>
       </c>
-      <c r="AG27" s="55" t="s">
-        <v>82</v>
+      <c r="AG27" s="55" t="n">
+        <v>1981.5</v>
       </c>
       <c r="AH27" s="55" t="n">
         <v>1981.15000000000009</v>
       </c>
-      <c r="AI27" s="55"/>
+      <c r="AI27" s="55" t="n">
+        <v>1981.15000000000009</v>
+      </c>
       <c r="AJ27" s="55"/>
     </row>
     <row r="28" spans="26:36">
       <c r="Z28" s="50" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AA28" s="50" t="n">
         <v>11</v>
@@ -6821,13 +7055,15 @@
       <c r="AF28" s="55" t="n">
         <v>2062.34999999999991</v>
       </c>
-      <c r="AG28" s="55" t="s">
-        <v>83</v>
+      <c r="AG28" s="55" t="n">
+        <v>2062.5</v>
       </c>
       <c r="AH28" s="55" t="n">
         <v>2062.34999999999991</v>
       </c>
-      <c r="AI28" s="55"/>
+      <c r="AI28" s="55" t="n">
+        <v>2062.34999999999991</v>
+      </c>
       <c r="AJ28" s="55"/>
     </row>
   </sheetData>
@@ -6848,7 +7084,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1643203916" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1643288762" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -6857,16 +7093,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1643203916" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1643203916" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1643203916" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1643203916" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1643288762" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1643288762" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1643288762" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1643288762" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1643203916" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1643288762" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -6879,8 +7115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AJ29"/>
   <sheetViews>
-    <sheetView view="normal" topLeftCell="Z4" zoomScale="90" workbookViewId="0">
-      <selection activeCell="AH29" sqref="AH29"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="Z4" zoomScale="90" workbookViewId="0">
+      <selection activeCell="AI29" sqref="AI29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.20"/>
@@ -6898,7 +7134,7 @@
     <col min="18" max="18" width="9.752475" customWidth="1" style="54"/>
     <col min="19" max="20" width="9.574257" customWidth="1" style="54"/>
     <col min="21" max="26" width="9.138614" customWidth="1" style="54"/>
-    <col min="27" max="27" width="19.138614" customWidth="1" style="54"/>
+    <col min="27" max="27" width="13.366337" customWidth="1" style="54"/>
     <col min="28" max="30" width="10.861386" customWidth="1" style="54"/>
     <col min="31" max="32" width="10.574257" customWidth="1" style="54"/>
     <col min="33" max="16384" width="9.138614" customWidth="1" style="54"/>
@@ -6942,7 +7178,7 @@
     <row r="3" spans="2:36">
       <c r="B3" s="50"/>
       <c r="C3" s="50" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D3" s="49" t="s">
         <v>2</v>
@@ -6961,7 +7197,7 @@
       <c r="L3" s="49"/>
       <c r="N3" s="51"/>
       <c r="O3" s="51" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="P3" s="49" t="s">
         <v>2</v>
@@ -6980,7 +7216,7 @@
       <c r="X3" s="49"/>
       <c r="Z3" s="50"/>
       <c r="AA3" s="50" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AB3" s="49" t="s">
         <v>2</v>
@@ -7127,7 +7363,9 @@
       <c r="J5" s="55" t="n">
         <v>1986.15000000000009</v>
       </c>
-      <c r="K5" s="55"/>
+      <c r="K5" s="55" t="n">
+        <v>1961.72000000000003</v>
+      </c>
       <c r="L5" s="55"/>
       <c r="N5" s="51" t="s">
         <v>11</v>
@@ -7156,7 +7394,9 @@
       <c r="V5" s="55" t="n">
         <v>3439</v>
       </c>
-      <c r="W5" s="55"/>
+      <c r="W5" s="55" t="n">
+        <v>3401</v>
+      </c>
       <c r="X5" s="55"/>
       <c r="Z5" s="50" t="s">
         <v>12</v>
@@ -7185,7 +7425,9 @@
       <c r="AH5" s="55" t="n">
         <v>62006.8099999999977</v>
       </c>
-      <c r="AI5" s="55"/>
+      <c r="AI5" s="55" t="n">
+        <v>62006.8099999999977</v>
+      </c>
       <c r="AJ5" s="55"/>
     </row>
     <row r="6" spans="2:36">
@@ -7231,7 +7473,9 @@
       <c r="V6" s="55" t="n">
         <v>39977.8199999999997</v>
       </c>
-      <c r="W6" s="55"/>
+      <c r="W6" s="55" t="n">
+        <v>39761.6100000000006</v>
+      </c>
       <c r="X6" s="55"/>
       <c r="Z6" s="50" t="s">
         <v>15</v>
@@ -7260,7 +7504,9 @@
       <c r="AH6" s="55" t="n">
         <v>32380.7000000000007</v>
       </c>
-      <c r="AI6" s="55"/>
+      <c r="AI6" s="55" t="n">
+        <v>31286.619999999999</v>
+      </c>
       <c r="AJ6" s="55"/>
     </row>
     <row r="7" spans="2:36">
@@ -7291,7 +7537,9 @@
       <c r="J7" s="55" t="n">
         <v>6635</v>
       </c>
-      <c r="K7" s="55"/>
+      <c r="K7" s="55" t="n">
+        <v>6348</v>
+      </c>
       <c r="L7" s="55"/>
       <c r="N7" s="51" t="s">
         <v>17</v>
@@ -7320,7 +7568,9 @@
       <c r="V7" s="55" t="n">
         <v>4797</v>
       </c>
-      <c r="W7" s="55"/>
+      <c r="W7" s="55" t="n">
+        <v>4787</v>
+      </c>
       <c r="X7" s="55"/>
       <c r="Z7" s="50" t="s">
         <v>18</v>
@@ -7349,7 +7599,9 @@
       <c r="AH7" s="55" t="n">
         <v>40887.3000000000029</v>
       </c>
-      <c r="AI7" s="55"/>
+      <c r="AI7" s="55" t="n">
+        <v>39037.6999999999971</v>
+      </c>
       <c r="AJ7" s="55"/>
     </row>
     <row r="8" spans="2:36">
@@ -7380,7 +7632,9 @@
       <c r="J8" s="55" t="n">
         <v>19769</v>
       </c>
-      <c r="K8" s="55"/>
+      <c r="K8" s="55" t="n">
+        <v>19502</v>
+      </c>
       <c r="L8" s="55"/>
       <c r="N8" s="51" t="s">
         <v>20</v>
@@ -7424,7 +7678,9 @@
       <c r="AH8" s="55" t="n">
         <v>82166.3800000000047</v>
       </c>
-      <c r="AI8" s="55"/>
+      <c r="AI8" s="55" t="n">
+        <v>75728.3500000000058</v>
+      </c>
       <c r="AJ8" s="55"/>
     </row>
     <row r="9" spans="2:36">
@@ -7455,7 +7711,9 @@
       <c r="J9" s="55" t="n">
         <v>1068</v>
       </c>
-      <c r="K9" s="55"/>
+      <c r="K9" s="55" t="n">
+        <v>1012</v>
+      </c>
       <c r="L9" s="55"/>
       <c r="N9" s="51" t="s">
         <v>23</v>
@@ -7499,7 +7757,9 @@
       <c r="AH9" s="55" t="n">
         <v>42507.9499999999971</v>
       </c>
-      <c r="AI9" s="55"/>
+      <c r="AI9" s="55" t="n">
+        <v>42319</v>
+      </c>
       <c r="AJ9" s="55"/>
     </row>
     <row r="10" spans="2:36">
@@ -7530,7 +7790,9 @@
       <c r="J10" s="55" t="n">
         <v>1174</v>
       </c>
-      <c r="K10" s="55"/>
+      <c r="K10" s="55" t="n">
+        <v>1141</v>
+      </c>
       <c r="L10" s="55"/>
       <c r="N10" s="51" t="s">
         <v>26</v>
@@ -7574,7 +7836,9 @@
       <c r="AH10" s="55" t="n">
         <v>50601.8799999999974</v>
       </c>
-      <c r="AI10" s="55"/>
+      <c r="AI10" s="55" t="n">
+        <v>48427.5599999999977</v>
+      </c>
       <c r="AJ10" s="55"/>
     </row>
     <row r="11" spans="2:36">
@@ -7605,7 +7869,9 @@
       <c r="J11" s="55" t="n">
         <v>4324.48999999999978</v>
       </c>
-      <c r="K11" s="55"/>
+      <c r="K11" s="55" t="n">
+        <v>4324.48999999999978</v>
+      </c>
       <c r="L11" s="55"/>
       <c r="N11" s="51" t="s">
         <v>30</v>
@@ -7649,7 +7915,9 @@
       <c r="AH11" s="55" t="n">
         <v>72191.5500000000029</v>
       </c>
-      <c r="AI11" s="55"/>
+      <c r="AI11" s="55" t="n">
+        <v>71556.3600000000006</v>
+      </c>
       <c r="AJ11" s="55"/>
     </row>
     <row r="12" spans="2:36">
@@ -7680,7 +7948,9 @@
       <c r="J12" s="55" t="n">
         <v>53622.8899999999994</v>
       </c>
-      <c r="K12" s="55"/>
+      <c r="K12" s="55" t="n">
+        <v>52619.9400000000023</v>
+      </c>
       <c r="L12" s="55"/>
       <c r="N12" s="51" t="s">
         <v>33</v>
@@ -7724,7 +7994,9 @@
       <c r="AH12" s="55" t="n">
         <v>39882.4300000000003</v>
       </c>
-      <c r="AI12" s="55"/>
+      <c r="AI12" s="55" t="n">
+        <v>39442.8899999999994</v>
+      </c>
       <c r="AJ12" s="55"/>
     </row>
     <row r="13" spans="2:36">
@@ -7755,7 +8027,9 @@
       <c r="J13" s="55" t="n">
         <v>13041</v>
       </c>
-      <c r="K13" s="55"/>
+      <c r="K13" s="55" t="n">
+        <v>13041</v>
+      </c>
       <c r="L13" s="55"/>
       <c r="N13" s="51" t="s">
         <v>36</v>
@@ -7784,7 +8058,9 @@
       <c r="V13" s="55" t="n">
         <v>8281</v>
       </c>
-      <c r="W13" s="55"/>
+      <c r="W13" s="55" t="n">
+        <v>8191</v>
+      </c>
       <c r="X13" s="55"/>
       <c r="Z13" s="50" t="s">
         <v>37</v>
@@ -7813,7 +8089,9 @@
       <c r="AH13" s="55" t="n">
         <v>38509.5299999999988</v>
       </c>
-      <c r="AI13" s="55"/>
+      <c r="AI13" s="55" t="s">
+        <v>83</v>
+      </c>
       <c r="AJ13" s="55"/>
     </row>
     <row r="14" spans="2:36">
@@ -7844,7 +8122,9 @@
       <c r="J14" s="55" t="n">
         <v>1884.68000000000006</v>
       </c>
-      <c r="K14" s="55"/>
+      <c r="K14" s="55" t="n">
+        <v>1470</v>
+      </c>
       <c r="L14" s="55"/>
       <c r="N14" s="51" t="s">
         <v>39</v>
@@ -7873,7 +8153,9 @@
       <c r="V14" s="55" t="n">
         <v>16197.6200000000008</v>
       </c>
-      <c r="W14" s="55"/>
+      <c r="W14" s="55" t="n">
+        <v>15968.7800000000007</v>
+      </c>
       <c r="X14" s="55"/>
       <c r="Z14" s="50" t="s">
         <v>40</v>
@@ -7902,7 +8184,9 @@
       <c r="AH14" s="55" t="n">
         <v>62172.2799999999988</v>
       </c>
-      <c r="AI14" s="55"/>
+      <c r="AI14" s="55" t="n">
+        <v>61031.5599999999977</v>
+      </c>
       <c r="AJ14" s="55"/>
     </row>
     <row r="15" spans="2:36">
@@ -7933,7 +8217,9 @@
       <c r="J15" s="55" t="n">
         <v>1884.68000000000006</v>
       </c>
-      <c r="K15" s="55"/>
+      <c r="K15" s="55" t="n">
+        <v>1856.48000000000002</v>
+      </c>
       <c r="L15" s="55"/>
       <c r="N15" s="51" t="s">
         <v>42</v>
@@ -7962,7 +8248,9 @@
       <c r="V15" s="55" t="n">
         <v>20349.9199999999983</v>
       </c>
-      <c r="W15" s="55"/>
+      <c r="W15" s="55" t="n">
+        <v>20232.0600000000013</v>
+      </c>
       <c r="X15" s="55"/>
       <c r="Z15" s="50" t="s">
         <v>43</v>
@@ -8014,7 +8302,9 @@
       <c r="J16" s="55" t="n">
         <v>4510.59000000000015</v>
       </c>
-      <c r="K16" s="55"/>
+      <c r="K16" s="55" t="n">
+        <v>4371.36999999999989</v>
+      </c>
       <c r="L16" s="55"/>
       <c r="N16" s="51" t="s">
         <v>45</v>
@@ -8043,7 +8333,9 @@
       <c r="V16" s="55" t="n">
         <v>21685.4900000000016</v>
       </c>
-      <c r="W16" s="55"/>
+      <c r="W16" s="55" t="n">
+        <v>21685.880000000001</v>
+      </c>
       <c r="X16" s="55"/>
       <c r="Z16" s="50" t="s">
         <v>46</v>
@@ -8072,7 +8364,9 @@
       <c r="AH16" s="55" t="n">
         <v>946.850000000000023</v>
       </c>
-      <c r="AI16" s="55"/>
+      <c r="AI16" s="55" t="n">
+        <v>901.17999999999995</v>
+      </c>
       <c r="AJ16" s="55"/>
     </row>
     <row r="17" spans="2:36">
@@ -8103,7 +8397,9 @@
       <c r="J17" s="55" t="n">
         <v>4972.60000000000036</v>
       </c>
-      <c r="K17" s="55"/>
+      <c r="K17" s="55" t="n">
+        <v>4793.60000000000036</v>
+      </c>
       <c r="L17" s="55"/>
       <c r="N17" s="51" t="s">
         <v>48</v>
@@ -8132,7 +8428,9 @@
       <c r="V17" s="55" t="n">
         <v>17264.5499999999993</v>
       </c>
-      <c r="W17" s="55"/>
+      <c r="W17" s="55" t="n">
+        <v>17179.7200000000012</v>
+      </c>
       <c r="X17" s="55"/>
       <c r="Z17" s="50" t="s">
         <v>49</v>
@@ -8161,7 +8459,9 @@
       <c r="AH17" s="55" t="n">
         <v>1804.08999999999992</v>
       </c>
-      <c r="AI17" s="55"/>
+      <c r="AI17" s="55" t="n">
+        <v>1754.75</v>
+      </c>
       <c r="AJ17" s="55"/>
     </row>
     <row r="18" spans="2:36">
@@ -8192,7 +8492,9 @@
       <c r="J18" s="55" t="n">
         <v>390</v>
       </c>
-      <c r="K18" s="55"/>
+      <c r="K18" s="55" t="n">
+        <v>390</v>
+      </c>
       <c r="L18" s="55"/>
       <c r="N18" s="51" t="s">
         <v>51</v>
@@ -8221,7 +8523,9 @@
       <c r="V18" s="55" t="n">
         <v>19459.4000000000015</v>
       </c>
-      <c r="W18" s="55"/>
+      <c r="W18" s="55" t="n">
+        <v>19064.7700000000004</v>
+      </c>
       <c r="X18" s="55"/>
       <c r="Z18" s="50" t="s">
         <v>52</v>
@@ -8248,7 +8552,9 @@
       <c r="AH18" s="55" t="n">
         <v>5421.56999999999971</v>
       </c>
-      <c r="AI18" s="55"/>
+      <c r="AI18" s="55" t="n">
+        <v>5311.51000000000022</v>
+      </c>
       <c r="AJ18" s="55"/>
     </row>
     <row r="19" spans="2:36">
@@ -8279,7 +8585,9 @@
       <c r="J19" s="55" t="n">
         <v>286.550000000000011</v>
       </c>
-      <c r="K19" s="55"/>
+      <c r="K19" s="55" t="n">
+        <v>286.550000000000011</v>
+      </c>
       <c r="L19" s="55"/>
       <c r="N19" s="51" t="s">
         <v>54</v>
@@ -8308,7 +8616,9 @@
       <c r="V19" s="55" t="n">
         <v>24834.4300000000003</v>
       </c>
-      <c r="W19" s="55"/>
+      <c r="W19" s="55" t="n">
+        <v>23480.7999999999993</v>
+      </c>
       <c r="X19" s="55"/>
       <c r="Z19" s="50" t="s">
         <v>56</v>
@@ -8329,12 +8639,14 @@
       <c r="AF19" s="55"/>
       <c r="AG19" s="55"/>
       <c r="AH19" s="55"/>
-      <c r="AI19" s="55"/>
+      <c r="AI19" s="55" t="n">
+        <v>6974.89000000000033</v>
+      </c>
       <c r="AJ19" s="55"/>
     </row>
     <row r="20" spans="2:36">
       <c r="B20" s="50" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C20" s="50" t="n">
         <v>57</v>
@@ -8360,10 +8672,12 @@
       <c r="J20" s="55" t="n">
         <v>365.110000000000014</v>
       </c>
-      <c r="K20" s="55"/>
+      <c r="K20" s="55" t="n">
+        <v>363.319999999999993</v>
+      </c>
       <c r="L20" s="55"/>
       <c r="N20" s="51" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O20" s="51" t="n">
         <v>75</v>
@@ -8389,10 +8703,12 @@
       <c r="V20" s="55" t="n">
         <v>17267.5800000000017</v>
       </c>
-      <c r="W20" s="55"/>
+      <c r="W20" s="55" t="n">
+        <v>16572.0400000000009</v>
+      </c>
       <c r="X20" s="55"/>
       <c r="Z20" s="50" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AA20" s="50" t="n">
         <v>131</v>
@@ -8418,12 +8734,14 @@
       <c r="AH20" s="55" t="n">
         <v>16124</v>
       </c>
-      <c r="AI20" s="55"/>
+      <c r="AI20" s="55" t="n">
+        <v>16043</v>
+      </c>
       <c r="AJ20" s="55"/>
     </row>
     <row r="21" spans="2:36">
       <c r="B21" s="50" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C21" s="50" t="n">
         <v>75</v>
@@ -8449,10 +8767,12 @@
       <c r="J21" s="55" t="n">
         <v>447.649999999999977</v>
       </c>
-      <c r="K21" s="55"/>
+      <c r="K21" s="55" t="n">
+        <v>446.019999999999982</v>
+      </c>
       <c r="L21" s="55"/>
       <c r="N21" s="51" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O21" s="51" t="n">
         <v>75</v>
@@ -8478,10 +8798,12 @@
       <c r="V21" s="55" t="n">
         <v>16977.3499999999985</v>
       </c>
-      <c r="W21" s="55"/>
+      <c r="W21" s="55" t="n">
+        <v>16977.6699999999983</v>
+      </c>
       <c r="X21" s="55"/>
       <c r="Z21" s="50" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AA21" s="50" t="n">
         <v>401</v>
@@ -8507,12 +8829,14 @@
       <c r="AH21" s="55" t="n">
         <v>35918</v>
       </c>
-      <c r="AI21" s="55"/>
+      <c r="AI21" s="55" t="n">
+        <v>35859</v>
+      </c>
       <c r="AJ21" s="55"/>
     </row>
     <row r="22" spans="2:36">
       <c r="B22" s="50" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C22" s="50" t="n">
         <v>19</v>
@@ -8538,10 +8862,12 @@
       <c r="J22" s="55" t="n">
         <v>553</v>
       </c>
-      <c r="K22" s="55"/>
+      <c r="K22" s="55" t="n">
+        <v>553</v>
+      </c>
       <c r="L22" s="55"/>
       <c r="N22" s="51" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="O22" s="51" t="n">
         <v>75</v>
@@ -8562,15 +8888,17 @@
         <v>16640.5499999999993</v>
       </c>
       <c r="U22" s="55" t="n">
-        <v>16746.6899999999987</v>
+        <v>16746.6899999999951</v>
       </c>
       <c r="V22" s="55" t="n">
-        <v>16892.0299999999988</v>
-      </c>
-      <c r="W22" s="55"/>
+        <v>16892.0299999999952</v>
+      </c>
+      <c r="W22" s="55" t="n">
+        <v>16051.9300000000003</v>
+      </c>
       <c r="X22" s="55"/>
       <c r="Z22" s="50" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AA22" s="50" t="n">
         <v>774</v>
@@ -8593,7 +8921,7 @@
     </row>
     <row r="23" spans="2:36">
       <c r="B23" s="50" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C23" s="50" t="n">
         <v>196</v>
@@ -8619,10 +8947,12 @@
       <c r="J23" s="55" t="n">
         <v>1852.1099999999999</v>
       </c>
-      <c r="K23" s="55"/>
+      <c r="K23" s="55" t="n">
+        <v>1825.29999999999995</v>
+      </c>
       <c r="L23" s="55"/>
       <c r="N23" s="51" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="O23" s="51" t="n">
         <v>78</v>
@@ -8648,10 +8978,12 @@
       <c r="V23" s="55" t="n">
         <v>9242.6200000000008</v>
       </c>
-      <c r="W23" s="55"/>
+      <c r="W23" s="55" t="n">
+        <v>8970.14999999999964</v>
+      </c>
       <c r="X23" s="55"/>
       <c r="Z23" s="50" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AA23" s="50" t="n">
         <v>52</v>
@@ -8677,12 +9009,14 @@
       <c r="AH23" s="55" t="n">
         <v>510.810000000000002</v>
       </c>
-      <c r="AI23" s="55"/>
+      <c r="AI23" s="55" t="n">
+        <v>480.069999999999993</v>
+      </c>
       <c r="AJ23" s="55"/>
     </row>
     <row r="24" spans="2:36">
       <c r="B24" s="50" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C24" s="50" t="n">
         <v>12</v>
@@ -8708,10 +9042,12 @@
       <c r="J24" s="55" t="n">
         <v>640</v>
       </c>
-      <c r="K24" s="55"/>
+      <c r="K24" s="55" t="n">
+        <v>640</v>
+      </c>
       <c r="L24" s="55"/>
       <c r="N24" s="51" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O24" s="51" t="n">
         <v>238</v>
@@ -8737,10 +9073,12 @@
       <c r="V24" s="55" t="n">
         <v>34393.5999999999985</v>
       </c>
-      <c r="W24" s="55"/>
+      <c r="W24" s="55" t="n">
+        <v>32497.7799999999988</v>
+      </c>
       <c r="X24" s="55"/>
       <c r="Z24" s="50" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AA24" s="50" t="n">
         <v>31</v>
@@ -8766,12 +9104,14 @@
       <c r="AH24" s="55" t="n">
         <v>719</v>
       </c>
-      <c r="AI24" s="55"/>
+      <c r="AI24" s="55" t="n">
+        <v>719</v>
+      </c>
       <c r="AJ24" s="55"/>
     </row>
     <row r="25" spans="2:36">
       <c r="B25" s="50" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C25" s="50" t="n">
         <v>15</v>
@@ -8797,10 +9137,12 @@
       <c r="J25" s="55" t="n">
         <v>1276</v>
       </c>
-      <c r="K25" s="55"/>
+      <c r="K25" s="55" t="n">
+        <v>1351</v>
+      </c>
       <c r="L25" s="55"/>
       <c r="N25" s="51" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O25" s="51" t="n">
         <v>1034</v>
@@ -8821,7 +9163,7 @@
       <c r="W25" s="55"/>
       <c r="X25" s="55"/>
       <c r="Z25" s="50" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AA25" s="50" t="n">
         <v>168</v>
@@ -8847,12 +9189,14 @@
       <c r="AH25" s="55" t="n">
         <v>87227.9199999999983</v>
       </c>
-      <c r="AI25" s="55"/>
+      <c r="AI25" s="55" t="n">
+        <v>87227.9199999999983</v>
+      </c>
       <c r="AJ25" s="55"/>
     </row>
     <row r="26" spans="2:36">
       <c r="B26" s="50" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C26" s="50" t="n">
         <v>18</v>
@@ -8878,10 +9222,12 @@
       <c r="J26" s="55" t="n">
         <v>802</v>
       </c>
-      <c r="K26" s="55"/>
+      <c r="K26" s="55" t="s">
+        <v>84</v>
+      </c>
       <c r="L26" s="55"/>
       <c r="N26" s="51" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="O26" s="51" t="n">
         <v>420</v>
@@ -8907,10 +9253,12 @@
       <c r="V26" s="55" t="n">
         <v>2114</v>
       </c>
-      <c r="W26" s="55"/>
+      <c r="W26" s="55" t="n">
+        <v>2088</v>
+      </c>
       <c r="X26" s="55"/>
       <c r="Z26" s="50" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AA26" s="50" t="n">
         <v>168</v>
@@ -8936,12 +9284,14 @@
       <c r="AH26" s="55" t="n">
         <v>2844.80999999999995</v>
       </c>
-      <c r="AI26" s="55"/>
+      <c r="AI26" s="55" t="n">
+        <v>2799.09999999999991</v>
+      </c>
       <c r="AJ26" s="55"/>
     </row>
     <row r="27" spans="26:36">
       <c r="Z27" s="50" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AA27" s="50" t="n">
         <v>12</v>
@@ -8967,12 +9317,14 @@
       <c r="AH27" s="55" t="n">
         <v>2852.11000000000013</v>
       </c>
-      <c r="AI27" s="55"/>
+      <c r="AI27" s="55" t="n">
+        <v>2808.82999999999993</v>
+      </c>
       <c r="AJ27" s="55"/>
     </row>
     <row r="28" spans="26:36">
       <c r="Z28" s="50" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AA28" s="50" t="n">
         <v>16</v>
@@ -8998,7 +9350,9 @@
       <c r="AH28" s="55" t="n">
         <v>2936.28999999999996</v>
       </c>
-      <c r="AI28" s="55"/>
+      <c r="AI28" s="55" t="n">
+        <v>2936.28999999999996</v>
+      </c>
       <c r="AJ28" s="55"/>
     </row>
     <row r="29" spans="34:34">
@@ -9024,7 +9378,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1643203916" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1643288762" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -9033,16 +9387,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1643203916" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1643203916" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1643203916" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1643203916" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1643288762" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1643288762" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1643288762" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1643288762" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1643203916" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1643288762" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Tabelando resultados da busca local add-drop
</commit_message>
<xml_diff>
--- a/Comparaçoes/BuscasLocais.xlsx
+++ b/Comparaçoes/BuscasLocais.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15795" windowHeight="4785" tabRatio="500" activeTab="2"/>
+    <workbookView windowWidth="16095" windowHeight="4785" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="k = n|4" sheetId="1" r:id="rId1"/>
@@ -296,11 +296,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -322,14 +322,15 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF44546A"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -343,12 +344,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -356,13 +351,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color rgb="FF44546A"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -387,6 +375,13 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF44546A"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -402,15 +397,26 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color rgb="FF44546A"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF44546A"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -423,20 +429,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -456,7 +456,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE697"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7C7C7"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBEBEB"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA8D08C"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8CAAB"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC5DFB3"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C6E7"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4AF82"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFED7D31"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD964"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CA"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4472C4"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8EA9DB"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE1EFD8"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF70AD47"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -468,49 +588,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF8EA9DB"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFD964"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF4472C4"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFE697"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFF2CA"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF70AD47"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEBEBEB"/>
+        <fgColor rgb="FFBDD7EE"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -528,109 +624,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF8CAAB"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB4C6E7"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC5DFB3"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC7C7C7"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE1EFD8"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9E1F2"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA8D08C"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBDD7EE"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFBE3D5"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF9BC2E6"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4AF82"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFED7D31"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFBE3D5"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -844,6 +844,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF5B9BD5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -859,22 +877,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color rgb="FF5B9BD5"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF5B9BD5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -890,15 +903,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF5B9BD5"/>
       </bottom>
       <diagonal/>
     </border>
@@ -927,17 +931,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF5B9BD5"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF5B9BD5"/>
       </bottom>
       <diagonal/>
     </border>
@@ -946,31 +946,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -979,115 +994,100 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1095,22 +1095,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1119,13 +1119,13 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1137,13 +1137,13 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1152,22 +1152,22 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1179,7 +1179,7 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1501,8 +1501,8 @@
   <sheetPr/>
   <dimension ref="B2:AY28"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="AI15" workbookViewId="0">
-      <selection activeCell="AO29" sqref="AO29"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="AF15" workbookViewId="0">
+      <selection activeCell="AS29" sqref="AS29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -1837,7 +1837,9 @@
       <c r="J5" s="2">
         <v>683.65</v>
       </c>
-      <c r="K5" s="2"/>
+      <c r="K5" s="2">
+        <v>723.11</v>
+      </c>
       <c r="L5" s="2">
         <v>707.34</v>
       </c>
@@ -1881,7 +1883,9 @@
       <c r="AA5" s="11">
         <v>558</v>
       </c>
-      <c r="AB5" s="2"/>
+      <c r="AB5" s="2">
+        <v>558</v>
+      </c>
       <c r="AC5" s="20">
         <v>582</v>
       </c>
@@ -1925,7 +1929,9 @@
       <c r="AR5" s="11">
         <v>25126.84</v>
       </c>
-      <c r="AS5" s="2"/>
+      <c r="AS5" s="2">
+        <v>23589.53</v>
+      </c>
       <c r="AT5" s="20">
         <v>25126.84</v>
       </c>
@@ -1991,7 +1997,9 @@
       <c r="AA6" s="11">
         <v>9818.95</v>
       </c>
-      <c r="AB6" s="2"/>
+      <c r="AB6" s="2">
+        <v>9934.05</v>
+      </c>
       <c r="AC6" s="20">
         <v>10082.97</v>
       </c>
@@ -2035,7 +2043,9 @@
       <c r="AR6" s="11">
         <v>7165.83</v>
       </c>
-      <c r="AS6" s="2"/>
+      <c r="AS6" s="2">
+        <v>7379.46</v>
+      </c>
       <c r="AT6" s="20">
         <v>7537.29</v>
       </c>
@@ -2081,7 +2091,9 @@
       <c r="J7" s="2">
         <v>1373</v>
       </c>
-      <c r="K7" s="2"/>
+      <c r="K7" s="2">
+        <v>1354</v>
+      </c>
       <c r="L7" s="2">
         <v>1373</v>
       </c>
@@ -2121,7 +2133,9 @@
       <c r="AA7" s="11">
         <v>1404</v>
       </c>
-      <c r="AB7" s="2"/>
+      <c r="AB7" s="2">
+        <v>1405</v>
+      </c>
       <c r="AC7" s="20">
         <v>1356</v>
       </c>
@@ -2161,7 +2175,9 @@
       <c r="AR7" s="11">
         <v>13755.23</v>
       </c>
-      <c r="AS7" s="2"/>
+      <c r="AS7" s="2">
+        <v>12877.05</v>
+      </c>
       <c r="AT7" s="20">
         <v>14065.44</v>
       </c>
@@ -2207,7 +2223,9 @@
       <c r="J8" s="2">
         <v>4334</v>
       </c>
-      <c r="K8" s="2"/>
+      <c r="K8" s="2">
+        <v>4440</v>
+      </c>
       <c r="L8" s="2">
         <v>4532</v>
       </c>
@@ -2271,7 +2289,9 @@
       <c r="AR8" s="11">
         <v>23341.46</v>
       </c>
-      <c r="AS8" s="2"/>
+      <c r="AS8" s="2">
+        <v>23907.89</v>
+      </c>
       <c r="AT8" s="20">
         <v>23147.12</v>
       </c>
@@ -2317,7 +2337,9 @@
       <c r="J9" s="2">
         <v>292</v>
       </c>
-      <c r="K9" s="2"/>
+      <c r="K9" s="2">
+        <v>275</v>
+      </c>
       <c r="L9" s="2">
         <v>292</v>
       </c>
@@ -2385,7 +2407,9 @@
       <c r="AR9" s="11">
         <v>12001.03</v>
       </c>
-      <c r="AS9" s="2"/>
+      <c r="AS9" s="2">
+        <v>12001.03</v>
+      </c>
       <c r="AT9" s="20">
         <v>11480.73</v>
       </c>
@@ -2431,7 +2455,9 @@
       <c r="J10" s="2">
         <v>352</v>
       </c>
-      <c r="K10" s="2"/>
+      <c r="K10" s="2">
+        <v>319</v>
+      </c>
       <c r="L10" s="2">
         <v>352</v>
       </c>
@@ -2499,7 +2525,9 @@
       <c r="AR10" s="11">
         <v>15403.25</v>
       </c>
-      <c r="AS10" s="2"/>
+      <c r="AS10" s="2">
+        <v>16537.99</v>
+      </c>
       <c r="AT10" s="20">
         <v>15403.26</v>
       </c>
@@ -2545,7 +2573,9 @@
       <c r="J11" s="2">
         <v>556.81</v>
       </c>
-      <c r="K11" s="2"/>
+      <c r="K11" s="2">
+        <v>490.84</v>
+      </c>
       <c r="L11" s="2">
         <v>556.81</v>
       </c>
@@ -2609,7 +2639,9 @@
       <c r="AR11" s="11">
         <v>23231.19</v>
       </c>
-      <c r="AS11" s="2"/>
+      <c r="AS11" s="2">
+        <v>23248.9</v>
+      </c>
       <c r="AT11" s="20">
         <v>23231.19</v>
       </c>
@@ -2655,7 +2687,9 @@
       <c r="J12" s="2">
         <v>11580.32</v>
       </c>
-      <c r="K12" s="2"/>
+      <c r="K12" s="2">
+        <v>11680.14</v>
+      </c>
       <c r="L12" s="2">
         <v>12834.58</v>
       </c>
@@ -2719,7 +2753,9 @@
       <c r="AR12" s="11">
         <v>8023.61</v>
       </c>
-      <c r="AS12" s="2"/>
+      <c r="AS12" s="2">
+        <v>7800</v>
+      </c>
       <c r="AT12" s="20">
         <v>8023.61</v>
       </c>
@@ -2761,7 +2797,9 @@
       <c r="J13" s="2">
         <v>4607</v>
       </c>
-      <c r="K13" s="2"/>
+      <c r="K13" s="2">
+        <v>4607</v>
+      </c>
       <c r="L13" s="2">
         <v>4607</v>
       </c>
@@ -2801,7 +2839,9 @@
       <c r="AA13" s="11">
         <v>3155</v>
       </c>
-      <c r="AB13" s="2"/>
+      <c r="AB13" s="2">
+        <v>2884</v>
+      </c>
       <c r="AC13" s="20">
         <v>3155</v>
       </c>
@@ -2845,7 +2885,9 @@
       <c r="AR13" s="11">
         <v>11699.66</v>
       </c>
-      <c r="AS13" s="2"/>
+      <c r="AS13" s="2">
+        <v>12256.31</v>
+      </c>
       <c r="AT13" s="20">
         <v>10546.96</v>
       </c>
@@ -2887,7 +2929,9 @@
       <c r="J14" s="2">
         <v>480</v>
       </c>
-      <c r="K14" s="2"/>
+      <c r="K14" s="2">
+        <v>520</v>
+      </c>
       <c r="L14" s="2">
         <v>570</v>
       </c>
@@ -2927,7 +2971,9 @@
       <c r="AA14" s="11">
         <v>4792.31</v>
       </c>
-      <c r="AB14" s="2"/>
+      <c r="AB14" s="2">
+        <v>4492.73</v>
+      </c>
       <c r="AC14" s="20">
         <v>4788.84</v>
       </c>
@@ -2971,7 +3017,9 @@
       <c r="AR14" s="11">
         <v>22573.29</v>
       </c>
-      <c r="AS14" s="2"/>
+      <c r="AS14" s="2">
+        <v>23304.76</v>
+      </c>
       <c r="AT14" s="20">
         <v>21586.45</v>
       </c>
@@ -3013,7 +3061,9 @@
       <c r="J15" s="2">
         <v>249.88</v>
       </c>
-      <c r="K15" s="2"/>
+      <c r="K15" s="2">
+        <v>224.88</v>
+      </c>
       <c r="L15" s="2">
         <v>249.88</v>
       </c>
@@ -3057,7 +3107,9 @@
       <c r="AA15" s="11">
         <v>7222.1</v>
       </c>
-      <c r="AB15" s="2"/>
+      <c r="AB15" s="2">
+        <v>7429.09</v>
+      </c>
       <c r="AC15" s="20">
         <v>7646.9</v>
       </c>
@@ -3133,7 +3185,9 @@
       <c r="J16" s="2">
         <v>1215.96</v>
       </c>
-      <c r="K16" s="2"/>
+      <c r="K16" s="2">
+        <v>1176.78</v>
+      </c>
       <c r="L16" s="2">
         <v>1215.96</v>
       </c>
@@ -3177,7 +3231,9 @@
       <c r="AA16" s="11">
         <v>6846.38</v>
       </c>
-      <c r="AB16" s="2"/>
+      <c r="AB16" s="2">
+        <v>6899.46</v>
+      </c>
       <c r="AC16" s="20">
         <v>6741.11</v>
       </c>
@@ -3221,7 +3277,9 @@
       <c r="AR16" s="11">
         <v>306.99</v>
       </c>
-      <c r="AS16" s="2"/>
+      <c r="AS16" s="2">
+        <v>341.87</v>
+      </c>
       <c r="AT16" s="20">
         <v>292.55</v>
       </c>
@@ -3267,7 +3325,9 @@
       <c r="J17" s="2">
         <v>1381.35</v>
       </c>
-      <c r="K17" s="2"/>
+      <c r="K17" s="2">
+        <v>1455.85</v>
+      </c>
       <c r="L17" s="2">
         <v>1245.96</v>
       </c>
@@ -3311,7 +3371,9 @@
       <c r="AA17" s="11">
         <v>4469.81</v>
       </c>
-      <c r="AB17" s="2"/>
+      <c r="AB17" s="2">
+        <v>4405.8</v>
+      </c>
       <c r="AC17" s="20">
         <v>5384.91</v>
       </c>
@@ -3355,7 +3417,9 @@
       <c r="AR17" s="11">
         <v>593.08</v>
       </c>
-      <c r="AS17" s="2"/>
+      <c r="AS17" s="2">
+        <v>594.47</v>
+      </c>
       <c r="AT17" s="20">
         <v>546.13</v>
       </c>
@@ -3401,7 +3465,9 @@
       <c r="J18" s="2">
         <v>100</v>
       </c>
-      <c r="K18" s="2"/>
+      <c r="K18" s="2">
+        <v>103</v>
+      </c>
       <c r="L18" s="2">
         <v>100</v>
       </c>
@@ -3445,7 +3511,9 @@
       <c r="AA18" s="11">
         <v>5396.33</v>
       </c>
-      <c r="AB18" s="2"/>
+      <c r="AB18" s="2">
+        <v>5281.26</v>
+      </c>
       <c r="AC18" s="20">
         <v>5396.33</v>
       </c>
@@ -3489,7 +3557,9 @@
       <c r="AR18" s="11">
         <v>1696.55</v>
       </c>
-      <c r="AS18" s="2"/>
+      <c r="AS18" s="2">
+        <v>1724.74</v>
+      </c>
       <c r="AT18" s="20">
         <v>1700.81</v>
       </c>
@@ -3531,7 +3601,9 @@
       <c r="J19" s="2">
         <v>77.04</v>
       </c>
-      <c r="K19" s="2"/>
+      <c r="K19" s="2">
+        <v>77.04</v>
+      </c>
       <c r="L19" s="2">
         <v>77.04</v>
       </c>
@@ -3575,7 +3647,9 @@
       <c r="AA19" s="11">
         <v>8120.14</v>
       </c>
-      <c r="AB19" s="2"/>
+      <c r="AB19" s="2">
+        <v>7915.92</v>
+      </c>
       <c r="AC19" s="20">
         <v>7231.98</v>
       </c>
@@ -3617,7 +3691,9 @@
       <c r="AR19" s="11">
         <v>2352.71</v>
       </c>
-      <c r="AS19" s="2"/>
+      <c r="AS19" s="2">
+        <v>2434.48</v>
+      </c>
       <c r="AT19" s="20">
         <v>2218.16</v>
       </c>
@@ -3659,7 +3735,9 @@
       <c r="J20" s="2">
         <v>99.45</v>
       </c>
-      <c r="K20" s="2"/>
+      <c r="K20" s="2">
+        <v>99.45</v>
+      </c>
       <c r="L20" s="2">
         <v>99.45</v>
       </c>
@@ -3703,7 +3781,9 @@
       <c r="AA20" s="11">
         <v>5775.96</v>
       </c>
-      <c r="AB20" s="2"/>
+      <c r="AB20" s="2">
+        <v>5811.52</v>
+      </c>
       <c r="AC20" s="20">
         <v>4293.02</v>
       </c>
@@ -3747,7 +3827,9 @@
       <c r="AR20" s="11">
         <v>5476</v>
       </c>
-      <c r="AS20" s="2"/>
+      <c r="AS20" s="2">
+        <v>5382</v>
+      </c>
       <c r="AT20" s="20">
         <v>5420</v>
       </c>
@@ -3789,7 +3871,9 @@
       <c r="J21" s="2">
         <v>132.75</v>
       </c>
-      <c r="K21" s="2"/>
+      <c r="K21" s="2">
+        <v>118.57</v>
+      </c>
       <c r="L21" s="2">
         <v>139.62</v>
       </c>
@@ -3833,7 +3917,9 @@
       <c r="AA21" s="11">
         <v>5246.28</v>
       </c>
-      <c r="AB21" s="2"/>
+      <c r="AB21" s="2">
+        <v>5220.64</v>
+      </c>
       <c r="AC21" s="20">
         <v>5246.28</v>
       </c>
@@ -3877,7 +3963,9 @@
       <c r="AR21" s="11">
         <v>12012</v>
       </c>
-      <c r="AS21" s="2"/>
+      <c r="AS21" s="2">
+        <v>11838</v>
+      </c>
       <c r="AT21" s="20">
         <v>12196</v>
       </c>
@@ -3919,7 +4007,9 @@
       <c r="J22" s="2">
         <v>147</v>
       </c>
-      <c r="K22" s="2"/>
+      <c r="K22" s="2">
+        <v>145</v>
+      </c>
       <c r="L22" s="2">
         <v>147</v>
       </c>
@@ -3963,7 +4053,9 @@
       <c r="AA22" s="11">
         <v>3842.76</v>
       </c>
-      <c r="AB22" s="2"/>
+      <c r="AB22" s="2">
+        <v>3842.76</v>
+      </c>
       <c r="AC22" s="20">
         <v>3919.58</v>
       </c>
@@ -4041,7 +4133,9 @@
       <c r="J23" s="2">
         <v>652.59</v>
       </c>
-      <c r="K23" s="2"/>
+      <c r="K23" s="2">
+        <v>658.92</v>
+      </c>
       <c r="L23" s="2">
         <v>655.8</v>
       </c>
@@ -4085,7 +4179,9 @@
       <c r="AA23" s="11">
         <v>2033.36</v>
       </c>
-      <c r="AB23" s="2"/>
+      <c r="AB23" s="2">
+        <v>2067.87</v>
+      </c>
       <c r="AC23" s="20">
         <v>2002.98</v>
       </c>
@@ -4129,7 +4225,9 @@
       <c r="AR23" s="11">
         <v>127.18</v>
       </c>
-      <c r="AS23" s="2"/>
+      <c r="AS23" s="2">
+        <v>119.95</v>
+      </c>
       <c r="AT23" s="20">
         <v>127.18</v>
       </c>
@@ -4175,7 +4273,9 @@
       <c r="J24" s="2">
         <v>154</v>
       </c>
-      <c r="K24" s="2"/>
+      <c r="K24" s="2">
+        <v>154</v>
+      </c>
       <c r="L24" s="2">
         <v>154</v>
       </c>
@@ -4219,7 +4319,9 @@
       <c r="AA24" s="11">
         <v>8969.49</v>
       </c>
-      <c r="AB24" s="2"/>
+      <c r="AB24" s="2">
+        <v>9131.48</v>
+      </c>
       <c r="AC24" s="20">
         <v>9406.35</v>
       </c>
@@ -4263,7 +4365,9 @@
       <c r="AR24" s="11">
         <v>146</v>
       </c>
-      <c r="AS24" s="2"/>
+      <c r="AS24" s="2">
+        <v>146</v>
+      </c>
       <c r="AT24" s="20">
         <v>146</v>
       </c>
@@ -4309,7 +4413,9 @@
       <c r="J25" s="25">
         <v>248</v>
       </c>
-      <c r="K25" s="25"/>
+      <c r="K25" s="25">
+        <v>233</v>
+      </c>
       <c r="L25" s="25">
         <v>248</v>
       </c>
@@ -4383,7 +4489,9 @@
       <c r="AR25" s="11">
         <v>27500</v>
       </c>
-      <c r="AS25" s="2"/>
+      <c r="AS25" s="2">
+        <v>27500</v>
+      </c>
       <c r="AT25" s="20">
         <v>27500</v>
       </c>
@@ -4425,7 +4533,9 @@
       <c r="J26" s="2">
         <v>162</v>
       </c>
-      <c r="K26" s="2"/>
+      <c r="K26" s="2">
+        <v>162</v>
+      </c>
       <c r="L26" s="2">
         <v>162</v>
       </c>
@@ -4469,7 +4579,9 @@
       <c r="AA26" s="2">
         <v>535</v>
       </c>
-      <c r="AB26" s="2"/>
+      <c r="AB26" s="2">
+        <v>565</v>
+      </c>
       <c r="AC26" s="2">
         <v>640</v>
       </c>
@@ -4509,7 +4621,9 @@
       <c r="AR26" s="11">
         <v>1038.03</v>
       </c>
-      <c r="AS26" s="2"/>
+      <c r="AS26" s="2">
+        <v>1018.34</v>
+      </c>
       <c r="AT26" s="20">
         <v>1094.89</v>
       </c>
@@ -4551,7 +4665,9 @@
       <c r="AR27" s="11">
         <v>751.06</v>
       </c>
-      <c r="AS27" s="2"/>
+      <c r="AS27" s="2">
+        <v>751.06</v>
+      </c>
       <c r="AT27" s="20">
         <v>751.06</v>
       </c>
@@ -4597,7 +4713,9 @@
       <c r="AR28" s="11">
         <v>456.58</v>
       </c>
-      <c r="AS28" s="2"/>
+      <c r="AS28" s="2">
+        <v>456.58</v>
+      </c>
       <c r="AT28" s="20">
         <v>456.58</v>
       </c>
@@ -4644,8 +4762,8 @@
   <sheetPr/>
   <dimension ref="B2:AY28"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="AF15" workbookViewId="0">
-      <selection activeCell="AO29" sqref="AO29"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="AI15" workbookViewId="0">
+      <selection activeCell="AS29" sqref="AS29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -4979,7 +5097,9 @@
       <c r="J5" s="3">
         <v>1425.65</v>
       </c>
-      <c r="K5" s="3"/>
+      <c r="K5" s="3">
+        <v>1539.34</v>
+      </c>
       <c r="L5" s="3">
         <v>1328.54</v>
       </c>
@@ -5023,7 +5143,9 @@
       <c r="AA5" s="11">
         <v>1691</v>
       </c>
-      <c r="AB5" s="2"/>
+      <c r="AB5" s="2">
+        <v>1691</v>
+      </c>
       <c r="AC5" s="20">
         <v>1691</v>
       </c>
@@ -5067,7 +5189,9 @@
       <c r="AR5" s="2">
         <v>44106.74</v>
       </c>
-      <c r="AS5" s="2"/>
+      <c r="AS5" s="2">
+        <v>43786.95</v>
+      </c>
       <c r="AT5" s="2">
         <v>44106.74</v>
       </c>
@@ -5133,7 +5257,9 @@
       <c r="AA6" s="11">
         <v>22425.03</v>
       </c>
-      <c r="AB6" s="2"/>
+      <c r="AB6" s="2">
+        <v>23160.51</v>
+      </c>
       <c r="AC6" s="20">
         <v>26964.52</v>
       </c>
@@ -5177,7 +5303,9 @@
       <c r="AR6" s="2">
         <v>15274.43</v>
       </c>
-      <c r="AS6" s="2"/>
+      <c r="AS6" s="2">
+        <v>15553.25</v>
+      </c>
       <c r="AT6" s="2">
         <v>16472.98</v>
       </c>
@@ -5223,7 +5351,9 @@
       <c r="J7" s="2">
         <v>3674</v>
       </c>
-      <c r="K7" s="2"/>
+      <c r="K7" s="2">
+        <v>3655</v>
+      </c>
       <c r="L7" s="2">
         <v>3674</v>
       </c>
@@ -5263,7 +5393,9 @@
       <c r="AA7" s="11">
         <v>3062</v>
       </c>
-      <c r="AB7" s="2"/>
+      <c r="AB7" s="2">
+        <v>3062</v>
+      </c>
       <c r="AC7" s="20">
         <v>2950</v>
       </c>
@@ -5303,7 +5435,9 @@
       <c r="AR7" s="2">
         <v>22298.23</v>
       </c>
-      <c r="AS7" s="2"/>
+      <c r="AS7" s="2">
+        <v>22208.58</v>
+      </c>
       <c r="AT7" s="2">
         <v>21887.89</v>
       </c>
@@ -5349,7 +5483,9 @@
       <c r="J8" s="2">
         <v>9700</v>
       </c>
-      <c r="K8" s="2"/>
+      <c r="K8" s="2">
+        <v>10405</v>
+      </c>
       <c r="L8" s="2">
         <v>11824</v>
       </c>
@@ -5413,7 +5549,9 @@
       <c r="AR8" s="2">
         <v>49348.67</v>
       </c>
-      <c r="AS8" s="2"/>
+      <c r="AS8" s="2">
+        <v>51047.96</v>
+      </c>
       <c r="AT8" s="2">
         <v>48383.81</v>
       </c>
@@ -5459,7 +5597,9 @@
       <c r="J9" s="2">
         <v>581</v>
       </c>
-      <c r="K9" s="2"/>
+      <c r="K9" s="2">
+        <v>581</v>
+      </c>
       <c r="L9" s="2">
         <v>581</v>
       </c>
@@ -5527,7 +5667,9 @@
       <c r="AR9" s="2">
         <v>28343.34</v>
       </c>
-      <c r="AS9" s="2"/>
+      <c r="AS9" s="2">
+        <v>28471</v>
+      </c>
       <c r="AT9" s="2">
         <v>26341.82</v>
       </c>
@@ -5573,7 +5715,9 @@
       <c r="J10" s="2">
         <v>818</v>
       </c>
-      <c r="K10" s="2"/>
+      <c r="K10" s="2">
+        <v>813</v>
+      </c>
       <c r="L10" s="2">
         <v>818</v>
       </c>
@@ -5641,7 +5785,9 @@
       <c r="AR10" s="2">
         <v>34036.73</v>
       </c>
-      <c r="AS10" s="2"/>
+      <c r="AS10" s="2">
+        <v>35491.82</v>
+      </c>
       <c r="AT10" s="2">
         <v>34036.73</v>
       </c>
@@ -5687,7 +5833,9 @@
       <c r="J11" s="2">
         <v>1813.95</v>
       </c>
-      <c r="K11" s="2"/>
+      <c r="K11" s="2">
+        <v>1836.69</v>
+      </c>
       <c r="L11" s="2">
         <v>1813.95</v>
       </c>
@@ -5751,7 +5899,9 @@
       <c r="AR11" s="2">
         <v>52534.33</v>
       </c>
-      <c r="AS11" s="2"/>
+      <c r="AS11" s="2">
+        <v>48472.31</v>
+      </c>
       <c r="AT11" s="2">
         <v>52927.27</v>
       </c>
@@ -5797,7 +5947,9 @@
       <c r="J12" s="2">
         <v>29059.75</v>
       </c>
-      <c r="K12" s="2"/>
+      <c r="K12" s="2">
+        <v>30002.94</v>
+      </c>
       <c r="L12" s="2">
         <v>27954.99</v>
       </c>
@@ -5861,7 +6013,9 @@
       <c r="AR12" s="2">
         <v>21514.76</v>
       </c>
-      <c r="AS12" s="2"/>
+      <c r="AS12" s="2">
+        <v>21708.66</v>
+      </c>
       <c r="AT12" s="2">
         <v>21495.76</v>
       </c>
@@ -5903,7 +6057,9 @@
       <c r="J13" s="2">
         <v>9455</v>
       </c>
-      <c r="K13" s="2"/>
+      <c r="K13" s="2">
+        <v>8731</v>
+      </c>
       <c r="L13" s="2">
         <v>9812</v>
       </c>
@@ -5943,7 +6099,9 @@
       <c r="AA13" s="11">
         <v>5381</v>
       </c>
-      <c r="AB13" s="2"/>
+      <c r="AB13" s="2">
+        <v>5412</v>
+      </c>
       <c r="AC13" s="20">
         <v>6289</v>
       </c>
@@ -5987,7 +6145,9 @@
       <c r="AR13" s="2">
         <v>24326.71</v>
       </c>
-      <c r="AS13" s="2"/>
+      <c r="AS13" s="2">
+        <v>25901.24</v>
+      </c>
       <c r="AT13" s="2">
         <v>24783.47</v>
       </c>
@@ -6029,7 +6189,9 @@
       <c r="J14" s="2">
         <v>980</v>
       </c>
-      <c r="K14" s="2"/>
+      <c r="K14" s="2">
+        <v>1130</v>
+      </c>
       <c r="L14" s="2">
         <v>1090</v>
       </c>
@@ -6069,7 +6231,9 @@
       <c r="AA14" s="11">
         <v>9744.28</v>
       </c>
-      <c r="AB14" s="2"/>
+      <c r="AB14" s="2">
+        <v>9795.47</v>
+      </c>
       <c r="AC14" s="20">
         <v>10444.9</v>
       </c>
@@ -6113,7 +6277,9 @@
       <c r="AR14" s="2">
         <v>42428.85</v>
       </c>
-      <c r="AS14" s="2"/>
+      <c r="AS14" s="2">
+        <v>43081.62</v>
+      </c>
       <c r="AT14" s="2">
         <v>42621.95</v>
       </c>
@@ -6155,7 +6321,9 @@
       <c r="J15" s="2">
         <v>1339.12</v>
       </c>
-      <c r="K15" s="2"/>
+      <c r="K15" s="2">
+        <v>1244.77</v>
+      </c>
       <c r="L15" s="2">
         <v>1339.12</v>
       </c>
@@ -6199,7 +6367,9 @@
       <c r="AA15" s="11">
         <v>14150.08</v>
       </c>
-      <c r="AB15" s="2"/>
+      <c r="AB15" s="2">
+        <v>15235.59</v>
+      </c>
       <c r="AC15" s="20">
         <v>13836.8</v>
       </c>
@@ -6275,7 +6445,9 @@
       <c r="J16" s="2">
         <v>2726.8</v>
       </c>
-      <c r="K16" s="2"/>
+      <c r="K16" s="2">
+        <v>2760.54</v>
+      </c>
       <c r="L16" s="2">
         <v>2565.23</v>
       </c>
@@ -6319,7 +6491,9 @@
       <c r="AA16" s="11">
         <v>15446.02</v>
       </c>
-      <c r="AB16" s="2"/>
+      <c r="AB16" s="2">
+        <v>15796.78</v>
+      </c>
       <c r="AC16" s="20">
         <v>15428.8</v>
       </c>
@@ -6363,7 +6537,9 @@
       <c r="AR16" s="2">
         <v>599.44</v>
       </c>
-      <c r="AS16" s="2"/>
+      <c r="AS16" s="2">
+        <v>661.47</v>
+      </c>
       <c r="AT16" s="2">
         <v>600.55</v>
       </c>
@@ -6409,7 +6585,9 @@
       <c r="J17" s="2">
         <v>3345.2</v>
       </c>
-      <c r="K17" s="2"/>
+      <c r="K17" s="2">
+        <v>3578.25</v>
+      </c>
       <c r="L17" s="2">
         <v>3089.54</v>
       </c>
@@ -6453,7 +6631,9 @@
       <c r="AA17" s="11">
         <v>11037.6</v>
       </c>
-      <c r="AB17" s="2"/>
+      <c r="AB17" s="2">
+        <v>11768</v>
+      </c>
       <c r="AC17" s="20">
         <v>10913.61</v>
       </c>
@@ -6497,7 +6677,9 @@
       <c r="AR17" s="2">
         <v>1253.27</v>
       </c>
-      <c r="AS17" s="2"/>
+      <c r="AS17" s="2">
+        <v>1285.41</v>
+      </c>
       <c r="AT17" s="2">
         <v>1158.97</v>
       </c>
@@ -6543,7 +6725,9 @@
       <c r="J18" s="2">
         <v>248</v>
       </c>
-      <c r="K18" s="2"/>
+      <c r="K18" s="2">
+        <v>251</v>
+      </c>
       <c r="L18" s="2">
         <v>248</v>
       </c>
@@ -6587,7 +6771,9 @@
       <c r="AA18" s="11">
         <v>12931.04</v>
       </c>
-      <c r="AB18" s="2"/>
+      <c r="AB18" s="2">
+        <v>13373.56</v>
+      </c>
       <c r="AC18" s="20">
         <v>11828.96</v>
       </c>
@@ -6631,7 +6817,9 @@
       <c r="AR18" s="2">
         <v>3569.88</v>
       </c>
-      <c r="AS18" s="2"/>
+      <c r="AS18" s="2">
+        <v>3648.34</v>
+      </c>
       <c r="AT18" s="2">
         <v>3574.95</v>
       </c>
@@ -6673,7 +6861,9 @@
       <c r="J19" s="2">
         <v>190.34</v>
       </c>
-      <c r="K19" s="2"/>
+      <c r="K19" s="2">
+        <v>190.34</v>
+      </c>
       <c r="L19" s="2">
         <v>190.34</v>
       </c>
@@ -6717,7 +6907,9 @@
       <c r="AA19" s="11">
         <v>16340.73</v>
       </c>
-      <c r="AB19" s="2"/>
+      <c r="AB19" s="2">
+        <v>17120.65</v>
+      </c>
       <c r="AC19" s="20">
         <v>15996.61</v>
       </c>
@@ -6797,7 +6989,9 @@
       <c r="J20" s="2">
         <v>240.5</v>
       </c>
-      <c r="K20" s="2"/>
+      <c r="K20" s="2">
+        <v>232.44</v>
+      </c>
       <c r="L20" s="2">
         <v>224.72</v>
       </c>
@@ -6841,7 +7035,9 @@
       <c r="AA20" s="11">
         <v>11626.21</v>
       </c>
-      <c r="AB20" s="2"/>
+      <c r="AB20" s="2">
+        <v>12035.93</v>
+      </c>
       <c r="AC20" s="20">
         <v>10824.74</v>
       </c>
@@ -6885,7 +7081,9 @@
       <c r="AR20" s="2">
         <v>10488</v>
       </c>
-      <c r="AS20" s="2"/>
+      <c r="AS20" s="2">
+        <v>10558</v>
+      </c>
       <c r="AT20" s="2">
         <v>10384</v>
       </c>
@@ -6927,7 +7125,9 @@
       <c r="J21" s="2">
         <v>266.89</v>
       </c>
-      <c r="K21" s="2"/>
+      <c r="K21" s="2">
+        <v>268.73</v>
+      </c>
       <c r="L21" s="2">
         <v>313.78</v>
       </c>
@@ -6971,7 +7171,9 @@
       <c r="AA21" s="11">
         <v>11210.26</v>
       </c>
-      <c r="AB21" s="2"/>
+      <c r="AB21" s="2">
+        <v>11092.2</v>
+      </c>
       <c r="AC21" s="20">
         <v>11197.73</v>
       </c>
@@ -7015,7 +7217,9 @@
       <c r="AR21" s="2">
         <v>23179</v>
       </c>
-      <c r="AS21" s="2"/>
+      <c r="AS21" s="2">
+        <v>23202</v>
+      </c>
       <c r="AT21" s="2">
         <v>23486</v>
       </c>
@@ -7057,7 +7261,9 @@
       <c r="J22" s="2">
         <v>391</v>
       </c>
-      <c r="K22" s="2"/>
+      <c r="K22" s="2">
+        <v>391</v>
+      </c>
       <c r="L22" s="2">
         <v>391</v>
       </c>
@@ -7101,7 +7307,9 @@
       <c r="AA22" s="11">
         <v>9883.13</v>
       </c>
-      <c r="AB22" s="2"/>
+      <c r="AB22" s="2">
+        <v>9535.85</v>
+      </c>
       <c r="AC22" s="20">
         <v>9449.58</v>
       </c>
@@ -7177,7 +7385,9 @@
       <c r="J23" s="2">
         <v>1350.3</v>
       </c>
-      <c r="K23" s="2"/>
+      <c r="K23" s="2">
+        <v>1367.16</v>
+      </c>
       <c r="L23" s="2">
         <v>1205.6</v>
       </c>
@@ -7221,7 +7431,9 @@
       <c r="AA23" s="11">
         <v>5255.49</v>
       </c>
-      <c r="AB23" s="2"/>
+      <c r="AB23" s="2">
+        <v>5350.1</v>
+      </c>
       <c r="AC23" s="20">
         <v>5838.62</v>
       </c>
@@ -7265,7 +7477,9 @@
       <c r="AR23" s="2">
         <v>248.69</v>
       </c>
-      <c r="AS23" s="2"/>
+      <c r="AS23" s="2">
+        <v>248.5</v>
+      </c>
       <c r="AT23" s="2">
         <v>282.18</v>
       </c>
@@ -7311,7 +7525,9 @@
       <c r="J24" s="2">
         <v>426</v>
       </c>
-      <c r="K24" s="2"/>
+      <c r="K24" s="2">
+        <v>426</v>
+      </c>
       <c r="L24" s="2">
         <v>359</v>
       </c>
@@ -7355,7 +7571,9 @@
       <c r="AA24" s="11">
         <v>20147.6</v>
       </c>
-      <c r="AB24" s="2"/>
+      <c r="AB24" s="2">
+        <v>20562.68</v>
+      </c>
       <c r="AC24" s="20">
         <v>21122.47</v>
       </c>
@@ -7399,7 +7617,9 @@
       <c r="AR24" s="2">
         <v>425</v>
       </c>
-      <c r="AS24" s="2"/>
+      <c r="AS24" s="2">
+        <v>448</v>
+      </c>
       <c r="AT24" s="2">
         <v>485</v>
       </c>
@@ -7445,7 +7665,9 @@
       <c r="J25" s="2">
         <v>683</v>
       </c>
-      <c r="K25" s="2"/>
+      <c r="K25" s="2">
+        <v>683</v>
+      </c>
       <c r="L25" s="2">
         <v>732</v>
       </c>
@@ -7519,7 +7741,9 @@
       <c r="AR25" s="2">
         <v>69730.67</v>
       </c>
-      <c r="AS25" s="2"/>
+      <c r="AS25" s="2">
+        <v>73607.36</v>
+      </c>
       <c r="AT25" s="2">
         <v>73643.86</v>
       </c>
@@ -7561,7 +7785,9 @@
       <c r="J26" s="2">
         <v>413</v>
       </c>
-      <c r="K26" s="2"/>
+      <c r="K26" s="2">
+        <v>413</v>
+      </c>
       <c r="L26" s="2">
         <v>413</v>
       </c>
@@ -7605,7 +7831,9 @@
       <c r="AA26" s="11">
         <v>1161</v>
       </c>
-      <c r="AB26" s="2"/>
+      <c r="AB26" s="2">
+        <v>1241</v>
+      </c>
       <c r="AC26" s="20">
         <v>1298</v>
       </c>
@@ -7645,7 +7873,9 @@
       <c r="AR26" s="2">
         <v>2092.8</v>
       </c>
-      <c r="AS26" s="2"/>
+      <c r="AS26" s="2">
+        <v>2109.73</v>
+      </c>
       <c r="AT26" s="2">
         <v>2166.1</v>
       </c>
@@ -7687,7 +7917,9 @@
       <c r="AR27" s="2">
         <v>1981.5</v>
       </c>
-      <c r="AS27" s="2"/>
+      <c r="AS27" s="2">
+        <v>1981.15</v>
+      </c>
       <c r="AT27" s="2">
         <v>1981.15</v>
       </c>
@@ -7733,7 +7965,9 @@
       <c r="AR28" s="2">
         <v>2062.5</v>
       </c>
-      <c r="AS28" s="2"/>
+      <c r="AS28" s="2">
+        <v>2086.03</v>
+      </c>
       <c r="AT28" s="2">
         <v>2062.35</v>
       </c>
@@ -7780,8 +8014,8 @@
   <sheetPr/>
   <dimension ref="B2:AY28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="AE15" workbookViewId="0">
-      <selection activeCell="AO29" sqref="AO29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="AJ15" workbookViewId="0">
+      <selection activeCell="AS29" sqref="AS29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -8120,7 +8354,9 @@
       <c r="J5" s="2">
         <v>2149.65</v>
       </c>
-      <c r="K5" s="2"/>
+      <c r="K5" s="2">
+        <v>2286.97</v>
+      </c>
       <c r="L5" s="2">
         <v>1986.15</v>
       </c>
@@ -8164,7 +8400,9 @@
       <c r="AA5" s="2">
         <v>3311</v>
       </c>
-      <c r="AB5" s="2"/>
+      <c r="AB5" s="2">
+        <v>3393</v>
+      </c>
       <c r="AC5" s="2">
         <v>3439</v>
       </c>
@@ -8208,7 +8446,9 @@
       <c r="AR5" s="2">
         <v>69677.34</v>
       </c>
-      <c r="AS5" s="2"/>
+      <c r="AS5" s="2">
+        <v>68501.9</v>
+      </c>
       <c r="AT5" s="2">
         <v>62006.81</v>
       </c>
@@ -8274,7 +8514,9 @@
       <c r="AA6" s="2">
         <v>36870.59</v>
       </c>
-      <c r="AB6" s="2"/>
+      <c r="AB6" s="2">
+        <v>37634.77</v>
+      </c>
       <c r="AC6" s="2">
         <v>39977.82</v>
       </c>
@@ -8318,7 +8560,9 @@
       <c r="AR6" s="2">
         <v>31079.42</v>
       </c>
-      <c r="AS6" s="2"/>
+      <c r="AS6" s="2">
+        <v>31797.33</v>
+      </c>
       <c r="AT6" s="2">
         <v>32380.7</v>
       </c>
@@ -8364,7 +8608,9 @@
       <c r="J7" s="2">
         <v>6635</v>
       </c>
-      <c r="K7" s="2"/>
+      <c r="K7" s="2">
+        <v>6671</v>
+      </c>
       <c r="L7" s="2">
         <v>6635</v>
       </c>
@@ -8404,7 +8650,9 @@
       <c r="AA7" s="2">
         <v>4810</v>
       </c>
-      <c r="AB7" s="2"/>
+      <c r="AB7" s="2">
+        <v>4850</v>
+      </c>
       <c r="AC7" s="2">
         <v>4797</v>
       </c>
@@ -8444,7 +8692,9 @@
       <c r="AR7" s="2">
         <v>39439.89</v>
       </c>
-      <c r="AS7" s="2"/>
+      <c r="AS7" s="2">
+        <v>41163.02</v>
+      </c>
       <c r="AT7" s="2">
         <v>40887.3</v>
       </c>
@@ -8490,7 +8740,9 @@
       <c r="J8" s="2">
         <v>17882</v>
       </c>
-      <c r="K8" s="2"/>
+      <c r="K8" s="2">
+        <v>18960</v>
+      </c>
       <c r="L8" s="2">
         <v>19769</v>
       </c>
@@ -8554,7 +8806,9 @@
       <c r="AR8" s="2">
         <v>78690.72</v>
       </c>
-      <c r="AS8" s="2"/>
+      <c r="AS8" s="2">
+        <v>81838.74</v>
+      </c>
       <c r="AT8" s="2">
         <v>82166.38</v>
       </c>
@@ -8600,7 +8854,9 @@
       <c r="J9" s="2">
         <v>1068</v>
       </c>
-      <c r="K9" s="2"/>
+      <c r="K9" s="2">
+        <v>1009</v>
+      </c>
       <c r="L9" s="2">
         <v>1068</v>
       </c>
@@ -8668,7 +8924,9 @@
       <c r="AR9" s="2">
         <v>42908.79</v>
       </c>
-      <c r="AS9" s="2"/>
+      <c r="AS9" s="2">
+        <v>43036.45</v>
+      </c>
       <c r="AT9" s="2">
         <v>42507.95</v>
       </c>
@@ -8714,7 +8972,9 @@
       <c r="J10" s="2">
         <v>1174</v>
       </c>
-      <c r="K10" s="2"/>
+      <c r="K10" s="2">
+        <v>1174</v>
+      </c>
       <c r="L10" s="2">
         <v>1174</v>
       </c>
@@ -8782,7 +9042,9 @@
       <c r="AR10" s="2">
         <v>49587.01</v>
       </c>
-      <c r="AS10" s="2"/>
+      <c r="AS10" s="2">
+        <v>52046.34</v>
+      </c>
       <c r="AT10" s="2">
         <v>50601.88</v>
       </c>
@@ -8828,7 +9090,9 @@
       <c r="J11" s="2">
         <v>4586.4</v>
       </c>
-      <c r="K11" s="2"/>
+      <c r="K11" s="2">
+        <v>4422.83</v>
+      </c>
       <c r="L11" s="2">
         <v>4324.49</v>
       </c>
@@ -8892,7 +9156,9 @@
       <c r="AR11" s="2">
         <v>69909.44</v>
       </c>
-      <c r="AS11" s="2"/>
+      <c r="AS11" s="2">
+        <v>57201.69</v>
+      </c>
       <c r="AT11" s="2">
         <v>72191.55</v>
       </c>
@@ -8938,7 +9204,9 @@
       <c r="J12" s="2">
         <v>50245.07</v>
       </c>
-      <c r="K12" s="2"/>
+      <c r="K12" s="2">
+        <v>53554.15</v>
+      </c>
       <c r="L12" s="2">
         <v>53622.89</v>
       </c>
@@ -9002,7 +9270,9 @@
       <c r="AR12" s="2">
         <v>34202.96</v>
       </c>
-      <c r="AS12" s="2"/>
+      <c r="AS12" s="2">
+        <v>34714.43</v>
+      </c>
       <c r="AT12" s="2">
         <v>39882.43</v>
       </c>
@@ -9044,7 +9314,9 @@
       <c r="J13" s="2">
         <v>12573</v>
       </c>
-      <c r="K13" s="2"/>
+      <c r="K13" s="2">
+        <v>12758</v>
+      </c>
       <c r="L13" s="2">
         <v>13041</v>
       </c>
@@ -9084,7 +9356,9 @@
       <c r="AA13" s="2">
         <v>7839</v>
       </c>
-      <c r="AB13" s="2"/>
+      <c r="AB13" s="2">
+        <v>7980</v>
+      </c>
       <c r="AC13" s="2">
         <v>8281</v>
       </c>
@@ -9128,7 +9402,9 @@
       <c r="AR13" s="2">
         <v>38200.65</v>
       </c>
-      <c r="AS13" s="2"/>
+      <c r="AS13" s="2">
+        <v>39733.74</v>
+      </c>
       <c r="AT13" s="2">
         <v>38509.53</v>
       </c>
@@ -9170,7 +9446,9 @@
       <c r="J14" s="2">
         <v>1490</v>
       </c>
-      <c r="K14" s="2"/>
+      <c r="K14" s="2">
+        <v>1740</v>
+      </c>
       <c r="L14" s="2">
         <v>1884.68</v>
       </c>
@@ -9210,7 +9488,9 @@
       <c r="AA14" s="2">
         <v>15712.96</v>
       </c>
-      <c r="AB14" s="2"/>
+      <c r="AB14" s="2">
+        <v>17063.82</v>
+      </c>
       <c r="AC14" s="2">
         <v>16197.62</v>
       </c>
@@ -9254,7 +9534,9 @@
       <c r="AR14" s="2">
         <v>67419.59</v>
       </c>
-      <c r="AS14" s="2"/>
+      <c r="AS14" s="2">
+        <v>70952.95</v>
+      </c>
       <c r="AT14" s="2">
         <v>62172.28</v>
       </c>
@@ -9296,7 +9578,9 @@
       <c r="J15" s="2">
         <v>1884.68</v>
       </c>
-      <c r="K15" s="2"/>
+      <c r="K15" s="2">
+        <v>1822.27</v>
+      </c>
       <c r="L15" s="2">
         <v>1884.68</v>
       </c>
@@ -9340,7 +9624,9 @@
       <c r="AA15" s="2">
         <v>20666.07</v>
       </c>
-      <c r="AB15" s="2"/>
+      <c r="AB15" s="2">
+        <v>21603.99</v>
+      </c>
       <c r="AC15" s="2">
         <v>20349.92</v>
       </c>
@@ -9412,7 +9698,9 @@
       <c r="J16" s="2">
         <v>4633.18</v>
       </c>
-      <c r="K16" s="2"/>
+      <c r="K16" s="2">
+        <v>4719.99</v>
+      </c>
       <c r="L16" s="2">
         <v>4510.59</v>
       </c>
@@ -9456,7 +9744,9 @@
       <c r="AA16" s="2">
         <v>23526.06</v>
       </c>
-      <c r="AB16" s="2"/>
+      <c r="AB16" s="2">
+        <v>24376.58</v>
+      </c>
       <c r="AC16" s="2">
         <v>21685.49</v>
       </c>
@@ -9500,7 +9790,9 @@
       <c r="AR16" s="2">
         <v>923.11</v>
       </c>
-      <c r="AS16" s="2"/>
+      <c r="AS16" s="2">
+        <v>1013.64</v>
+      </c>
       <c r="AT16" s="2">
         <v>946.85</v>
       </c>
@@ -9546,7 +9838,9 @@
       <c r="J17" s="2">
         <v>4874.37</v>
       </c>
-      <c r="K17" s="2"/>
+      <c r="K17" s="2">
+        <v>5380.78</v>
+      </c>
       <c r="L17" s="2">
         <v>4972.6</v>
       </c>
@@ -9590,7 +9884,9 @@
       <c r="AA17" s="2">
         <v>18160.32</v>
       </c>
-      <c r="AB17" s="2"/>
+      <c r="AB17" s="2">
+        <v>18312.38</v>
+      </c>
       <c r="AC17" s="2">
         <v>17264.55</v>
       </c>
@@ -9634,7 +9930,9 @@
       <c r="AR17" s="2">
         <v>1867.75</v>
       </c>
-      <c r="AS17" s="2"/>
+      <c r="AS17" s="2">
+        <v>1917.42</v>
+      </c>
       <c r="AT17" s="2">
         <v>1804.09</v>
       </c>
@@ -9680,7 +9978,9 @@
       <c r="J18" s="2">
         <v>390</v>
       </c>
-      <c r="K18" s="2"/>
+      <c r="K18" s="2">
+        <v>393</v>
+      </c>
       <c r="L18" s="2">
         <v>390</v>
       </c>
@@ -9724,7 +10024,9 @@
       <c r="AA18" s="2">
         <v>19505.76</v>
       </c>
-      <c r="AB18" s="2"/>
+      <c r="AB18" s="2">
+        <v>20132.75</v>
+      </c>
       <c r="AC18" s="2">
         <v>19459.4</v>
       </c>
@@ -9766,7 +10068,9 @@
         <v>5334.7</v>
       </c>
       <c r="AR18" s="2"/>
-      <c r="AS18" s="2"/>
+      <c r="AS18" s="2">
+        <v>5641.94</v>
+      </c>
       <c r="AT18" s="2">
         <v>5421.57</v>
       </c>
@@ -9808,7 +10112,9 @@
       <c r="J19" s="2">
         <v>318.28</v>
       </c>
-      <c r="K19" s="2"/>
+      <c r="K19" s="2">
+        <v>321.53</v>
+      </c>
       <c r="L19" s="2">
         <v>286.55</v>
       </c>
@@ -9852,7 +10158,9 @@
       <c r="AA19" s="2">
         <v>23838.38</v>
       </c>
-      <c r="AB19" s="2"/>
+      <c r="AB19" s="2">
+        <v>24802.49</v>
+      </c>
       <c r="AC19" s="2">
         <v>24834.43</v>
       </c>
@@ -9930,7 +10238,9 @@
       <c r="J20" s="2">
         <v>373.07</v>
       </c>
-      <c r="K20" s="2"/>
+      <c r="K20" s="2">
+        <v>366.52</v>
+      </c>
       <c r="L20" s="2">
         <v>365.11</v>
       </c>
@@ -9974,7 +10284,9 @@
       <c r="AA20" s="2">
         <v>18188.32</v>
       </c>
-      <c r="AB20" s="2"/>
+      <c r="AB20" s="2">
+        <v>18750.03</v>
+      </c>
       <c r="AC20" s="2">
         <v>17267.58</v>
       </c>
@@ -10018,7 +10330,9 @@
       <c r="AR20" s="2">
         <v>16073</v>
       </c>
-      <c r="AS20" s="2"/>
+      <c r="AS20" s="2">
+        <v>16279</v>
+      </c>
       <c r="AT20" s="2">
         <v>16124</v>
       </c>
@@ -10060,7 +10374,9 @@
       <c r="J21" s="2">
         <v>444.62</v>
       </c>
-      <c r="K21" s="2"/>
+      <c r="K21" s="2">
+        <v>450.71</v>
+      </c>
       <c r="L21" s="2">
         <v>447.65</v>
       </c>
@@ -10104,7 +10420,9 @@
       <c r="AA21" s="2">
         <v>16911.52</v>
       </c>
-      <c r="AB21" s="2"/>
+      <c r="AB21" s="2">
+        <v>16983.06</v>
+      </c>
       <c r="AC21" s="2">
         <v>16977.35</v>
       </c>
@@ -10148,7 +10466,9 @@
       <c r="AR21" s="2">
         <v>35323</v>
       </c>
-      <c r="AS21" s="2"/>
+      <c r="AS21" s="2">
+        <v>35878</v>
+      </c>
       <c r="AT21" s="2">
         <v>35918</v>
       </c>
@@ -10190,7 +10510,9 @@
       <c r="J22" s="2">
         <v>528</v>
       </c>
-      <c r="K22" s="2"/>
+      <c r="K22" s="2">
+        <v>605</v>
+      </c>
       <c r="L22" s="2">
         <v>553</v>
       </c>
@@ -10234,7 +10556,9 @@
       <c r="AA22" s="2">
         <v>16746.69</v>
       </c>
-      <c r="AB22" s="2"/>
+      <c r="AB22" s="2">
+        <v>17078.29</v>
+      </c>
       <c r="AC22" s="2">
         <v>16892.03</v>
       </c>
@@ -10306,7 +10630,9 @@
       <c r="J23" s="2">
         <v>1907.05</v>
       </c>
-      <c r="K23" s="2"/>
+      <c r="K23" s="2">
+        <v>1954.59</v>
+      </c>
       <c r="L23" s="2">
         <v>1852.11</v>
       </c>
@@ -10350,7 +10676,9 @@
       <c r="AA23" s="2">
         <v>8672.71</v>
       </c>
-      <c r="AB23" s="2"/>
+      <c r="AB23" s="2">
+        <v>8981.95</v>
+      </c>
       <c r="AC23" s="2">
         <v>9242.62</v>
       </c>
@@ -10394,7 +10722,9 @@
       <c r="AR23" s="2">
         <v>433.59</v>
       </c>
-      <c r="AS23" s="2"/>
+      <c r="AS23" s="2">
+        <v>437.11</v>
+      </c>
       <c r="AT23" s="2">
         <v>510.81</v>
       </c>
@@ -10440,7 +10770,9 @@
       <c r="J24" s="2">
         <v>813</v>
       </c>
-      <c r="K24" s="2"/>
+      <c r="K24" s="2">
+        <v>813</v>
+      </c>
       <c r="L24" s="2">
         <v>640</v>
       </c>
@@ -10484,7 +10816,9 @@
       <c r="AA24" s="2">
         <v>32866.01</v>
       </c>
-      <c r="AB24" s="2"/>
+      <c r="AB24" s="2">
+        <v>33806.02</v>
+      </c>
       <c r="AC24" s="2">
         <v>34393.6</v>
       </c>
@@ -10528,7 +10862,9 @@
       <c r="AR24" s="2">
         <v>727</v>
       </c>
-      <c r="AS24" s="2"/>
+      <c r="AS24" s="2">
+        <v>871</v>
+      </c>
       <c r="AT24" s="2">
         <v>719</v>
       </c>
@@ -10574,7 +10910,9 @@
       <c r="J25" s="2">
         <v>1276</v>
       </c>
-      <c r="K25" s="2"/>
+      <c r="K25" s="2">
+        <v>1351</v>
+      </c>
       <c r="L25" s="2">
         <v>1276</v>
       </c>
@@ -10644,7 +10982,9 @@
       <c r="AR25" s="2">
         <v>102850.23</v>
       </c>
-      <c r="AS25" s="2"/>
+      <c r="AS25" s="2">
+        <v>116558.93</v>
+      </c>
       <c r="AT25" s="2">
         <v>87227.92</v>
       </c>
@@ -10686,7 +11026,9 @@
       <c r="J26" s="2">
         <v>802</v>
       </c>
-      <c r="K26" s="2"/>
+      <c r="K26" s="2">
+        <v>802</v>
+      </c>
       <c r="L26" s="2">
         <v>802</v>
       </c>
@@ -10730,7 +11072,9 @@
       <c r="AA26" s="2">
         <v>2012</v>
       </c>
-      <c r="AB26" s="2"/>
+      <c r="AB26" s="2">
+        <v>2142</v>
+      </c>
       <c r="AC26" s="2">
         <v>2114</v>
       </c>
@@ -10770,7 +11114,9 @@
       <c r="AR26" s="2">
         <v>3123.67</v>
       </c>
-      <c r="AS26" s="2"/>
+      <c r="AS26" s="2">
+        <v>3221.8</v>
+      </c>
       <c r="AT26" s="2">
         <v>2844.81</v>
       </c>
@@ -10812,7 +11158,9 @@
       <c r="AR27" s="2">
         <v>2852.11</v>
       </c>
-      <c r="AS27" s="2"/>
+      <c r="AS27" s="2">
+        <v>3035.89</v>
+      </c>
       <c r="AT27" s="2">
         <v>2852.11</v>
       </c>
@@ -10858,7 +11206,9 @@
       <c r="AR28" s="2">
         <v>2936.29</v>
       </c>
-      <c r="AS28" s="2"/>
+      <c r="AS28" s="2">
+        <v>2812.38</v>
+      </c>
       <c r="AT28" s="2">
         <v>2936.29</v>
       </c>

</xml_diff>

<commit_message>
Tabelação dos resultados da busca local Add Drop
</commit_message>
<xml_diff>
--- a/Comparaçoes/BuscasLocais.xlsx
+++ b/Comparaçoes/BuscasLocais.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16095" windowHeight="4785" tabRatio="500" activeTab="2"/>
+    <workbookView windowWidth="13725" windowHeight="12885" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="k = n|4" sheetId="1" r:id="rId1"/>
@@ -296,11 +296,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -322,9 +322,21 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color rgb="FF44546A"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -337,54 +349,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color rgb="FF44546A"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -398,19 +370,47 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF44546A"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF44546A"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -428,15 +428,15 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -456,13 +456,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
+        <fgColor rgb="FFFFF2CA"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9E1F2"/>
+        <fgColor rgb="FFE1EFD8"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8EA9DB"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -474,19 +486,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF5B9BD5"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8CAAB"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC7C7C7"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -498,19 +528,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA8D08C"/>
+        <fgColor rgb="FF70AD47"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF8CAAB"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FF4472C4"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -522,7 +546,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB4C6E7"/>
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -540,43 +570,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFD964"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF2CA"/>
+        <fgColor rgb="FFBDD7EE"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF4472C4"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8EA9DB"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE1EFD8"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF70AD47"/>
+        <fgColor rgb="FFFBE3D5"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -588,49 +600,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFA8D08C"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBDD7EE"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDEBF7"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF5B9BD5"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFBE3D5"/>
+        <fgColor rgb="FFD9E1F2"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF9BC2E6"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB4C6E7"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD964"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7C7C7"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -844,11 +844,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF5B9BD5"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -858,6 +864,35 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF5B9BD5"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF5B9BD5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFACCCEA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF5B9BD5"/>
       </bottom>
       <diagonal/>
     </border>
@@ -893,30 +928,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFACCCEA"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -930,164 +941,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF5B9BD5"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF5B9BD5"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="21" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1095,22 +1095,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1119,13 +1119,13 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1137,13 +1137,13 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1152,22 +1152,22 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1179,7 +1179,7 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1501,8 +1501,8 @@
   <sheetPr/>
   <dimension ref="B2:AY28"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="AF15" workbookViewId="0">
-      <selection activeCell="AS29" sqref="AS29"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AW29" sqref="AW29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -1849,7 +1849,9 @@
       <c r="N5" s="2">
         <v>680.72</v>
       </c>
-      <c r="O5" s="2"/>
+      <c r="O5" s="2">
+        <v>734.19</v>
+      </c>
       <c r="P5" s="26">
         <v>606</v>
       </c>
@@ -1895,7 +1897,9 @@
       <c r="AE5" s="10">
         <v>582</v>
       </c>
-      <c r="AF5" s="10"/>
+      <c r="AF5" s="10">
+        <v>595</v>
+      </c>
       <c r="AG5" s="28">
         <v>558</v>
       </c>
@@ -1941,7 +1945,9 @@
       <c r="AV5" s="10">
         <v>25126.84</v>
       </c>
-      <c r="AW5" s="10"/>
+      <c r="AW5" s="10">
+        <v>23589.53</v>
+      </c>
       <c r="AX5" s="14">
         <v>17728</v>
       </c>
@@ -2009,7 +2015,9 @@
       <c r="AE6" s="10">
         <v>10846.48</v>
       </c>
-      <c r="AF6" s="10"/>
+      <c r="AF6" s="10">
+        <v>10207.52</v>
+      </c>
       <c r="AG6" s="28">
         <v>7704</v>
       </c>
@@ -2055,7 +2063,9 @@
       <c r="AV6" s="10">
         <v>7304.83</v>
       </c>
-      <c r="AW6" s="10"/>
+      <c r="AW6" s="10">
+        <v>7968.56</v>
+      </c>
       <c r="AX6" s="14">
         <v>6981</v>
       </c>
@@ -2103,7 +2113,9 @@
       <c r="N7" s="2">
         <v>1373</v>
       </c>
-      <c r="O7" s="2"/>
+      <c r="O7" s="2">
+        <v>1407</v>
+      </c>
       <c r="P7" s="26"/>
       <c r="Q7" s="28"/>
       <c r="S7" s="10" t="s">
@@ -2145,7 +2157,9 @@
       <c r="AE7" s="10">
         <v>1356</v>
       </c>
-      <c r="AF7" s="10"/>
+      <c r="AF7" s="10">
+        <v>1482</v>
+      </c>
       <c r="AG7" s="28"/>
       <c r="AH7" s="28"/>
       <c r="AJ7" s="10" t="s">
@@ -2187,7 +2201,9 @@
       <c r="AV7" s="10">
         <v>13755.23</v>
       </c>
-      <c r="AW7" s="10"/>
+      <c r="AW7" s="10">
+        <v>12877.06</v>
+      </c>
       <c r="AX7" s="14">
         <v>9596</v>
       </c>
@@ -2235,7 +2251,9 @@
       <c r="N8" s="2">
         <v>4442</v>
       </c>
-      <c r="O8" s="2"/>
+      <c r="O8" s="2">
+        <v>4719</v>
+      </c>
       <c r="P8" s="26"/>
       <c r="Q8" s="28"/>
       <c r="S8" s="10" t="s">
@@ -2301,7 +2319,9 @@
       <c r="AV8" s="10">
         <v>23695.72</v>
       </c>
-      <c r="AW8" s="10"/>
+      <c r="AW8" s="10">
+        <v>24085.25</v>
+      </c>
       <c r="AX8" s="14">
         <v>20928</v>
       </c>
@@ -2349,7 +2369,9 @@
       <c r="N9" s="2">
         <v>292</v>
       </c>
-      <c r="O9" s="2"/>
+      <c r="O9" s="2">
+        <v>307</v>
+      </c>
       <c r="P9" s="26">
         <v>246</v>
       </c>
@@ -2419,7 +2441,9 @@
       <c r="AV9" s="10">
         <v>11478.8</v>
       </c>
-      <c r="AW9" s="10"/>
+      <c r="AW9" s="10">
+        <v>12332.25</v>
+      </c>
       <c r="AX9" s="14">
         <v>10743</v>
       </c>
@@ -2467,7 +2491,9 @@
       <c r="N10" s="2">
         <v>352</v>
       </c>
-      <c r="O10" s="2"/>
+      <c r="O10" s="2">
+        <v>364</v>
+      </c>
       <c r="P10" s="26">
         <v>282</v>
       </c>
@@ -2537,7 +2563,9 @@
       <c r="AV10" s="10">
         <v>15933.44</v>
       </c>
-      <c r="AW10" s="10"/>
+      <c r="AW10" s="10">
+        <v>16933.76</v>
+      </c>
       <c r="AX10" s="14">
         <v>15403</v>
       </c>
@@ -2585,7 +2613,9 @@
       <c r="N11" s="2">
         <v>556.81</v>
       </c>
-      <c r="O11" s="2"/>
+      <c r="O11" s="2">
+        <v>490.84</v>
+      </c>
       <c r="P11" s="26">
         <v>489</v>
       </c>
@@ -2651,7 +2681,9 @@
       <c r="AV11" s="10">
         <v>23618.37</v>
       </c>
-      <c r="AW11" s="10"/>
+      <c r="AW11" s="10">
+        <v>25256.58</v>
+      </c>
       <c r="AX11" s="14">
         <v>18594</v>
       </c>
@@ -2699,7 +2731,9 @@
       <c r="N12" s="2">
         <v>14418.93</v>
       </c>
-      <c r="O12" s="2"/>
+      <c r="O12" s="2">
+        <v>12914.67</v>
+      </c>
       <c r="P12" s="26">
         <v>9840</v>
       </c>
@@ -2765,7 +2799,9 @@
       <c r="AV12" s="10">
         <v>8023.61</v>
       </c>
-      <c r="AW12" s="10"/>
+      <c r="AW12" s="10">
+        <v>7932.46</v>
+      </c>
       <c r="AX12" s="14"/>
       <c r="AY12" s="14"/>
     </row>
@@ -2809,7 +2845,9 @@
       <c r="N13" s="2">
         <v>4607</v>
       </c>
-      <c r="O13" s="2"/>
+      <c r="O13" s="2">
+        <v>6760</v>
+      </c>
       <c r="P13" s="26"/>
       <c r="Q13" s="28"/>
       <c r="S13" s="10" t="s">
@@ -2851,7 +2889,9 @@
       <c r="AE13" s="10">
         <v>3155</v>
       </c>
-      <c r="AF13" s="10"/>
+      <c r="AF13" s="10">
+        <v>3642</v>
+      </c>
       <c r="AG13" s="28">
         <v>2094</v>
       </c>
@@ -2897,7 +2937,9 @@
       <c r="AV13" s="10">
         <v>10546.96</v>
       </c>
-      <c r="AW13" s="10"/>
+      <c r="AW13" s="10">
+        <v>10775.33</v>
+      </c>
       <c r="AX13" s="14"/>
       <c r="AY13" s="14"/>
     </row>
@@ -2941,7 +2983,9 @@
       <c r="N14" s="2">
         <v>530</v>
       </c>
-      <c r="O14" s="2"/>
+      <c r="O14" s="2">
+        <v>560</v>
+      </c>
       <c r="P14" s="26"/>
       <c r="Q14" s="28"/>
       <c r="S14" s="10" t="s">
@@ -2983,7 +3027,9 @@
       <c r="AE14" s="10">
         <v>4788.84</v>
       </c>
-      <c r="AF14" s="10"/>
+      <c r="AF14" s="10">
+        <v>5048.49</v>
+      </c>
       <c r="AG14" s="28">
         <v>4369</v>
       </c>
@@ -3029,7 +3075,9 @@
       <c r="AV14" s="10">
         <v>23412.51</v>
       </c>
-      <c r="AW14" s="10"/>
+      <c r="AW14" s="10">
+        <v>22848.54</v>
+      </c>
       <c r="AX14" s="14"/>
       <c r="AY14" s="14"/>
     </row>
@@ -3073,7 +3121,9 @@
       <c r="N15" s="2">
         <v>249.88</v>
       </c>
-      <c r="O15" s="2"/>
+      <c r="O15" s="2">
+        <v>224.8</v>
+      </c>
       <c r="P15" s="26">
         <v>151</v>
       </c>
@@ -3119,7 +3169,9 @@
       <c r="AE15" s="10">
         <v>7222.1</v>
       </c>
-      <c r="AF15" s="10"/>
+      <c r="AF15" s="10">
+        <v>7914.8</v>
+      </c>
       <c r="AG15" s="28">
         <v>5286</v>
       </c>
@@ -3197,7 +3249,9 @@
       <c r="N16" s="2">
         <v>1203.1</v>
       </c>
-      <c r="O16" s="2"/>
+      <c r="O16" s="2">
+        <v>1238.52</v>
+      </c>
       <c r="P16" s="26">
         <v>1116</v>
       </c>
@@ -3243,7 +3297,9 @@
       <c r="AE16" s="10">
         <v>6741.11</v>
       </c>
-      <c r="AF16" s="10"/>
+      <c r="AF16" s="10">
+        <v>7023.63</v>
+      </c>
       <c r="AG16" s="28">
         <v>6138</v>
       </c>
@@ -3289,7 +3345,9 @@
       <c r="AV16" s="10">
         <v>337.72</v>
       </c>
-      <c r="AW16" s="10"/>
+      <c r="AW16" s="10">
+        <v>296.42</v>
+      </c>
       <c r="AX16" s="14">
         <v>260</v>
       </c>
@@ -3337,7 +3395,9 @@
       <c r="N17" s="2">
         <v>1245.96</v>
       </c>
-      <c r="O17" s="2"/>
+      <c r="O17" s="2">
+        <v>1352.22</v>
+      </c>
       <c r="P17" s="26">
         <v>1204</v>
       </c>
@@ -3383,7 +3443,9 @@
       <c r="AE17" s="10">
         <v>5457.17</v>
       </c>
-      <c r="AF17" s="10"/>
+      <c r="AF17" s="10">
+        <v>5427.54</v>
+      </c>
       <c r="AG17" s="28">
         <v>4014</v>
       </c>
@@ -3429,7 +3491,9 @@
       <c r="AV17" s="10">
         <v>538.97</v>
       </c>
-      <c r="AW17" s="10"/>
+      <c r="AW17" s="10">
+        <v>568.83</v>
+      </c>
       <c r="AX17" s="14">
         <v>538</v>
       </c>
@@ -3477,7 +3541,9 @@
       <c r="N18" s="2">
         <v>100</v>
       </c>
-      <c r="O18" s="2"/>
+      <c r="O18" s="2">
+        <v>112</v>
+      </c>
       <c r="P18" s="26">
         <v>99</v>
       </c>
@@ -3523,7 +3589,9 @@
       <c r="AE18" s="10">
         <v>6491</v>
       </c>
-      <c r="AF18" s="10"/>
+      <c r="AF18" s="10">
+        <v>5420.45</v>
+      </c>
       <c r="AG18" s="28">
         <v>5119</v>
       </c>
@@ -3569,7 +3637,9 @@
       <c r="AV18" s="10">
         <v>1660.87</v>
       </c>
-      <c r="AW18" s="10"/>
+      <c r="AW18" s="10">
+        <v>1730.24</v>
+      </c>
       <c r="AX18" s="14"/>
       <c r="AY18" s="14"/>
     </row>
@@ -3613,7 +3683,9 @@
       <c r="N19" s="2">
         <v>77.04</v>
       </c>
-      <c r="O19" s="2"/>
+      <c r="O19" s="2">
+        <v>95.45</v>
+      </c>
       <c r="P19" s="26">
         <v>71</v>
       </c>
@@ -3659,7 +3731,9 @@
       <c r="AE19" s="10">
         <v>7231.98</v>
       </c>
-      <c r="AF19" s="10"/>
+      <c r="AF19" s="10">
+        <v>7510.96</v>
+      </c>
       <c r="AG19" s="28">
         <v>5890</v>
       </c>
@@ -3703,7 +3777,9 @@
       <c r="AV19" s="10">
         <v>2190.99</v>
       </c>
-      <c r="AW19" s="10"/>
+      <c r="AW19" s="10">
+        <v>2296.7</v>
+      </c>
       <c r="AX19" s="14"/>
       <c r="AY19" s="14"/>
     </row>
@@ -3747,7 +3823,9 @@
       <c r="N20" s="2">
         <v>99.45</v>
       </c>
-      <c r="O20" s="2"/>
+      <c r="O20" s="2">
+        <v>113.55</v>
+      </c>
       <c r="P20" s="26">
         <v>99</v>
       </c>
@@ -3793,7 +3871,9 @@
       <c r="AE20" s="10">
         <v>4293.02</v>
       </c>
-      <c r="AF20" s="10"/>
+      <c r="AF20" s="10">
+        <v>4424.39</v>
+      </c>
       <c r="AG20" s="28">
         <v>4293</v>
       </c>
@@ -3839,7 +3919,9 @@
       <c r="AV20" s="10">
         <v>5387</v>
       </c>
-      <c r="AW20" s="10"/>
+      <c r="AW20" s="10">
+        <v>5195</v>
+      </c>
       <c r="AX20" s="14"/>
       <c r="AY20" s="14"/>
     </row>
@@ -3883,7 +3965,9 @@
       <c r="N21" s="2">
         <v>328.73</v>
       </c>
-      <c r="O21" s="2"/>
+      <c r="O21" s="2">
+        <v>146.85</v>
+      </c>
       <c r="P21" s="26">
         <v>101</v>
       </c>
@@ -3929,7 +4013,9 @@
       <c r="AE21" s="10">
         <v>5246.28</v>
       </c>
-      <c r="AF21" s="10"/>
+      <c r="AF21" s="10">
+        <v>5489.97</v>
+      </c>
       <c r="AG21" s="28">
         <v>3991</v>
       </c>
@@ -3975,7 +4061,9 @@
       <c r="AV21" s="10">
         <v>12013</v>
       </c>
-      <c r="AW21" s="10"/>
+      <c r="AW21" s="10">
+        <v>11838</v>
+      </c>
       <c r="AX21" s="14"/>
       <c r="AY21" s="14"/>
     </row>
@@ -4019,7 +4107,9 @@
       <c r="N22" s="2">
         <v>147</v>
       </c>
-      <c r="O22" s="2"/>
+      <c r="O22" s="2">
+        <v>157</v>
+      </c>
       <c r="P22" s="26">
         <v>145</v>
       </c>
@@ -4065,7 +4155,9 @@
       <c r="AE22" s="10">
         <v>3919.59</v>
       </c>
-      <c r="AF22" s="10"/>
+      <c r="AF22" s="10">
+        <v>4416.04</v>
+      </c>
       <c r="AG22" s="28">
         <v>3663</v>
       </c>
@@ -4145,7 +4237,9 @@
       <c r="N23" s="2">
         <v>656.53</v>
       </c>
-      <c r="O23" s="2"/>
+      <c r="O23" s="2">
+        <v>698.99</v>
+      </c>
       <c r="P23" s="26">
         <v>509</v>
       </c>
@@ -4191,7 +4285,9 @@
       <c r="AE23" s="10">
         <v>2002.98</v>
       </c>
-      <c r="AF23" s="10"/>
+      <c r="AF23" s="10">
+        <v>2201.61</v>
+      </c>
       <c r="AG23" s="28">
         <v>2108</v>
       </c>
@@ -4237,7 +4333,9 @@
       <c r="AV23" s="10">
         <v>127.18</v>
       </c>
-      <c r="AW23" s="10"/>
+      <c r="AW23" s="10">
+        <v>134.46</v>
+      </c>
       <c r="AX23" s="14">
         <v>110</v>
       </c>
@@ -4285,7 +4383,9 @@
       <c r="N24" s="2">
         <v>154</v>
       </c>
-      <c r="O24" s="2"/>
+      <c r="O24" s="2">
+        <v>178</v>
+      </c>
       <c r="P24" s="26">
         <v>143</v>
       </c>
@@ -4331,7 +4431,9 @@
       <c r="AE24" s="10">
         <v>9133.3</v>
       </c>
-      <c r="AF24" s="10"/>
+      <c r="AF24" s="10">
+        <v>10171.85</v>
+      </c>
       <c r="AG24" s="28">
         <v>8705</v>
       </c>
@@ -4377,7 +4479,9 @@
       <c r="AV24" s="10">
         <v>146</v>
       </c>
-      <c r="AW24" s="10"/>
+      <c r="AW24" s="10">
+        <v>181</v>
+      </c>
       <c r="AX24" s="14">
         <v>66</v>
       </c>
@@ -4425,7 +4529,9 @@
       <c r="N25" s="25">
         <v>292</v>
       </c>
-      <c r="O25" s="25"/>
+      <c r="O25" s="25">
+        <v>299</v>
+      </c>
       <c r="P25" s="26">
         <v>178</v>
       </c>
@@ -4459,7 +4565,9 @@
       <c r="AC25" s="29"/>
       <c r="AD25" s="15"/>
       <c r="AE25" s="15"/>
-      <c r="AF25" s="15"/>
+      <c r="AF25" s="15">
+        <v>12941.44</v>
+      </c>
       <c r="AG25" s="28"/>
       <c r="AH25" s="28"/>
       <c r="AJ25" s="10" t="s">
@@ -4501,7 +4609,9 @@
       <c r="AV25" s="10">
         <v>27500</v>
       </c>
-      <c r="AW25" s="10"/>
+      <c r="AW25" s="10">
+        <v>28000</v>
+      </c>
       <c r="AX25" s="14"/>
       <c r="AY25" s="14"/>
     </row>
@@ -4545,7 +4655,9 @@
       <c r="N26" s="2">
         <v>162</v>
       </c>
-      <c r="O26" s="6"/>
+      <c r="O26" s="6">
+        <v>207</v>
+      </c>
       <c r="P26" s="27">
         <v>231</v>
       </c>
@@ -4591,7 +4703,9 @@
       <c r="AE26" s="2">
         <v>649</v>
       </c>
-      <c r="AF26" s="6"/>
+      <c r="AF26" s="6">
+        <v>642</v>
+      </c>
       <c r="AG26" s="30"/>
       <c r="AH26" s="28"/>
       <c r="AJ26" s="10" t="s">
@@ -4633,7 +4747,9 @@
       <c r="AV26" s="10">
         <v>1083.13</v>
       </c>
-      <c r="AW26" s="10"/>
+      <c r="AW26" s="10">
+        <v>1099.83</v>
+      </c>
       <c r="AX26" s="14"/>
       <c r="AY26" s="14"/>
     </row>
@@ -4677,7 +4793,9 @@
       <c r="AV27" s="10">
         <v>751.06</v>
       </c>
-      <c r="AW27" s="10"/>
+      <c r="AW27" s="10">
+        <v>649.52</v>
+      </c>
       <c r="AX27" s="14">
         <v>618</v>
       </c>
@@ -4725,7 +4843,9 @@
       <c r="AV28" s="10">
         <v>456.58</v>
       </c>
-      <c r="AW28" s="10"/>
+      <c r="AW28" s="10">
+        <v>640.59</v>
+      </c>
       <c r="AX28" s="14">
         <v>447</v>
       </c>
@@ -4762,8 +4882,8 @@
   <sheetPr/>
   <dimension ref="B2:AY28"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="AI15" workbookViewId="0">
-      <selection activeCell="AS29" sqref="AS29"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AW29" sqref="AW29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -5109,7 +5229,9 @@
       <c r="N5" s="3">
         <v>1328.54</v>
       </c>
-      <c r="O5" s="3"/>
+      <c r="O5" s="3">
+        <v>1345.49</v>
+      </c>
       <c r="P5" s="18">
         <v>1234</v>
       </c>
@@ -5155,7 +5277,9 @@
       <c r="AE5" s="10">
         <v>2015</v>
       </c>
-      <c r="AF5" s="10"/>
+      <c r="AF5" s="10">
+        <v>1870</v>
+      </c>
       <c r="AG5" s="19">
         <v>1691</v>
       </c>
@@ -5201,7 +5325,9 @@
       <c r="AV5" s="2">
         <v>44106.74</v>
       </c>
-      <c r="AW5" s="2"/>
+      <c r="AW5" s="2">
+        <v>44028.59</v>
+      </c>
       <c r="AX5" s="14">
         <v>37793</v>
       </c>
@@ -5269,7 +5395,9 @@
       <c r="AE6" s="10">
         <v>27728.02</v>
       </c>
-      <c r="AF6" s="10"/>
+      <c r="AF6" s="10">
+        <v>26506.82</v>
+      </c>
       <c r="AG6" s="19">
         <v>17634</v>
       </c>
@@ -5315,7 +5443,9 @@
       <c r="AV6" s="2">
         <v>15263.07</v>
       </c>
-      <c r="AW6" s="2"/>
+      <c r="AW6" s="2">
+        <v>17101.06</v>
+      </c>
       <c r="AX6" s="14">
         <v>14839</v>
       </c>
@@ -5363,7 +5493,9 @@
       <c r="N7" s="2">
         <v>3636</v>
       </c>
-      <c r="O7" s="2"/>
+      <c r="O7" s="2">
+        <v>3717</v>
+      </c>
       <c r="P7" s="19"/>
       <c r="Q7" s="14"/>
       <c r="S7" s="10" t="s">
@@ -5405,7 +5537,9 @@
       <c r="AE7" s="10">
         <v>3345</v>
       </c>
-      <c r="AF7" s="10"/>
+      <c r="AF7" s="10">
+        <v>3210</v>
+      </c>
       <c r="AG7" s="19"/>
       <c r="AH7" s="14"/>
       <c r="AJ7" s="10" t="s">
@@ -5447,7 +5581,9 @@
       <c r="AV7" s="2">
         <v>22971.05</v>
       </c>
-      <c r="AW7" s="2"/>
+      <c r="AW7" s="2">
+        <v>22849.76</v>
+      </c>
       <c r="AX7" s="14">
         <v>21420</v>
       </c>
@@ -5495,7 +5631,9 @@
       <c r="N8" s="2">
         <v>11707</v>
       </c>
-      <c r="O8" s="2"/>
+      <c r="O8" s="2">
+        <v>11665</v>
+      </c>
       <c r="P8" s="19"/>
       <c r="Q8" s="14"/>
       <c r="S8" s="10" t="s">
@@ -5561,7 +5699,9 @@
       <c r="AV8" s="2">
         <v>46500.98</v>
       </c>
-      <c r="AW8" s="2"/>
+      <c r="AW8" s="2">
+        <v>52717.31</v>
+      </c>
       <c r="AX8" s="14">
         <v>47911</v>
       </c>
@@ -5609,7 +5749,9 @@
       <c r="N9" s="2">
         <v>581</v>
       </c>
-      <c r="O9" s="2"/>
+      <c r="O9" s="2">
+        <v>631</v>
+      </c>
       <c r="P9" s="19">
         <v>581</v>
       </c>
@@ -5679,7 +5821,9 @@
       <c r="AV9" s="2">
         <v>26329.54</v>
       </c>
-      <c r="AW9" s="2"/>
+      <c r="AW9" s="2">
+        <v>26309.61</v>
+      </c>
       <c r="AX9" s="14">
         <v>26296</v>
       </c>
@@ -5727,7 +5871,9 @@
       <c r="N10" s="2">
         <v>838</v>
       </c>
-      <c r="O10" s="2"/>
+      <c r="O10" s="2">
+        <v>907</v>
+      </c>
       <c r="P10" s="19">
         <v>672</v>
       </c>
@@ -5797,7 +5943,9 @@
       <c r="AV10" s="2">
         <v>34036.73</v>
       </c>
-      <c r="AW10" s="2"/>
+      <c r="AW10" s="2">
+        <v>35951.88</v>
+      </c>
       <c r="AX10" s="14">
         <v>30712</v>
       </c>
@@ -5845,7 +5993,9 @@
       <c r="N11" s="2">
         <v>1813.95</v>
       </c>
-      <c r="O11" s="2"/>
+      <c r="O11" s="2">
+        <v>1915.64</v>
+      </c>
       <c r="P11" s="19">
         <v>1766</v>
       </c>
@@ -5911,7 +6061,9 @@
       <c r="AV11" s="2">
         <v>51993.05</v>
       </c>
-      <c r="AW11" s="2"/>
+      <c r="AW11" s="2">
+        <v>52932.54</v>
+      </c>
       <c r="AX11" s="14">
         <v>33349</v>
       </c>
@@ -5959,7 +6111,9 @@
       <c r="N12" s="2">
         <v>28438.57</v>
       </c>
-      <c r="O12" s="2"/>
+      <c r="O12" s="2">
+        <v>30231.8</v>
+      </c>
       <c r="P12" s="19">
         <v>24862</v>
       </c>
@@ -6025,7 +6179,9 @@
       <c r="AV12" s="2">
         <v>21297.39</v>
       </c>
-      <c r="AW12" s="2"/>
+      <c r="AW12" s="2">
+        <v>25149.11</v>
+      </c>
       <c r="AX12" s="14"/>
       <c r="AY12" s="14"/>
     </row>
@@ -6069,7 +6225,9 @@
       <c r="N13" s="2">
         <v>9455</v>
       </c>
-      <c r="O13" s="2"/>
+      <c r="O13" s="2">
+        <v>9495</v>
+      </c>
       <c r="P13" s="19"/>
       <c r="Q13" s="14"/>
       <c r="S13" s="10" t="s">
@@ -6111,7 +6269,9 @@
       <c r="AE13" s="10">
         <v>6289</v>
       </c>
-      <c r="AF13" s="10"/>
+      <c r="AF13" s="10">
+        <v>6255</v>
+      </c>
       <c r="AG13" s="19">
         <v>4238</v>
       </c>
@@ -6157,7 +6317,9 @@
       <c r="AV13" s="2">
         <v>23600.58</v>
       </c>
-      <c r="AW13" s="2"/>
+      <c r="AW13" s="2">
+        <v>25084.9</v>
+      </c>
       <c r="AX13" s="14"/>
       <c r="AY13" s="14"/>
     </row>
@@ -6201,7 +6363,9 @@
       <c r="N14" s="2">
         <v>1000</v>
       </c>
-      <c r="O14" s="2"/>
+      <c r="O14" s="2">
+        <v>1150</v>
+      </c>
       <c r="P14" s="19"/>
       <c r="Q14" s="14"/>
       <c r="S14" s="10" t="s">
@@ -6243,7 +6407,9 @@
       <c r="AE14" s="10">
         <v>10081.68</v>
       </c>
-      <c r="AF14" s="10"/>
+      <c r="AF14" s="10">
+        <v>10818.87</v>
+      </c>
       <c r="AG14" s="19">
         <v>9073</v>
       </c>
@@ -6289,7 +6455,9 @@
       <c r="AV14" s="2">
         <v>43478.16</v>
       </c>
-      <c r="AW14" s="2"/>
+      <c r="AW14" s="2">
+        <v>42619.94</v>
+      </c>
       <c r="AX14" s="14"/>
       <c r="AY14" s="14"/>
     </row>
@@ -6333,7 +6501,9 @@
       <c r="N15" s="2">
         <v>1339.12</v>
       </c>
-      <c r="O15" s="2"/>
+      <c r="O15" s="2">
+        <v>1592.99</v>
+      </c>
       <c r="P15" s="19">
         <v>842</v>
       </c>
@@ -6379,7 +6549,9 @@
       <c r="AE15" s="10">
         <v>13896.17</v>
       </c>
-      <c r="AF15" s="10"/>
+      <c r="AF15" s="10">
+        <v>14754.37</v>
+      </c>
       <c r="AG15" s="19">
         <v>11412</v>
       </c>
@@ -6457,7 +6629,9 @@
       <c r="N16" s="2">
         <v>2565.23</v>
       </c>
-      <c r="O16" s="2"/>
+      <c r="O16" s="2">
+        <v>2670.92</v>
+      </c>
       <c r="P16" s="19">
         <v>2492</v>
       </c>
@@ -6503,7 +6677,9 @@
       <c r="AE16" s="10">
         <v>15482.82</v>
       </c>
-      <c r="AF16" s="10"/>
+      <c r="AF16" s="10">
+        <v>15807.67</v>
+      </c>
       <c r="AG16" s="19">
         <v>13315</v>
       </c>
@@ -6549,7 +6725,9 @@
       <c r="AV16" s="2">
         <v>599.63</v>
       </c>
-      <c r="AW16" s="2"/>
+      <c r="AW16" s="2">
+        <v>624.02</v>
+      </c>
       <c r="AX16" s="14">
         <v>554</v>
       </c>
@@ -6597,7 +6775,9 @@
       <c r="N17" s="2">
         <v>3151.81</v>
       </c>
-      <c r="O17" s="2"/>
+      <c r="O17" s="2">
+        <v>3208.01</v>
+      </c>
       <c r="P17" s="19">
         <v>2772</v>
       </c>
@@ -6643,7 +6823,9 @@
       <c r="AE17" s="10">
         <v>10913.61</v>
       </c>
-      <c r="AF17" s="10"/>
+      <c r="AF17" s="10">
+        <v>10639.58</v>
+      </c>
       <c r="AG17" s="19">
         <v>9071</v>
       </c>
@@ -6689,7 +6871,9 @@
       <c r="AV17" s="2">
         <v>1143.23</v>
       </c>
-      <c r="AW17" s="2"/>
+      <c r="AW17" s="2">
+        <v>1176.12</v>
+      </c>
       <c r="AX17" s="14">
         <v>1106</v>
       </c>
@@ -6737,7 +6921,9 @@
       <c r="N18" s="2">
         <v>247</v>
       </c>
-      <c r="O18" s="2"/>
+      <c r="O18" s="2">
+        <v>267</v>
+      </c>
       <c r="P18" s="19">
         <v>227</v>
       </c>
@@ -6783,7 +6969,9 @@
       <c r="AE18" s="10">
         <v>11746.46</v>
       </c>
-      <c r="AF18" s="10"/>
+      <c r="AF18" s="10">
+        <v>12164.05</v>
+      </c>
       <c r="AG18" s="19">
         <v>11501</v>
       </c>
@@ -6829,7 +7017,9 @@
       <c r="AV18" s="2">
         <v>3503.28</v>
       </c>
-      <c r="AW18" s="2"/>
+      <c r="AW18" s="2">
+        <v>3613.57</v>
+      </c>
       <c r="AX18" s="14"/>
       <c r="AY18" s="14"/>
     </row>
@@ -6873,7 +7063,9 @@
       <c r="N19" s="2">
         <v>190.24</v>
       </c>
-      <c r="O19" s="2"/>
+      <c r="O19" s="2">
+        <v>195.66</v>
+      </c>
       <c r="P19" s="19">
         <v>179</v>
       </c>
@@ -6919,7 +7111,9 @@
       <c r="AE19" s="10">
         <v>15789.91</v>
       </c>
-      <c r="AF19" s="10"/>
+      <c r="AF19" s="10">
+        <v>16161.46</v>
+      </c>
       <c r="AG19" s="19">
         <v>12787</v>
       </c>
@@ -6957,7 +7151,9 @@
       <c r="AV19" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="AW19" s="2"/>
+      <c r="AW19" s="2">
+        <v>4811.61</v>
+      </c>
       <c r="AX19" s="14"/>
       <c r="AY19" s="14"/>
     </row>
@@ -7001,7 +7197,9 @@
       <c r="N20" s="2">
         <v>224.72</v>
       </c>
-      <c r="O20" s="2"/>
+      <c r="O20" s="2">
+        <v>231.97</v>
+      </c>
       <c r="P20" s="19">
         <v>217</v>
       </c>
@@ -7047,7 +7245,9 @@
       <c r="AE20" s="10">
         <v>11241.49</v>
       </c>
-      <c r="AF20" s="10"/>
+      <c r="AF20" s="10">
+        <v>11534.65</v>
+      </c>
       <c r="AG20" s="19">
         <v>9428</v>
       </c>
@@ -7093,7 +7293,9 @@
       <c r="AV20" s="2">
         <v>10435</v>
       </c>
-      <c r="AW20" s="2"/>
+      <c r="AW20" s="2">
+        <v>10403</v>
+      </c>
       <c r="AX20" s="14"/>
       <c r="AY20" s="14"/>
     </row>
@@ -7137,7 +7339,9 @@
       <c r="N21" s="2">
         <v>332.22</v>
       </c>
-      <c r="O21" s="2"/>
+      <c r="O21" s="2">
+        <v>306.67</v>
+      </c>
       <c r="P21" s="19">
         <v>249</v>
       </c>
@@ -7183,7 +7387,9 @@
       <c r="AE21" s="10">
         <v>11210.26</v>
       </c>
-      <c r="AF21" s="10"/>
+      <c r="AF21" s="10">
+        <v>11251.45</v>
+      </c>
       <c r="AG21" s="19">
         <v>8808</v>
       </c>
@@ -7229,7 +7435,9 @@
       <c r="AV21" s="2">
         <v>23155</v>
       </c>
-      <c r="AW21" s="2"/>
+      <c r="AW21" s="2">
+        <v>23454</v>
+      </c>
       <c r="AX21" s="14"/>
       <c r="AY21" s="14"/>
     </row>
@@ -7273,7 +7481,9 @@
       <c r="N22" s="2">
         <v>391</v>
       </c>
-      <c r="O22" s="2"/>
+      <c r="O22" s="2">
+        <v>365</v>
+      </c>
       <c r="P22" s="19">
         <v>308</v>
       </c>
@@ -7319,7 +7529,9 @@
       <c r="AE22" s="10">
         <v>9385</v>
       </c>
-      <c r="AF22" s="10"/>
+      <c r="AF22" s="10">
+        <v>10145.38</v>
+      </c>
       <c r="AG22" s="19">
         <v>9370</v>
       </c>
@@ -7397,7 +7609,9 @@
       <c r="N23" s="2">
         <v>1200.69</v>
       </c>
-      <c r="O23" s="2"/>
+      <c r="O23" s="2">
+        <v>1231.94</v>
+      </c>
       <c r="P23" s="19">
         <v>1049</v>
       </c>
@@ -7443,7 +7657,9 @@
       <c r="AE23" s="10">
         <v>5645.72</v>
       </c>
-      <c r="AF23" s="10"/>
+      <c r="AF23" s="10">
+        <v>6482.68</v>
+      </c>
       <c r="AG23" s="19">
         <v>5532</v>
       </c>
@@ -7489,7 +7705,9 @@
       <c r="AV23" s="2">
         <v>280.47</v>
       </c>
-      <c r="AW23" s="2"/>
+      <c r="AW23" s="2">
+        <v>314.66</v>
+      </c>
       <c r="AX23" s="14">
         <v>250</v>
       </c>
@@ -7537,7 +7755,9 @@
       <c r="N24" s="2">
         <v>359</v>
       </c>
-      <c r="O24" s="2"/>
+      <c r="O24" s="2">
+        <v>396</v>
+      </c>
       <c r="P24" s="19">
         <v>359</v>
       </c>
@@ -7583,7 +7803,9 @@
       <c r="AE24" s="10">
         <v>20320.61</v>
       </c>
-      <c r="AF24" s="10"/>
+      <c r="AF24" s="10">
+        <v>21491.2</v>
+      </c>
       <c r="AG24" s="19">
         <v>17655</v>
       </c>
@@ -7629,7 +7851,9 @@
       <c r="AV24" s="2">
         <v>455</v>
       </c>
-      <c r="AW24" s="2"/>
+      <c r="AW24" s="2">
+        <v>517</v>
+      </c>
       <c r="AX24" s="14">
         <v>132</v>
       </c>
@@ -7677,7 +7901,9 @@
       <c r="N25" s="2">
         <v>1103</v>
       </c>
-      <c r="O25" s="2"/>
+      <c r="O25" s="2">
+        <v>903</v>
+      </c>
       <c r="P25" s="19">
         <v>683</v>
       </c>
@@ -7753,7 +7979,9 @@
       <c r="AV25" s="2">
         <v>70588.91</v>
       </c>
-      <c r="AW25" s="2"/>
+      <c r="AW25" s="2">
+        <v>74487.77</v>
+      </c>
       <c r="AX25" s="14"/>
       <c r="AY25" s="14"/>
     </row>
@@ -7797,7 +8025,9 @@
       <c r="N26" s="2">
         <v>438</v>
       </c>
-      <c r="O26" s="2"/>
+      <c r="O26" s="2">
+        <v>539</v>
+      </c>
       <c r="P26" s="19">
         <v>396</v>
       </c>
@@ -7843,7 +8073,9 @@
       <c r="AE26" s="10">
         <v>1277</v>
       </c>
-      <c r="AF26" s="10"/>
+      <c r="AF26" s="10">
+        <v>1285</v>
+      </c>
       <c r="AG26" s="19"/>
       <c r="AH26" s="14"/>
       <c r="AJ26" s="10" t="s">
@@ -7885,7 +8117,9 @@
       <c r="AV26" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="AW26" s="2"/>
+      <c r="AW26" s="2">
+        <v>2182.47</v>
+      </c>
       <c r="AX26" s="14"/>
       <c r="AY26" s="14"/>
     </row>
@@ -7929,7 +8163,9 @@
       <c r="AV27" s="2">
         <v>1981.71</v>
       </c>
-      <c r="AW27" s="2"/>
+      <c r="AW27" s="2">
+        <v>2315.62</v>
+      </c>
       <c r="AX27" s="14">
         <v>1329</v>
       </c>
@@ -7977,7 +8213,9 @@
       <c r="AV28" s="2">
         <v>2062.92</v>
       </c>
-      <c r="AW28" s="2"/>
+      <c r="AW28" s="2">
+        <v>2442.5</v>
+      </c>
       <c r="AX28" s="14">
         <v>1473</v>
       </c>
@@ -8014,8 +8252,8 @@
   <sheetPr/>
   <dimension ref="B2:AY28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="AJ15" workbookViewId="0">
-      <selection activeCell="AS29" sqref="AS29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AW29" sqref="AW29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -8366,7 +8604,9 @@
       <c r="N5" s="2">
         <v>1981.96</v>
       </c>
-      <c r="O5" s="2"/>
+      <c r="O5" s="2">
+        <v>1998.77</v>
+      </c>
       <c r="P5" s="8">
         <v>1894</v>
       </c>
@@ -8412,7 +8652,9 @@
       <c r="AE5" s="2">
         <v>3460</v>
       </c>
-      <c r="AF5" s="2"/>
+      <c r="AF5" s="2">
+        <v>3641</v>
+      </c>
       <c r="AG5" s="14">
         <v>3135</v>
       </c>
@@ -8458,7 +8700,9 @@
       <c r="AV5" s="2">
         <v>62006.81</v>
       </c>
-      <c r="AW5" s="2"/>
+      <c r="AW5" s="2">
+        <v>61648.17</v>
+      </c>
       <c r="AX5" s="14">
         <v>62262</v>
       </c>
@@ -8526,7 +8770,9 @@
       <c r="AE6" s="2">
         <v>40577.79</v>
       </c>
-      <c r="AF6" s="2"/>
+      <c r="AF6" s="2">
+        <v>40479.53</v>
+      </c>
       <c r="AG6" s="14">
         <v>29257</v>
       </c>
@@ -8572,7 +8818,9 @@
       <c r="AV6" s="2">
         <v>34216.34</v>
       </c>
-      <c r="AW6" s="2"/>
+      <c r="AW6" s="2">
+        <v>33658.06</v>
+      </c>
       <c r="AX6" s="14">
         <v>29684</v>
       </c>
@@ -8620,7 +8868,9 @@
       <c r="N7" s="2">
         <v>6453</v>
       </c>
-      <c r="O7" s="2"/>
+      <c r="O7" s="2">
+        <v>6899</v>
+      </c>
       <c r="P7" s="8"/>
       <c r="Q7" s="12"/>
       <c r="S7" s="10" t="s">
@@ -8662,7 +8912,9 @@
       <c r="AE7" s="2">
         <v>4978</v>
       </c>
-      <c r="AF7" s="2"/>
+      <c r="AF7" s="2">
+        <v>4932</v>
+      </c>
       <c r="AG7" s="14"/>
       <c r="AH7" s="14"/>
       <c r="AJ7" s="10" t="s">
@@ -8704,7 +8956,9 @@
       <c r="AV7" s="2">
         <v>37713.82</v>
       </c>
-      <c r="AW7" s="2"/>
+      <c r="AW7" s="2">
+        <v>41505.54</v>
+      </c>
       <c r="AX7" s="14">
         <v>36977</v>
       </c>
@@ -8752,7 +9006,9 @@
       <c r="N8" s="2">
         <v>19559</v>
       </c>
-      <c r="O8" s="2"/>
+      <c r="O8" s="2">
+        <v>19735</v>
+      </c>
       <c r="P8" s="8"/>
       <c r="Q8" s="12"/>
       <c r="S8" s="10" t="s">
@@ -8818,7 +9074,9 @@
       <c r="AV8" s="2">
         <v>77635.73</v>
       </c>
-      <c r="AW8" s="2"/>
+      <c r="AW8" s="2">
+        <v>80171.9</v>
+      </c>
       <c r="AX8" s="14">
         <v>67879</v>
       </c>
@@ -8866,7 +9124,9 @@
       <c r="N9" s="2">
         <v>1023</v>
       </c>
-      <c r="O9" s="2"/>
+      <c r="O9" s="2">
+        <v>1064</v>
+      </c>
       <c r="P9" s="8">
         <v>929</v>
       </c>
@@ -8936,7 +9196,9 @@
       <c r="AV9" s="2">
         <v>42495.67</v>
       </c>
-      <c r="AW9" s="2"/>
+      <c r="AW9" s="2">
+        <v>42952.99</v>
+      </c>
       <c r="AX9" s="14">
         <v>40274</v>
       </c>
@@ -8984,7 +9246,9 @@
       <c r="N10" s="2">
         <v>1194</v>
       </c>
-      <c r="O10" s="2"/>
+      <c r="O10" s="2">
+        <v>1277</v>
+      </c>
       <c r="P10" s="8">
         <v>1090</v>
       </c>
@@ -9054,7 +9318,9 @@
       <c r="AV10" s="2">
         <v>49587.01</v>
       </c>
-      <c r="AW10" s="2"/>
+      <c r="AW10" s="2">
+        <v>52601.62</v>
+      </c>
       <c r="AX10" s="14">
         <v>46434</v>
       </c>
@@ -9102,7 +9368,9 @@
       <c r="N11" s="2">
         <v>4501.89</v>
       </c>
-      <c r="O11" s="2"/>
+      <c r="O11" s="2">
+        <v>4898.62</v>
+      </c>
       <c r="P11" s="8">
         <v>3853</v>
       </c>
@@ -9168,7 +9436,9 @@
       <c r="AV11" s="2">
         <v>70462.56</v>
       </c>
-      <c r="AW11" s="2"/>
+      <c r="AW11" s="2">
+        <v>70984.94</v>
+      </c>
       <c r="AX11" s="14">
         <v>49022</v>
       </c>
@@ -9216,7 +9486,9 @@
       <c r="N12" s="2">
         <v>52051.58</v>
       </c>
-      <c r="O12" s="2"/>
+      <c r="O12" s="2">
+        <v>55267.25</v>
+      </c>
       <c r="P12" s="8">
         <v>51542</v>
       </c>
@@ -9282,7 +9554,9 @@
       <c r="AV12" s="2">
         <v>36542.39</v>
       </c>
-      <c r="AW12" s="2"/>
+      <c r="AW12" s="2">
+        <v>39827.34</v>
+      </c>
       <c r="AX12" s="14"/>
       <c r="AY12" s="14"/>
     </row>
@@ -9326,7 +9600,9 @@
       <c r="N13" s="2">
         <v>12573</v>
       </c>
-      <c r="O13" s="2"/>
+      <c r="O13" s="2">
+        <v>13230</v>
+      </c>
       <c r="P13" s="8"/>
       <c r="Q13" s="12"/>
       <c r="S13" s="10" t="s">
@@ -9368,7 +9644,9 @@
       <c r="AE13" s="2">
         <v>8281</v>
       </c>
-      <c r="AF13" s="2"/>
+      <c r="AF13" s="2">
+        <v>8642</v>
+      </c>
       <c r="AG13" s="14">
         <v>6937</v>
       </c>
@@ -9414,7 +9692,9 @@
       <c r="AV13" s="2">
         <v>36957.58</v>
       </c>
-      <c r="AW13" s="2"/>
+      <c r="AW13" s="2">
+        <v>39177.22</v>
+      </c>
       <c r="AX13" s="14"/>
       <c r="AY13" s="14"/>
     </row>
@@ -9458,7 +9738,9 @@
       <c r="N14" s="2">
         <v>1470</v>
       </c>
-      <c r="O14" s="2"/>
+      <c r="O14" s="2">
+        <v>1590</v>
+      </c>
       <c r="P14" s="8"/>
       <c r="Q14" s="12"/>
       <c r="S14" s="10" t="s">
@@ -9500,7 +9782,9 @@
       <c r="AE14" s="2">
         <v>15544.88</v>
       </c>
-      <c r="AF14" s="2"/>
+      <c r="AF14" s="2">
+        <v>16539.95</v>
+      </c>
       <c r="AG14" s="14">
         <v>13982</v>
       </c>
@@ -9546,7 +9830,9 @@
       <c r="AV14" s="2">
         <v>62569.65</v>
       </c>
-      <c r="AW14" s="2"/>
+      <c r="AW14" s="2">
+        <v>65237.16</v>
+      </c>
       <c r="AX14" s="14"/>
       <c r="AY14" s="14"/>
     </row>
@@ -9590,7 +9876,9 @@
       <c r="N15" s="2">
         <v>1884.68</v>
       </c>
-      <c r="O15" s="2"/>
+      <c r="O15" s="2">
+        <v>2047</v>
+      </c>
       <c r="P15" s="8">
         <v>1349</v>
       </c>
@@ -9636,7 +9924,9 @@
       <c r="AE15" s="2">
         <v>20412.16</v>
       </c>
-      <c r="AF15" s="2"/>
+      <c r="AF15" s="2">
+        <v>20992.62</v>
+      </c>
       <c r="AG15" s="14">
         <v>17787</v>
       </c>
@@ -9710,7 +10000,9 @@
       <c r="N16" s="2">
         <v>4328.01</v>
       </c>
-      <c r="O16" s="2"/>
+      <c r="O16" s="2">
+        <v>4626.48</v>
+      </c>
       <c r="P16" s="8">
         <v>4062</v>
       </c>
@@ -9756,7 +10048,9 @@
       <c r="AE16" s="2">
         <v>22427.35</v>
       </c>
-      <c r="AF16" s="2"/>
+      <c r="AF16" s="2">
+        <v>22422.54</v>
+      </c>
       <c r="AG16" s="14">
         <v>20705</v>
       </c>
@@ -9802,7 +10096,9 @@
       <c r="AV16" s="2">
         <v>924.39</v>
       </c>
-      <c r="AW16" s="2"/>
+      <c r="AW16" s="2">
+        <v>999.2</v>
+      </c>
       <c r="AX16" s="14">
         <v>868</v>
       </c>
@@ -9850,7 +10146,9 @@
       <c r="N17" s="2">
         <v>4933.01</v>
       </c>
-      <c r="O17" s="2"/>
+      <c r="O17" s="2">
+        <v>5063.63</v>
+      </c>
       <c r="P17" s="8">
         <v>4480</v>
       </c>
@@ -9896,7 +10194,9 @@
       <c r="AE17" s="2">
         <v>17030.73</v>
       </c>
-      <c r="AF17" s="2"/>
+      <c r="AF17" s="2">
+        <v>17619.81</v>
+      </c>
       <c r="AG17" s="14">
         <v>14648</v>
       </c>
@@ -9942,7 +10242,9 @@
       <c r="AV17" s="2">
         <v>1765.59</v>
       </c>
-      <c r="AW17" s="2"/>
+      <c r="AW17" s="2">
+        <v>1851.19</v>
+      </c>
       <c r="AX17" s="14">
         <v>1669</v>
       </c>
@@ -9990,7 +10292,9 @@
       <c r="N18" s="2">
         <v>390</v>
       </c>
-      <c r="O18" s="2"/>
+      <c r="O18" s="2">
+        <v>433</v>
+      </c>
       <c r="P18" s="8">
         <v>404</v>
       </c>
@@ -10036,7 +10340,9 @@
       <c r="AE18" s="2">
         <v>19376.91</v>
       </c>
-      <c r="AF18" s="2"/>
+      <c r="AF18" s="2">
+        <v>19113.56</v>
+      </c>
       <c r="AG18" s="14">
         <v>17090</v>
       </c>
@@ -10080,7 +10386,9 @@
       <c r="AV18" s="2">
         <v>5215.22</v>
       </c>
-      <c r="AW18" s="2"/>
+      <c r="AW18" s="2">
+        <v>5524.91</v>
+      </c>
       <c r="AX18" s="14"/>
       <c r="AY18" s="14"/>
     </row>
@@ -10124,7 +10432,9 @@
       <c r="N19" s="2">
         <v>294.57</v>
       </c>
-      <c r="O19" s="2"/>
+      <c r="O19" s="2">
+        <v>286.79</v>
+      </c>
       <c r="P19" s="8">
         <v>278</v>
       </c>
@@ -10170,7 +10480,9 @@
       <c r="AE19" s="2">
         <v>24342.48</v>
       </c>
-      <c r="AF19" s="2"/>
+      <c r="AF19" s="2">
+        <v>24895.61</v>
+      </c>
       <c r="AG19" s="14">
         <v>20553</v>
       </c>
@@ -10250,7 +10562,9 @@
       <c r="N20" s="2">
         <v>368.09</v>
       </c>
-      <c r="O20" s="2"/>
+      <c r="O20" s="2">
+        <v>368.06</v>
+      </c>
       <c r="P20" s="8">
         <v>345</v>
       </c>
@@ -10296,7 +10610,9 @@
       <c r="AE20" s="2">
         <v>17331.99</v>
       </c>
-      <c r="AF20" s="2"/>
+      <c r="AF20" s="2">
+        <v>17691.31</v>
+      </c>
       <c r="AG20" s="14">
         <v>14295</v>
       </c>
@@ -10342,7 +10658,9 @@
       <c r="AV20" s="2">
         <v>15960</v>
       </c>
-      <c r="AW20" s="2"/>
+      <c r="AW20" s="2">
+        <v>16166</v>
+      </c>
       <c r="AX20" s="14"/>
       <c r="AY20" s="14"/>
     </row>
@@ -10386,7 +10704,9 @@
       <c r="N21" s="2">
         <v>445.78</v>
       </c>
-      <c r="O21" s="2"/>
+      <c r="O21" s="2">
+        <v>456.79</v>
+      </c>
       <c r="P21" s="8">
         <v>398</v>
       </c>
@@ -10432,7 +10752,9 @@
       <c r="AE21" s="2">
         <v>16911.52</v>
       </c>
-      <c r="AF21" s="2"/>
+      <c r="AF21" s="2">
+        <v>16983.06</v>
+      </c>
       <c r="AG21" s="14">
         <v>13884</v>
       </c>
@@ -10478,7 +10800,9 @@
       <c r="AV21" s="2">
         <v>35455</v>
       </c>
-      <c r="AW21" s="2"/>
+      <c r="AW21" s="2">
+        <v>35729</v>
+      </c>
       <c r="AX21" s="14"/>
       <c r="AY21" s="14"/>
     </row>
@@ -10522,7 +10846,9 @@
       <c r="N22" s="2">
         <v>553</v>
       </c>
-      <c r="O22" s="2"/>
+      <c r="O22" s="2">
+        <v>655</v>
+      </c>
       <c r="P22" s="8">
         <v>492</v>
       </c>
@@ -10568,7 +10894,9 @@
       <c r="AE22" s="2">
         <v>16827.45</v>
       </c>
-      <c r="AF22" s="2"/>
+      <c r="AF22" s="2">
+        <v>17708.66</v>
+      </c>
       <c r="AG22" s="14">
         <v>15347</v>
       </c>
@@ -10642,7 +10970,9 @@
       <c r="N23" s="2">
         <v>1844.94</v>
       </c>
-      <c r="O23" s="2"/>
+      <c r="O23" s="2">
+        <v>1874.52</v>
+      </c>
       <c r="P23" s="8">
         <v>1671</v>
       </c>
@@ -10688,7 +11018,9 @@
       <c r="AE23" s="2">
         <v>8969.56</v>
       </c>
-      <c r="AF23" s="2"/>
+      <c r="AF23" s="2">
+        <v>9966.7</v>
+      </c>
       <c r="AG23" s="14">
         <v>8412</v>
       </c>
@@ -10734,7 +11066,9 @@
       <c r="AV23" s="2">
         <v>511.54</v>
       </c>
-      <c r="AW23" s="2"/>
+      <c r="AW23" s="2">
+        <v>528.49</v>
+      </c>
       <c r="AX23" s="14">
         <v>437</v>
       </c>
@@ -10782,7 +11116,9 @@
       <c r="N24" s="2">
         <v>640</v>
       </c>
-      <c r="O24" s="2"/>
+      <c r="O24" s="2">
+        <v>851</v>
+      </c>
       <c r="P24" s="8">
         <v>640</v>
       </c>
@@ -10828,7 +11164,9 @@
       <c r="AE24" s="2">
         <v>32515.89</v>
       </c>
-      <c r="AF24" s="2"/>
+      <c r="AF24" s="2">
+        <v>34843.11</v>
+      </c>
       <c r="AG24" s="14">
         <v>27963</v>
       </c>
@@ -10874,7 +11212,9 @@
       <c r="AV24" s="2">
         <v>730</v>
       </c>
-      <c r="AW24" s="2"/>
+      <c r="AW24" s="2">
+        <v>795</v>
+      </c>
       <c r="AX24" s="14">
         <v>281</v>
       </c>
@@ -10922,7 +11262,9 @@
       <c r="N25" s="2">
         <v>1276</v>
       </c>
-      <c r="O25" s="2"/>
+      <c r="O25" s="2">
+        <v>1577</v>
+      </c>
       <c r="P25" s="8">
         <v>1276</v>
       </c>
@@ -10994,7 +11336,9 @@
       <c r="AV25" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="AW25" s="2"/>
+      <c r="AW25" s="2">
+        <v>87845.96</v>
+      </c>
       <c r="AX25" s="14"/>
       <c r="AY25" s="14"/>
     </row>
@@ -11038,7 +11382,9 @@
       <c r="N26" s="2">
         <v>799</v>
       </c>
-      <c r="O26" s="2"/>
+      <c r="O26" s="2">
+        <v>924</v>
+      </c>
       <c r="P26" s="8">
         <v>763</v>
       </c>
@@ -11084,7 +11430,9 @@
       <c r="AE26" s="2">
         <v>2091</v>
       </c>
-      <c r="AF26" s="2"/>
+      <c r="AF26" s="2">
+        <v>2100</v>
+      </c>
       <c r="AG26" s="14"/>
       <c r="AH26" s="14"/>
       <c r="AJ26" s="10" t="s">
@@ -11126,7 +11474,9 @@
       <c r="AV26" s="2">
         <v>2827.67</v>
       </c>
-      <c r="AW26" s="2"/>
+      <c r="AW26" s="2">
+        <v>2894.55</v>
+      </c>
       <c r="AX26" s="14"/>
       <c r="AY26" s="14"/>
     </row>
@@ -11170,7 +11520,9 @@
       <c r="AV27" s="2">
         <v>2852.11</v>
       </c>
-      <c r="AW27" s="2"/>
+      <c r="AW27" s="2">
+        <v>3506.26</v>
+      </c>
       <c r="AX27" s="14">
         <v>2704</v>
       </c>
@@ -11218,7 +11570,9 @@
       <c r="AV28" s="2">
         <v>2825.56</v>
       </c>
-      <c r="AW28" s="2"/>
+      <c r="AW28" s="2">
+        <v>3461.13</v>
+      </c>
       <c r="AX28" s="14">
         <v>2618</v>
       </c>

</xml_diff>

<commit_message>
Tabelação dos resultados da hibrida2 com as buscas locais
</commit_message>
<xml_diff>
--- a/Comparaçoes/BuscasLocais.xlsx
+++ b/Comparaçoes/BuscasLocais.xlsx
@@ -11629,7 +11629,7 @@
   <dimension ref="B2:U71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I60" workbookViewId="0">
-      <selection activeCell="R72" sqref="R72"/>
+      <selection activeCell="S72" sqref="S72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15.75"/>
@@ -11741,7 +11741,9 @@
       <c r="D4" s="6">
         <v>857.38</v>
       </c>
-      <c r="E4" s="6"/>
+      <c r="E4" s="6">
+        <v>857.38</v>
+      </c>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="I4" s="9" t="s">
@@ -11753,7 +11755,9 @@
       <c r="K4" s="6">
         <v>1642.39</v>
       </c>
-      <c r="L4" s="6"/>
+      <c r="L4" s="6">
+        <v>1569.58</v>
+      </c>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="P4" s="9" t="s">
@@ -11765,7 +11769,9 @@
       <c r="R4" s="6">
         <v>2223.48</v>
       </c>
-      <c r="S4" s="6"/>
+      <c r="S4" s="6">
+        <v>2143.09</v>
+      </c>
       <c r="T4" s="6"/>
       <c r="U4" s="6"/>
     </row>
@@ -11811,7 +11817,9 @@
       <c r="D6" s="6">
         <v>1193</v>
       </c>
-      <c r="E6" s="6"/>
+      <c r="E6" s="6">
+        <v>1193</v>
+      </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="I6" s="9" t="s">
@@ -11823,7 +11831,9 @@
       <c r="K6" s="6">
         <v>4127</v>
       </c>
-      <c r="L6" s="6"/>
+      <c r="L6" s="6">
+        <v>3950</v>
+      </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
       <c r="P6" s="9" t="s">
@@ -11835,7 +11845,9 @@
       <c r="R6" s="6">
         <v>6346</v>
       </c>
-      <c r="S6" s="6"/>
+      <c r="S6" s="6">
+        <v>6152</v>
+      </c>
       <c r="T6" s="6"/>
       <c r="U6" s="6"/>
     </row>
@@ -11849,7 +11861,9 @@
       <c r="D7" s="6">
         <v>6774</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="6">
+        <v>6212</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="I7" s="9" t="s">
@@ -11861,7 +11875,9 @@
       <c r="K7" s="6">
         <v>17916</v>
       </c>
-      <c r="L7" s="6"/>
+      <c r="L7" s="6">
+        <v>16695</v>
+      </c>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
       <c r="P7" s="9" t="s">
@@ -11873,7 +11889,9 @@
       <c r="R7" s="6">
         <v>24187</v>
       </c>
-      <c r="S7" s="6"/>
+      <c r="S7" s="6">
+        <v>22975</v>
+      </c>
       <c r="T7" s="6"/>
       <c r="U7" s="6"/>
     </row>
@@ -11887,7 +11905,9 @@
       <c r="D8" s="6">
         <v>285</v>
       </c>
-      <c r="E8" s="6"/>
+      <c r="E8" s="6">
+        <v>285</v>
+      </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="I8" s="9" t="s">
@@ -11899,7 +11919,9 @@
       <c r="K8" s="6">
         <v>747</v>
       </c>
-      <c r="L8" s="6"/>
+      <c r="L8" s="6">
+        <v>747</v>
+      </c>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="P8" s="9" t="s">
@@ -11911,7 +11933,9 @@
       <c r="R8" s="6">
         <v>1082</v>
       </c>
-      <c r="S8" s="6"/>
+      <c r="S8" s="6">
+        <v>1048</v>
+      </c>
       <c r="T8" s="6"/>
       <c r="U8" s="6"/>
     </row>
@@ -11925,7 +11949,9 @@
       <c r="D9" s="6">
         <v>378</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="6">
+        <v>378</v>
+      </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="I9" s="9" t="s">
@@ -11937,7 +11963,9 @@
       <c r="K9" s="6">
         <v>898</v>
       </c>
-      <c r="L9" s="6"/>
+      <c r="L9" s="6">
+        <v>898</v>
+      </c>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="P9" s="9" t="s">
@@ -11949,7 +11977,9 @@
       <c r="R9" s="6">
         <v>1251</v>
       </c>
-      <c r="S9" s="6"/>
+      <c r="S9" s="6">
+        <v>1239</v>
+      </c>
       <c r="T9" s="6"/>
       <c r="U9" s="6"/>
     </row>
@@ -11963,7 +11993,9 @@
       <c r="D10" s="6">
         <v>559.76</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="6">
+        <v>559.76</v>
+      </c>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="I10" s="9" t="s">
@@ -11975,7 +12007,9 @@
       <c r="K10" s="6">
         <v>2277.18</v>
       </c>
-      <c r="L10" s="6"/>
+      <c r="L10" s="6">
+        <v>2175.72</v>
+      </c>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
       <c r="P10" s="9" t="s">
@@ -11987,7 +12021,9 @@
       <c r="R10" s="6">
         <v>4238.23</v>
       </c>
-      <c r="S10" s="6"/>
+      <c r="S10" s="6">
+        <v>4190.79</v>
+      </c>
       <c r="T10" s="6"/>
       <c r="U10" s="6"/>
     </row>
@@ -12001,7 +12037,9 @@
       <c r="D11" s="6">
         <v>14467.58</v>
       </c>
-      <c r="E11" s="6"/>
+      <c r="E11" s="6">
+        <v>13839.92</v>
+      </c>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="I11" s="9" t="s">
@@ -12013,7 +12051,9 @@
       <c r="K11" s="6">
         <v>30624.72</v>
       </c>
-      <c r="L11" s="6"/>
+      <c r="L11" s="6">
+        <v>29458.33</v>
+      </c>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="P11" s="9" t="s">
@@ -12025,7 +12065,9 @@
       <c r="R11" s="6">
         <v>57110.28</v>
       </c>
-      <c r="S11" s="6"/>
+      <c r="S11" s="6">
+        <v>53394.19</v>
+      </c>
       <c r="T11" s="6"/>
       <c r="U11" s="6"/>
     </row>
@@ -12039,7 +12081,9 @@
       <c r="D12" s="6">
         <v>4530</v>
       </c>
-      <c r="E12" s="6"/>
+      <c r="E12" s="6">
+        <v>4530</v>
+      </c>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="I12" s="9" t="s">
@@ -12051,7 +12095,9 @@
       <c r="K12" s="6">
         <v>9537</v>
       </c>
-      <c r="L12" s="6"/>
+      <c r="L12" s="6">
+        <v>9537</v>
+      </c>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="P12" s="9" t="s">
@@ -12063,7 +12109,9 @@
       <c r="R12" s="6">
         <v>12888</v>
       </c>
-      <c r="S12" s="6"/>
+      <c r="S12" s="6">
+        <v>12888</v>
+      </c>
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
     </row>
@@ -12077,7 +12125,9 @@
       <c r="D13" s="6">
         <v>560</v>
       </c>
-      <c r="E13" s="6"/>
+      <c r="E13" s="6">
+        <v>540</v>
+      </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="I13" s="9" t="s">
@@ -12089,7 +12139,9 @@
       <c r="K13" s="6">
         <v>1360</v>
       </c>
-      <c r="L13" s="6"/>
+      <c r="L13" s="6">
+        <v>1230</v>
+      </c>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
       <c r="P13" s="9" t="s">
@@ -12101,7 +12153,9 @@
       <c r="R13" s="6">
         <v>1950</v>
       </c>
-      <c r="S13" s="6"/>
+      <c r="S13" s="6">
+        <v>1730</v>
+      </c>
       <c r="T13" s="6"/>
       <c r="U13" s="6"/>
     </row>
@@ -12115,7 +12169,9 @@
       <c r="D14" s="6">
         <v>308.18</v>
       </c>
-      <c r="E14" s="6"/>
+      <c r="E14" s="6">
+        <v>308.18</v>
+      </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="I14" s="9" t="s">
@@ -12127,7 +12183,9 @@
       <c r="K14" s="6">
         <v>967.87</v>
       </c>
-      <c r="L14" s="6"/>
+      <c r="L14" s="6">
+        <v>967.86</v>
+      </c>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
       <c r="P14" s="9" t="s">
@@ -12139,7 +12197,9 @@
       <c r="R14" s="6">
         <v>1528.5</v>
       </c>
-      <c r="S14" s="6"/>
+      <c r="S14" s="6">
+        <v>1528.5</v>
+      </c>
       <c r="T14" s="6"/>
       <c r="U14" s="6"/>
     </row>
@@ -12153,7 +12213,9 @@
       <c r="D15" s="6">
         <v>1344.27</v>
       </c>
-      <c r="E15" s="6"/>
+      <c r="E15" s="6">
+        <v>1340.93</v>
+      </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="I15" s="9" t="s">
@@ -12165,7 +12227,9 @@
       <c r="K15" s="6">
         <v>3085.96</v>
       </c>
-      <c r="L15" s="6"/>
+      <c r="L15" s="6">
+        <v>2878.11</v>
+      </c>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
       <c r="P15" s="9" t="s">
@@ -12177,7 +12241,9 @@
       <c r="R15" s="6">
         <v>4975.69</v>
       </c>
-      <c r="S15" s="6"/>
+      <c r="S15" s="6">
+        <v>4649.43</v>
+      </c>
       <c r="T15" s="6"/>
       <c r="U15" s="6"/>
     </row>
@@ -12191,7 +12257,9 @@
       <c r="D16" s="6">
         <v>1657.12</v>
       </c>
-      <c r="E16" s="6"/>
+      <c r="E16" s="6">
+        <v>1576.27</v>
+      </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="I16" s="9" t="s">
@@ -12203,7 +12271,9 @@
       <c r="K16" s="6">
         <v>3670.88</v>
       </c>
-      <c r="L16" s="6"/>
+      <c r="L16" s="6">
+        <v>3552.23</v>
+      </c>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
       <c r="P16" s="9" t="s">
@@ -12215,7 +12285,9 @@
       <c r="R16" s="6">
         <v>5377.04</v>
       </c>
-      <c r="S16" s="6"/>
+      <c r="S16" s="6">
+        <v>5208.78</v>
+      </c>
       <c r="T16" s="6"/>
       <c r="U16" s="6"/>
     </row>
@@ -12229,7 +12301,9 @@
       <c r="D17" s="6">
         <v>125</v>
       </c>
-      <c r="E17" s="6"/>
+      <c r="E17" s="6">
+        <v>125</v>
+      </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="I17" s="9" t="s">
@@ -12241,7 +12315,9 @@
       <c r="K17" s="6">
         <v>296</v>
       </c>
-      <c r="L17" s="6"/>
+      <c r="L17" s="6">
+        <v>289</v>
+      </c>
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
       <c r="P17" s="9" t="s">
@@ -12253,7 +12329,9 @@
       <c r="R17" s="6">
         <v>444</v>
       </c>
-      <c r="S17" s="6"/>
+      <c r="S17" s="6">
+        <v>431</v>
+      </c>
       <c r="T17" s="6"/>
       <c r="U17" s="6"/>
     </row>
@@ -12267,7 +12345,9 @@
       <c r="D18" s="6">
         <v>80.96</v>
       </c>
-      <c r="E18" s="6"/>
+      <c r="E18" s="6">
+        <v>81.49</v>
+      </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="I18" s="9" t="s">
@@ -12279,7 +12359,9 @@
       <c r="K18" s="6">
         <v>187.81</v>
       </c>
-      <c r="L18" s="6"/>
+      <c r="L18" s="6">
+        <v>187.81</v>
+      </c>
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
       <c r="P18" s="9" t="s">
@@ -12291,7 +12373,9 @@
       <c r="R18" s="6">
         <v>332.12</v>
       </c>
-      <c r="S18" s="6"/>
+      <c r="S18" s="6">
+        <v>317.48</v>
+      </c>
       <c r="T18" s="6"/>
       <c r="U18" s="6"/>
     </row>
@@ -12305,7 +12389,9 @@
       <c r="D19" s="6">
         <v>114.81</v>
       </c>
-      <c r="E19" s="6"/>
+      <c r="E19" s="6">
+        <v>114.38</v>
+      </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="I19" s="9" t="s">
@@ -12317,7 +12403,9 @@
       <c r="K19" s="6">
         <v>245.31</v>
       </c>
-      <c r="L19" s="6"/>
+      <c r="L19" s="6">
+        <v>245.31</v>
+      </c>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
       <c r="P19" s="9" t="s">
@@ -12329,7 +12417,9 @@
       <c r="R19" s="6">
         <v>379.13</v>
       </c>
-      <c r="S19" s="6"/>
+      <c r="S19" s="6">
+        <v>367.562</v>
+      </c>
       <c r="T19" s="6"/>
       <c r="U19" s="6"/>
     </row>
@@ -12343,7 +12433,9 @@
       <c r="D20" s="6">
         <v>142.412</v>
       </c>
-      <c r="E20" s="6"/>
+      <c r="E20" s="6">
+        <v>139.65</v>
+      </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
       <c r="I20" s="9" t="s">
@@ -12355,7 +12447,9 @@
       <c r="K20" s="6">
         <v>319.66</v>
       </c>
-      <c r="L20" s="6"/>
+      <c r="L20" s="6">
+        <v>317.71</v>
+      </c>
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
       <c r="P20" s="9" t="s">
@@ -12367,7 +12461,9 @@
       <c r="R20" s="6">
         <v>446.94</v>
       </c>
-      <c r="S20" s="6"/>
+      <c r="S20" s="6">
+        <v>444.34</v>
+      </c>
       <c r="T20" s="6"/>
       <c r="U20" s="6"/>
     </row>
@@ -12381,7 +12477,9 @@
       <c r="D21" s="6">
         <v>148</v>
       </c>
-      <c r="E21" s="6"/>
+      <c r="E21" s="6">
+        <v>145</v>
+      </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
       <c r="I21" s="9" t="s">
@@ -12393,7 +12491,9 @@
       <c r="K21" s="6">
         <v>361</v>
       </c>
-      <c r="L21" s="6"/>
+      <c r="L21" s="6">
+        <v>361</v>
+      </c>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
       <c r="P21" s="9" t="s">
@@ -12405,7 +12505,9 @@
       <c r="R21" s="6">
         <v>501</v>
       </c>
-      <c r="S21" s="6"/>
+      <c r="S21" s="6">
+        <v>507</v>
+      </c>
       <c r="T21" s="6"/>
       <c r="U21" s="6"/>
     </row>
@@ -12419,7 +12521,9 @@
       <c r="D22" s="6">
         <v>603.37</v>
       </c>
-      <c r="E22" s="6"/>
+      <c r="E22" s="6">
+        <v>593.31</v>
+      </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="I22" s="9" t="s">
@@ -12431,7 +12535,9 @@
       <c r="K22" s="6">
         <v>1297.83</v>
       </c>
-      <c r="L22" s="6"/>
+      <c r="L22" s="6">
+        <v>1245.01</v>
+      </c>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
       <c r="P22" s="9" t="s">
@@ -12443,7 +12549,9 @@
       <c r="R22" s="6">
         <v>1937.62</v>
       </c>
-      <c r="S22" s="6"/>
+      <c r="S22" s="6">
+        <v>1842.51</v>
+      </c>
       <c r="T22" s="6"/>
       <c r="U22" s="6"/>
     </row>
@@ -12457,7 +12565,9 @@
       <c r="D23" s="6">
         <v>154</v>
       </c>
-      <c r="E23" s="6"/>
+      <c r="E23" s="6">
+        <v>154</v>
+      </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="I23" s="9" t="s">
@@ -12469,7 +12579,9 @@
       <c r="K23" s="6">
         <v>426</v>
       </c>
-      <c r="L23" s="6"/>
+      <c r="L23" s="6">
+        <v>426</v>
+      </c>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
       <c r="P23" s="9" t="s">
@@ -12481,7 +12593,9 @@
       <c r="R23" s="6">
         <v>718</v>
       </c>
-      <c r="S23" s="6"/>
+      <c r="S23" s="6">
+        <v>718</v>
+      </c>
       <c r="T23" s="6"/>
       <c r="U23" s="6"/>
     </row>
@@ -12495,7 +12609,9 @@
       <c r="D24" s="6">
         <v>195</v>
       </c>
-      <c r="E24" s="6"/>
+      <c r="E24" s="6">
+        <v>195</v>
+      </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="I24" s="9" t="s">
@@ -12507,7 +12623,9 @@
       <c r="K24" s="6">
         <v>736</v>
       </c>
-      <c r="L24" s="6"/>
+      <c r="L24" s="6">
+        <v>736</v>
+      </c>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
       <c r="P24" s="9" t="s">
@@ -12519,7 +12637,9 @@
       <c r="R24" s="6">
         <v>1219</v>
       </c>
-      <c r="S24" s="6"/>
+      <c r="S24" s="6">
+        <v>1294</v>
+      </c>
       <c r="T24" s="6"/>
       <c r="U24" s="6"/>
     </row>
@@ -12533,7 +12653,9 @@
       <c r="D25" s="6">
         <v>162</v>
       </c>
-      <c r="E25" s="6"/>
+      <c r="E25" s="6">
+        <v>162</v>
+      </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="I25" s="9" t="s">
@@ -12545,7 +12667,9 @@
       <c r="K25" s="6">
         <v>469</v>
       </c>
-      <c r="L25" s="6"/>
+      <c r="L25" s="6">
+        <v>469</v>
+      </c>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
       <c r="P25" s="9" t="s">
@@ -12557,7 +12681,9 @@
       <c r="R25" s="6">
         <v>832</v>
       </c>
-      <c r="S25" s="6"/>
+      <c r="S25" s="6">
+        <v>826</v>
+      </c>
       <c r="T25" s="6"/>
       <c r="U25" s="6"/>
     </row>
@@ -12569,9 +12695,11 @@
         <v>12</v>
       </c>
       <c r="D26" s="6">
-        <v>5890</v>
-      </c>
-      <c r="E26" s="6"/>
+        <v>590</v>
+      </c>
+      <c r="E26" s="6">
+        <v>590</v>
+      </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="I26" s="9" t="s">
@@ -12583,7 +12711,9 @@
       <c r="K26" s="6">
         <v>1693</v>
       </c>
-      <c r="L26" s="6"/>
+      <c r="L26" s="6">
+        <v>1693</v>
+      </c>
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
       <c r="P26" s="2" t="s">
@@ -12595,7 +12725,9 @@
       <c r="R26" s="6">
         <v>3200</v>
       </c>
-      <c r="S26" s="6"/>
+      <c r="S26" s="6">
+        <v>3200</v>
+      </c>
       <c r="T26" s="6"/>
       <c r="U26" s="6"/>
     </row>
@@ -12609,7 +12741,9 @@
       <c r="D27" s="6">
         <v>9467.2</v>
       </c>
-      <c r="E27" s="6"/>
+      <c r="E27" s="6">
+        <v>9467.2</v>
+      </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="I27" s="9" t="s">
@@ -12621,7 +12755,9 @@
       <c r="K27" s="6">
         <v>22736.35</v>
       </c>
-      <c r="L27" s="6"/>
+      <c r="L27" s="6">
+        <v>22633.87</v>
+      </c>
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
       <c r="P27" s="2" t="s">
@@ -12633,7 +12769,9 @@
       <c r="R27" s="6">
         <v>43235.06</v>
       </c>
-      <c r="S27" s="6"/>
+      <c r="S27" s="6">
+        <v>41078.31</v>
+      </c>
       <c r="T27" s="6"/>
       <c r="U27" s="6"/>
     </row>
@@ -12647,7 +12785,9 @@
       <c r="D28" s="6">
         <v>1761</v>
       </c>
-      <c r="E28" s="6"/>
+      <c r="E28" s="6">
+        <v>1738</v>
+      </c>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="I28" s="9" t="s">
@@ -12659,7 +12799,9 @@
       <c r="K28" s="6">
         <v>3200</v>
       </c>
-      <c r="L28" s="6"/>
+      <c r="L28" s="6">
+        <v>3198</v>
+      </c>
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
       <c r="P28" s="2" t="s">
@@ -12671,7 +12813,9 @@
       <c r="R28" s="6">
         <v>5002</v>
       </c>
-      <c r="S28" s="6"/>
+      <c r="S28" s="6">
+        <v>4990</v>
+      </c>
       <c r="T28" s="6"/>
       <c r="U28" s="6"/>
     </row>
@@ -12845,7 +12989,9 @@
       <c r="D34" s="6">
         <v>3467</v>
       </c>
-      <c r="E34" s="6"/>
+      <c r="E34" s="6">
+        <v>3467</v>
+      </c>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
       <c r="I34" s="9" t="s">
@@ -12857,7 +13003,9 @@
       <c r="K34" s="6">
         <v>7058</v>
       </c>
-      <c r="L34" s="6"/>
+      <c r="L34" s="6">
+        <v>7013</v>
+      </c>
       <c r="M34" s="6"/>
       <c r="N34" s="6"/>
       <c r="P34" s="2" t="s">
@@ -12869,7 +13017,9 @@
       <c r="R34" s="6">
         <v>9297</v>
       </c>
-      <c r="S34" s="6"/>
+      <c r="S34" s="6">
+        <v>8520</v>
+      </c>
       <c r="T34" s="6"/>
       <c r="U34" s="6"/>
     </row>
@@ -12883,7 +13033,9 @@
       <c r="D35" s="6">
         <v>5144.71</v>
       </c>
-      <c r="E35" s="6"/>
+      <c r="E35" s="6">
+        <v>5144.71</v>
+      </c>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
       <c r="I35" s="9" t="s">
@@ -12895,7 +13047,9 @@
       <c r="K35" s="6">
         <v>10518.73</v>
       </c>
-      <c r="L35" s="6"/>
+      <c r="L35" s="6">
+        <v>10518.73</v>
+      </c>
       <c r="M35" s="6"/>
       <c r="N35" s="6"/>
       <c r="P35" s="2" t="s">
@@ -12907,7 +13061,9 @@
       <c r="R35" s="6">
         <v>17010.05</v>
       </c>
-      <c r="S35" s="6"/>
+      <c r="S35" s="6">
+        <v>16562.79</v>
+      </c>
       <c r="T35" s="6"/>
       <c r="U35" s="6"/>
     </row>
@@ -12921,7 +13077,9 @@
       <c r="D36" s="6">
         <v>6684.86</v>
       </c>
-      <c r="E36" s="6"/>
+      <c r="E36" s="6">
+        <v>6712.4</v>
+      </c>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
       <c r="I36" s="9" t="s">
@@ -12933,7 +13091,9 @@
       <c r="K36" s="6">
         <v>16136.34</v>
       </c>
-      <c r="L36" s="6"/>
+      <c r="L36" s="6">
+        <v>15609.3</v>
+      </c>
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
       <c r="P36" s="2" t="s">
@@ -12945,7 +13105,9 @@
       <c r="R36" s="6">
         <v>22463.29</v>
       </c>
-      <c r="S36" s="6"/>
+      <c r="S36" s="6">
+        <v>21858.69</v>
+      </c>
       <c r="T36" s="6"/>
       <c r="U36" s="6"/>
     </row>
@@ -12959,7 +13121,9 @@
       <c r="D37" s="6">
         <v>8753.65</v>
       </c>
-      <c r="E37" s="6"/>
+      <c r="E37" s="6">
+        <v>8575.61</v>
+      </c>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
       <c r="I37" s="9" t="s">
@@ -12971,7 +13135,9 @@
       <c r="K37" s="6">
         <v>17508.68</v>
       </c>
-      <c r="L37" s="6"/>
+      <c r="L37" s="6">
+        <v>16811.29</v>
+      </c>
       <c r="M37" s="6"/>
       <c r="N37" s="6"/>
       <c r="P37" s="2" t="s">
@@ -12983,7 +13149,9 @@
       <c r="R37" s="6">
         <v>26270.54</v>
       </c>
-      <c r="S37" s="6"/>
+      <c r="S37" s="6">
+        <v>24999.08</v>
+      </c>
       <c r="T37" s="6"/>
       <c r="U37" s="6"/>
     </row>
@@ -12997,7 +13165,9 @@
       <c r="D38" s="6">
         <v>6073.32</v>
       </c>
-      <c r="E38" s="6"/>
+      <c r="E38" s="6">
+        <v>6073.32</v>
+      </c>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="I38" s="9" t="s">
@@ -13009,7 +13179,9 @@
       <c r="K38" s="6">
         <v>13173.97</v>
       </c>
-      <c r="L38" s="6"/>
+      <c r="L38" s="6">
+        <v>13003.85</v>
+      </c>
       <c r="M38" s="6"/>
       <c r="N38" s="6"/>
       <c r="P38" s="2" t="s">
@@ -13021,7 +13193,9 @@
       <c r="R38" s="6">
         <v>20957.67</v>
       </c>
-      <c r="S38" s="6"/>
+      <c r="S38" s="6">
+        <v>19373.25</v>
+      </c>
       <c r="T38" s="6"/>
       <c r="U38" s="6"/>
     </row>
@@ -13035,7 +13209,9 @@
       <c r="D39" s="6">
         <v>5464.73</v>
       </c>
-      <c r="E39" s="6"/>
+      <c r="E39" s="6">
+        <v>5464.73</v>
+      </c>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
       <c r="I39" s="9" t="s">
@@ -13047,7 +13223,9 @@
       <c r="K39" s="6">
         <v>14066.75</v>
       </c>
-      <c r="L39" s="6"/>
+      <c r="L39" s="6">
+        <v>14031.58</v>
+      </c>
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
       <c r="P39" s="2" t="s">
@@ -13059,7 +13237,9 @@
       <c r="R39" s="6">
         <v>21531.55</v>
       </c>
-      <c r="S39" s="6"/>
+      <c r="S39" s="6">
+        <v>20922.61</v>
+      </c>
       <c r="T39" s="6"/>
       <c r="U39" s="6"/>
     </row>
@@ -13073,7 +13253,9 @@
       <c r="D40" s="6">
         <v>6949.41</v>
       </c>
-      <c r="E40" s="6"/>
+      <c r="E40" s="6">
+        <v>6949.41</v>
+      </c>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
       <c r="I40" s="9" t="s">
@@ -13085,7 +13267,9 @@
       <c r="K40" s="6">
         <v>16931.06</v>
       </c>
-      <c r="L40" s="6"/>
+      <c r="L40" s="6">
+        <v>15920.92</v>
+      </c>
       <c r="M40" s="6"/>
       <c r="N40" s="6"/>
       <c r="P40" s="2" t="s">
@@ -13097,7 +13281,9 @@
       <c r="R40" s="6">
         <v>26280.18</v>
       </c>
-      <c r="S40" s="6"/>
+      <c r="S40" s="6">
+        <v>24079.93</v>
+      </c>
       <c r="T40" s="6"/>
       <c r="U40" s="6"/>
     </row>
@@ -13111,7 +13297,9 @@
       <c r="D41" s="6">
         <v>5019.55</v>
       </c>
-      <c r="E41" s="6"/>
+      <c r="E41" s="6">
+        <v>5019.55</v>
+      </c>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
       <c r="I41" s="9" t="s">
@@ -13123,7 +13311,9 @@
       <c r="K41" s="6">
         <v>13162.44</v>
       </c>
-      <c r="L41" s="6"/>
+      <c r="L41" s="6">
+        <v>12531.41</v>
+      </c>
       <c r="M41" s="6"/>
       <c r="N41" s="6"/>
       <c r="P41" s="2" t="s">
@@ -13135,7 +13325,9 @@
       <c r="R41" s="6">
         <v>18432.02</v>
       </c>
-      <c r="S41" s="6"/>
+      <c r="S41" s="6">
+        <v>16805.21</v>
+      </c>
       <c r="T41" s="6"/>
       <c r="U41" s="6"/>
     </row>
@@ -13149,7 +13341,9 @@
       <c r="D42" s="6">
         <v>5506.58</v>
       </c>
-      <c r="E42" s="6"/>
+      <c r="E42" s="6">
+        <v>5427.1</v>
+      </c>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
       <c r="I42" s="9" t="s">
@@ -13161,7 +13355,9 @@
       <c r="K42" s="6">
         <v>11215</v>
       </c>
-      <c r="L42" s="6"/>
+      <c r="L42" s="6">
+        <v>11143.51</v>
+      </c>
       <c r="M42" s="6"/>
       <c r="N42" s="6"/>
       <c r="P42" s="2" t="s">
@@ -13173,7 +13369,9 @@
       <c r="R42" s="6">
         <v>16747.59</v>
       </c>
-      <c r="S42" s="6"/>
+      <c r="S42" s="6">
+        <v>15855.52</v>
+      </c>
       <c r="T42" s="6"/>
       <c r="U42" s="6"/>
     </row>
@@ -13187,7 +13385,9 @@
       <c r="D43" s="6">
         <v>4039.09</v>
       </c>
-      <c r="E43" s="6"/>
+      <c r="E43" s="6">
+        <v>4039.09</v>
+      </c>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
       <c r="I43" s="9" t="s">
@@ -13199,7 +13399,9 @@
       <c r="K43" s="6">
         <v>10347.79</v>
       </c>
-      <c r="L43" s="6"/>
+      <c r="L43" s="6">
+        <v>10144.8</v>
+      </c>
       <c r="M43" s="6"/>
       <c r="N43" s="6"/>
       <c r="P43" s="2" t="s">
@@ -13211,7 +13413,9 @@
       <c r="R43" s="6">
         <v>17277.53</v>
       </c>
-      <c r="S43" s="6"/>
+      <c r="S43" s="6">
+        <v>17007.59</v>
+      </c>
       <c r="T43" s="6"/>
       <c r="U43" s="6"/>
     </row>
@@ -13225,7 +13429,9 @@
       <c r="D44" s="6">
         <v>1978.97</v>
       </c>
-      <c r="E44" s="6"/>
+      <c r="E44" s="6">
+        <v>1944.45</v>
+      </c>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="I44" s="9" t="s">
@@ -13237,7 +13443,9 @@
       <c r="K44" s="6">
         <v>5871.04</v>
       </c>
-      <c r="L44" s="6"/>
+      <c r="L44" s="6">
+        <v>5778.77</v>
+      </c>
       <c r="M44" s="6"/>
       <c r="N44" s="6"/>
       <c r="P44" s="2" t="s">
@@ -13249,7 +13457,9 @@
       <c r="R44" s="6">
         <v>8702.64</v>
       </c>
-      <c r="S44" s="6"/>
+      <c r="S44" s="6">
+        <v>8601.15</v>
+      </c>
       <c r="T44" s="6"/>
       <c r="U44" s="6"/>
     </row>
@@ -13263,7 +13473,9 @@
       <c r="D45" s="6">
         <v>9092.91</v>
       </c>
-      <c r="E45" s="6"/>
+      <c r="E45" s="6">
+        <v>8988.94</v>
+      </c>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
       <c r="I45" s="9" t="s">
@@ -13275,7 +13487,9 @@
       <c r="K45" s="6">
         <v>21968.62</v>
       </c>
-      <c r="L45" s="6"/>
+      <c r="L45" s="6">
+        <v>21184.39</v>
+      </c>
       <c r="M45" s="6"/>
       <c r="N45" s="6"/>
       <c r="P45" s="2" t="s">
@@ -13287,7 +13501,9 @@
       <c r="R45" s="6">
         <v>32158.06</v>
       </c>
-      <c r="S45" s="6"/>
+      <c r="S45" s="6">
+        <v>30699.83</v>
+      </c>
       <c r="T45" s="6"/>
       <c r="U45" s="6"/>
     </row>
@@ -13333,7 +13549,9 @@
       <c r="D47" s="6">
         <v>912</v>
       </c>
-      <c r="E47" s="6"/>
+      <c r="E47" s="6">
+        <v>889</v>
+      </c>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
       <c r="I47" s="9" t="s">
@@ -13345,7 +13563,9 @@
       <c r="K47" s="6">
         <v>1643</v>
       </c>
-      <c r="L47" s="6"/>
+      <c r="L47" s="6">
+        <v>1587</v>
+      </c>
       <c r="M47" s="6"/>
       <c r="N47" s="6"/>
       <c r="P47" s="2" t="s">
@@ -13357,7 +13577,9 @@
       <c r="R47" s="6">
         <v>2576</v>
       </c>
-      <c r="S47" s="6"/>
+      <c r="S47" s="6">
+        <v>2527</v>
+      </c>
       <c r="T47" s="6"/>
       <c r="U47" s="6"/>
     </row>
@@ -13371,7 +13593,9 @@
       <c r="D48" s="6">
         <v>27867.43</v>
       </c>
-      <c r="E48" s="6"/>
+      <c r="E48" s="6">
+        <v>27867.43</v>
+      </c>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
       <c r="I48" s="9" t="s">
@@ -13383,7 +13607,9 @@
       <c r="K48" s="6">
         <v>59008.16</v>
       </c>
-      <c r="L48" s="6"/>
+      <c r="L48" s="6">
+        <v>55887.14</v>
+      </c>
       <c r="M48" s="6"/>
       <c r="N48" s="6"/>
       <c r="P48" s="2" t="s">
@@ -13395,7 +13621,9 @@
       <c r="R48" s="6">
         <v>80905.41</v>
       </c>
-      <c r="S48" s="6"/>
+      <c r="S48" s="6">
+        <v>77734.18</v>
+      </c>
       <c r="T48" s="6"/>
       <c r="U48" s="6"/>
     </row>
@@ -13409,7 +13637,9 @@
       <c r="D49" s="6">
         <v>6949.45</v>
       </c>
-      <c r="E49" s="6"/>
+      <c r="E49" s="6">
+        <v>6949.45</v>
+      </c>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
       <c r="I49" s="9" t="s">
@@ -13421,7 +13651,9 @@
       <c r="K49" s="6">
         <v>14343.7</v>
       </c>
-      <c r="L49" s="6"/>
+      <c r="L49" s="6">
+        <v>14342.7</v>
+      </c>
       <c r="M49" s="6"/>
       <c r="N49" s="6"/>
       <c r="P49" s="2" t="s">
@@ -13433,7 +13665,9 @@
       <c r="R49" s="6">
         <v>29443.65</v>
       </c>
-      <c r="S49" s="6"/>
+      <c r="S49" s="6">
+        <v>29443.65</v>
+      </c>
       <c r="T49" s="6"/>
       <c r="U49" s="6"/>
     </row>
@@ -13447,7 +13681,9 @@
       <c r="D50" s="6">
         <v>10773.88</v>
       </c>
-      <c r="E50" s="6"/>
+      <c r="E50" s="6">
+        <v>10773.88</v>
+      </c>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="I50" s="9" t="s">
@@ -13459,7 +13695,9 @@
       <c r="K50" s="6">
         <v>24735.67</v>
       </c>
-      <c r="L50" s="6"/>
+      <c r="L50" s="6">
+        <v>24476.41</v>
+      </c>
       <c r="M50" s="6"/>
       <c r="N50" s="6"/>
       <c r="P50" s="2" t="s">
@@ -13471,7 +13709,9 @@
       <c r="R50" s="6">
         <v>41719.05</v>
       </c>
-      <c r="S50" s="6"/>
+      <c r="S50" s="6">
+        <v>40845.75</v>
+      </c>
       <c r="T50" s="6"/>
       <c r="U50" s="6"/>
     </row>
@@ -13485,7 +13725,9 @@
       <c r="D51" s="6">
         <v>23583.58</v>
       </c>
-      <c r="E51" s="6"/>
+      <c r="E51" s="6">
+        <v>23556.22</v>
+      </c>
       <c r="F51" s="6"/>
       <c r="G51" s="6"/>
       <c r="I51" s="9" t="s">
@@ -13497,7 +13739,9 @@
       <c r="K51" s="6">
         <v>56540.67</v>
       </c>
-      <c r="L51" s="6"/>
+      <c r="L51" s="6">
+        <v>55898.53</v>
+      </c>
       <c r="M51" s="6"/>
       <c r="N51" s="6"/>
       <c r="P51" s="2" t="s">
@@ -13509,7 +13753,9 @@
       <c r="R51" s="6">
         <v>77115.68</v>
       </c>
-      <c r="S51" s="6"/>
+      <c r="S51" s="6">
+        <v>75192.45</v>
+      </c>
       <c r="T51" s="6"/>
       <c r="U51" s="6"/>
     </row>
@@ -13523,7 +13769,9 @@
       <c r="D52" s="6">
         <v>12002.27</v>
       </c>
-      <c r="E52" s="6"/>
+      <c r="E52" s="6">
+        <v>11971.75</v>
+      </c>
       <c r="F52" s="6"/>
       <c r="G52" s="6"/>
       <c r="I52" s="9" t="s">
@@ -13535,7 +13783,9 @@
       <c r="K52" s="6">
         <v>27761.39</v>
       </c>
-      <c r="L52" s="6"/>
+      <c r="L52" s="6">
+        <v>27703.56</v>
+      </c>
       <c r="M52" s="6"/>
       <c r="N52" s="6"/>
       <c r="P52" s="2" t="s">
@@ -13547,7 +13797,9 @@
       <c r="R52" s="6">
         <v>43611.16</v>
       </c>
-      <c r="S52" s="6"/>
+      <c r="S52" s="6">
+        <v>43404.22</v>
+      </c>
       <c r="T52" s="6"/>
       <c r="U52" s="6"/>
     </row>
@@ -13561,7 +13813,9 @@
       <c r="D53" s="6">
         <v>14499.54</v>
       </c>
-      <c r="E53" s="6"/>
+      <c r="E53" s="6">
+        <v>13879.3</v>
+      </c>
       <c r="F53" s="6"/>
       <c r="G53" s="6"/>
       <c r="I53" s="9" t="s">
@@ -13573,7 +13827,9 @@
       <c r="K53" s="6">
         <v>34387.76</v>
       </c>
-      <c r="L53" s="6"/>
+      <c r="L53" s="6">
+        <v>33085.15</v>
+      </c>
       <c r="M53" s="6"/>
       <c r="N53" s="6"/>
       <c r="P53" s="2" t="s">
@@ -13585,7 +13841,9 @@
       <c r="R53" s="6">
         <v>50734.22</v>
       </c>
-      <c r="S53" s="6"/>
+      <c r="S53" s="6">
+        <v>48477</v>
+      </c>
       <c r="T53" s="6"/>
       <c r="U53" s="6"/>
     </row>
@@ -13599,7 +13857,9 @@
       <c r="D54" s="6">
         <v>24798.56</v>
       </c>
-      <c r="E54" s="6"/>
+      <c r="E54" s="6">
+        <v>24646.4</v>
+      </c>
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
       <c r="I54" s="9" t="s">
@@ -13611,7 +13871,9 @@
       <c r="K54" s="6">
         <v>47942.46</v>
       </c>
-      <c r="L54" s="6"/>
+      <c r="L54" s="6">
+        <v>46340.72</v>
+      </c>
       <c r="M54" s="6"/>
       <c r="N54" s="6"/>
       <c r="P54" s="2" t="s">
@@ -13623,7 +13885,9 @@
       <c r="R54" s="6">
         <v>74432.27</v>
       </c>
-      <c r="S54" s="6"/>
+      <c r="S54" s="6">
+        <v>72419.51</v>
+      </c>
       <c r="T54" s="6"/>
       <c r="U54" s="6"/>
     </row>
@@ -13637,7 +13901,9 @@
       <c r="D55" s="6">
         <v>8128.35</v>
       </c>
-      <c r="E55" s="6"/>
+      <c r="E55" s="6">
+        <v>8128.35</v>
+      </c>
       <c r="F55" s="6"/>
       <c r="G55" s="6"/>
       <c r="I55" s="9" t="s">
@@ -13649,7 +13915,9 @@
       <c r="K55" s="6">
         <v>26633.21</v>
       </c>
-      <c r="L55" s="6"/>
+      <c r="L55" s="6">
+        <v>25908.84</v>
+      </c>
       <c r="M55" s="6"/>
       <c r="N55" s="6"/>
       <c r="P55" s="2" t="s">
@@ -13661,7 +13929,9 @@
       <c r="R55" s="6">
         <v>34776.92</v>
       </c>
-      <c r="S55" s="6"/>
+      <c r="S55" s="6">
+        <v>34125.69</v>
+      </c>
       <c r="T55" s="6"/>
       <c r="U55" s="6"/>
     </row>
@@ -13675,7 +13945,9 @@
       <c r="D56" s="6">
         <v>12734.4</v>
       </c>
-      <c r="E56" s="6"/>
+      <c r="E56" s="6">
+        <v>12178.74</v>
+      </c>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
       <c r="I56" s="9" t="s">
@@ -13687,7 +13959,9 @@
       <c r="K56" s="6">
         <v>27358.78</v>
       </c>
-      <c r="L56" s="6"/>
+      <c r="L56" s="6">
+        <v>25755.28</v>
+      </c>
       <c r="M56" s="6"/>
       <c r="N56" s="6"/>
       <c r="P56" s="2" t="s">
@@ -13699,7 +13973,9 @@
       <c r="R56" s="6">
         <v>41039.33</v>
       </c>
-      <c r="S56" s="6"/>
+      <c r="S56" s="6">
+        <v>37324.59</v>
+      </c>
       <c r="T56" s="6"/>
       <c r="U56" s="6"/>
     </row>
@@ -13713,7 +13989,9 @@
       <c r="D57" s="6">
         <v>27132.56</v>
       </c>
-      <c r="E57" s="6"/>
+      <c r="E57" s="6">
+        <v>25467.89</v>
+      </c>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
       <c r="I57" s="9" t="s">
@@ -13725,7 +14003,9 @@
       <c r="K57" s="6">
         <v>45681.07</v>
       </c>
-      <c r="L57" s="6"/>
+      <c r="L57" s="6">
+        <v>43072.93</v>
+      </c>
       <c r="M57" s="6"/>
       <c r="N57" s="6"/>
       <c r="P57" s="2" t="s">
@@ -13737,7 +14017,9 @@
       <c r="R57" s="6">
         <v>76594.64</v>
       </c>
-      <c r="S57" s="6"/>
+      <c r="S57" s="6">
+        <v>74262.41</v>
+      </c>
       <c r="T57" s="6"/>
       <c r="U57" s="6"/>
     </row>
@@ -13783,7 +14065,9 @@
       <c r="D59" s="6">
         <v>366.6</v>
       </c>
-      <c r="E59" s="6"/>
+      <c r="E59" s="6">
+        <v>354.89</v>
+      </c>
       <c r="F59" s="6"/>
       <c r="G59" s="6"/>
       <c r="I59" s="9" t="s">
@@ -13795,7 +14079,9 @@
       <c r="K59" s="6">
         <v>710.33</v>
       </c>
-      <c r="L59" s="6"/>
+      <c r="L59" s="6">
+        <v>620.37</v>
+      </c>
       <c r="M59" s="6"/>
       <c r="N59" s="6"/>
       <c r="P59" s="2" t="s">
@@ -13807,7 +14093,9 @@
       <c r="R59" s="6">
         <v>1052.57</v>
       </c>
-      <c r="S59" s="6"/>
+      <c r="S59" s="6">
+        <v>934.35</v>
+      </c>
       <c r="T59" s="6"/>
       <c r="U59" s="6"/>
     </row>
@@ -13821,7 +14109,9 @@
       <c r="D60" s="6">
         <v>616.22</v>
       </c>
-      <c r="E60" s="6"/>
+      <c r="E60" s="6">
+        <v>586.25</v>
+      </c>
       <c r="F60" s="6"/>
       <c r="G60" s="6"/>
       <c r="I60" s="9" t="s">
@@ -13833,7 +14123,9 @@
       <c r="K60" s="6">
         <v>1295</v>
       </c>
-      <c r="L60" s="6"/>
+      <c r="L60" s="6">
+        <v>1231.83</v>
+      </c>
       <c r="M60" s="6"/>
       <c r="N60" s="6"/>
       <c r="P60" s="2" t="s">
@@ -13845,7 +14137,9 @@
       <c r="R60" s="6">
         <v>1973.92</v>
       </c>
-      <c r="S60" s="6"/>
+      <c r="S60" s="6">
+        <v>1846.98</v>
+      </c>
       <c r="T60" s="6"/>
       <c r="U60" s="6"/>
     </row>
@@ -13859,7 +14153,9 @@
       <c r="D61" s="6">
         <v>1827.72</v>
       </c>
-      <c r="E61" s="6"/>
+      <c r="E61" s="6">
+        <v>1773.27</v>
+      </c>
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
       <c r="I61" s="9" t="s">
@@ -13871,7 +14167,9 @@
       <c r="K61" s="6">
         <v>3850</v>
       </c>
-      <c r="L61" s="6"/>
+      <c r="L61" s="6">
+        <v>3654.255</v>
+      </c>
       <c r="M61" s="6"/>
       <c r="N61" s="6"/>
       <c r="P61" s="2" t="s">
@@ -13883,7 +14181,9 @@
       <c r="R61" s="6">
         <v>5797.76</v>
       </c>
-      <c r="S61" s="6"/>
+      <c r="S61" s="6">
+        <v>5499.61</v>
+      </c>
       <c r="T61" s="6"/>
       <c r="U61" s="6"/>
     </row>
@@ -13897,7 +14197,9 @@
       <c r="D62" s="6">
         <v>2438.46</v>
       </c>
-      <c r="E62" s="6"/>
+      <c r="E62" s="6">
+        <v>2256.22</v>
+      </c>
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
       <c r="I62" s="9" t="s">
@@ -13919,7 +14221,9 @@
       <c r="R62" s="6">
         <v>7612.84</v>
       </c>
-      <c r="S62" s="6"/>
+      <c r="S62" s="6">
+        <v>7170.59</v>
+      </c>
       <c r="T62" s="6"/>
       <c r="U62" s="6"/>
     </row>
@@ -13933,7 +14237,9 @@
       <c r="D63" s="6">
         <v>5202</v>
       </c>
-      <c r="E63" s="6"/>
+      <c r="E63" s="6">
+        <v>5202</v>
+      </c>
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
       <c r="I63" s="9" t="s">
@@ -13945,7 +14251,9 @@
       <c r="K63" s="6">
         <v>10389</v>
       </c>
-      <c r="L63" s="6"/>
+      <c r="L63" s="6">
+        <v>10348</v>
+      </c>
       <c r="M63" s="6"/>
       <c r="N63" s="6"/>
       <c r="P63" s="2" t="s">
@@ -13957,7 +14265,9 @@
       <c r="R63" s="6">
         <v>15780</v>
       </c>
-      <c r="S63" s="6"/>
+      <c r="S63" s="6">
+        <v>15741</v>
+      </c>
       <c r="T63" s="6"/>
       <c r="U63" s="6"/>
     </row>
@@ -13971,7 +14281,9 @@
       <c r="D64" s="6">
         <v>12053</v>
       </c>
-      <c r="E64" s="6"/>
+      <c r="E64" s="6">
+        <v>12026</v>
+      </c>
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
       <c r="I64" s="9" t="s">
@@ -13983,7 +14295,9 @@
       <c r="K64" s="6">
         <v>23225</v>
       </c>
-      <c r="L64" s="6"/>
+      <c r="L64" s="6">
+        <v>23218</v>
+      </c>
       <c r="M64" s="6"/>
       <c r="N64" s="6"/>
       <c r="P64" s="2" t="s">
@@ -13995,7 +14309,9 @@
       <c r="R64" s="6">
         <v>35940</v>
       </c>
-      <c r="S64" s="6"/>
+      <c r="S64" s="6">
+        <v>35913</v>
+      </c>
       <c r="T64" s="6"/>
       <c r="U64" s="6"/>
     </row>
@@ -14041,7 +14357,9 @@
       <c r="D66" s="6">
         <v>102.42</v>
       </c>
-      <c r="E66" s="6"/>
+      <c r="E66" s="6">
+        <v>102.42</v>
+      </c>
       <c r="F66" s="6"/>
       <c r="G66" s="6"/>
       <c r="I66" s="9" t="s">
@@ -14053,7 +14371,9 @@
       <c r="K66" s="6">
         <v>281.96</v>
       </c>
-      <c r="L66" s="6"/>
+      <c r="L66" s="6">
+        <v>281.96</v>
+      </c>
       <c r="M66" s="6"/>
       <c r="N66" s="6"/>
       <c r="P66" s="2" t="s">
@@ -14065,7 +14385,9 @@
       <c r="R66" s="6">
         <v>474.46</v>
       </c>
-      <c r="S66" s="6"/>
+      <c r="S66" s="6">
+        <v>457.08</v>
+      </c>
       <c r="T66" s="6"/>
       <c r="U66" s="6"/>
     </row>
@@ -14079,7 +14401,9 @@
       <c r="D67" s="6">
         <v>152</v>
       </c>
-      <c r="E67" s="6"/>
+      <c r="E67" s="6">
+        <v>152</v>
+      </c>
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
       <c r="I67" s="9" t="s">
@@ -14091,7 +14415,9 @@
       <c r="K67" s="6">
         <v>609</v>
       </c>
-      <c r="L67" s="6"/>
+      <c r="L67" s="6">
+        <v>599</v>
+      </c>
       <c r="M67" s="6"/>
       <c r="N67" s="6"/>
       <c r="P67" s="2" t="s">
@@ -14103,7 +14429,9 @@
       <c r="R67" s="6">
         <v>860</v>
       </c>
-      <c r="S67" s="6"/>
+      <c r="S67" s="6">
+        <v>806</v>
+      </c>
       <c r="T67" s="6"/>
       <c r="U67" s="6"/>
     </row>
@@ -14117,7 +14445,9 @@
       <c r="D68" s="6">
         <v>36118.03</v>
       </c>
-      <c r="E68" s="6"/>
+      <c r="E68" s="6">
+        <v>31239.35</v>
+      </c>
       <c r="F68" s="6"/>
       <c r="G68" s="6"/>
       <c r="I68" s="9" t="s">
@@ -14129,7 +14459,9 @@
       <c r="K68" s="6">
         <v>69289.87</v>
       </c>
-      <c r="L68" s="6"/>
+      <c r="L68" s="6">
+        <v>63679.49</v>
+      </c>
       <c r="M68" s="6"/>
       <c r="N68" s="6"/>
       <c r="P68" s="2" t="s">
@@ -14141,7 +14473,9 @@
       <c r="R68" s="6">
         <v>119846.32</v>
       </c>
-      <c r="S68" s="6"/>
+      <c r="S68" s="6">
+        <v>101426.26</v>
+      </c>
       <c r="T68" s="6"/>
       <c r="U68" s="6"/>
     </row>
@@ -14155,7 +14489,9 @@
       <c r="D69" s="6">
         <v>1063.31</v>
       </c>
-      <c r="E69" s="6"/>
+      <c r="E69" s="6">
+        <v>1006.78</v>
+      </c>
       <c r="F69" s="6"/>
       <c r="G69" s="6"/>
       <c r="I69" s="9" t="s">
@@ -14167,7 +14503,9 @@
       <c r="K69" s="6">
         <v>2213.78</v>
       </c>
-      <c r="L69" s="6"/>
+      <c r="L69" s="6">
+        <v>2129.31</v>
+      </c>
       <c r="M69" s="6"/>
       <c r="N69" s="6"/>
       <c r="P69" s="2" t="s">
@@ -14179,7 +14517,9 @@
       <c r="R69" s="6">
         <v>3191.36</v>
       </c>
-      <c r="S69" s="6"/>
+      <c r="S69" s="6">
+        <v>2959.47</v>
+      </c>
       <c r="T69" s="6"/>
       <c r="U69" s="6"/>
     </row>
@@ -14193,7 +14533,9 @@
       <c r="D70" s="6">
         <v>751.06</v>
       </c>
-      <c r="E70" s="6"/>
+      <c r="E70" s="6">
+        <v>751.06</v>
+      </c>
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
       <c r="I70" s="9" t="s">
@@ -14205,7 +14547,9 @@
       <c r="K70" s="6">
         <v>1511.76</v>
       </c>
-      <c r="L70" s="6"/>
+      <c r="L70" s="6">
+        <v>1511.75</v>
+      </c>
       <c r="M70" s="6"/>
       <c r="N70" s="6"/>
       <c r="P70" s="2" t="s">
@@ -14217,7 +14561,9 @@
       <c r="R70" s="6">
         <v>2777.32</v>
       </c>
-      <c r="S70" s="6"/>
+      <c r="S70" s="6">
+        <v>2777.32</v>
+      </c>
       <c r="T70" s="6"/>
       <c r="U70" s="6"/>
     </row>
@@ -14231,7 +14577,9 @@
       <c r="D71" s="6">
         <v>784.47</v>
       </c>
-      <c r="E71" s="6"/>
+      <c r="E71" s="6">
+        <v>784.47</v>
+      </c>
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
       <c r="I71" s="9" t="s">
@@ -14243,7 +14591,9 @@
       <c r="K71" s="6">
         <v>2613.9</v>
       </c>
-      <c r="L71" s="6"/>
+      <c r="L71" s="6">
+        <v>2573.69</v>
+      </c>
       <c r="M71" s="6"/>
       <c r="N71" s="6"/>
       <c r="P71" s="2" t="s">
@@ -14255,7 +14605,9 @@
       <c r="R71" s="6">
         <v>2986.61</v>
       </c>
-      <c r="S71" s="6"/>
+      <c r="S71" s="6">
+        <v>2986.61</v>
+      </c>
       <c r="T71" s="6"/>
       <c r="U71" s="6"/>
     </row>

</xml_diff>

<commit_message>
Atualização da análise completa
</commit_message>
<xml_diff>
--- a/Comparaçoes/BuscasLocais.xlsx
+++ b/Comparaçoes/BuscasLocais.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13725" windowHeight="12885" tabRatio="500" firstSheet="1" activeTab="2"/>
+    <workbookView windowWidth="14925" windowHeight="12885" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="k = n|4" sheetId="1" r:id="rId1"/>
@@ -309,11 +309,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="180" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -335,6 +335,13 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color rgb="FF44546A"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
@@ -342,19 +349,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -401,13 +396,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color rgb="FF44546A"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color rgb="FF44546A"/>
       <name val="Calibri"/>
@@ -422,7 +410,33 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -434,22 +448,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -469,7 +469,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFF2CA"/>
+        <fgColor rgb="FF5B9BD5"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4AF82"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9BC2E6"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF70AD47"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8EA9DB"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE697"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -481,19 +523,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFE697"/>
+        <fgColor rgb="FFB4C6E7"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFF2CA"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFED7D31"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -505,55 +547,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFED7D31"/>
+        <fgColor rgb="FFFFD964"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFBDD7EE"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF70AD47"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF8CAAB"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE1EFD8"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB4C6E7"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC5DFB3"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDEBF7"/>
+        <fgColor rgb="FFFBE3D5"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -571,7 +571,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FFC5DFB3"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA8D08C"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8CAAB"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC7C7C7"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -589,61 +625,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF5B9BD5"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFD964"/>
+        <fgColor rgb="FFBDD7EE"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF4AF82"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF9BC2E6"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA8D08C"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8EA9DB"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC7C7C7"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFBE3D5"/>
+        <fgColor rgb="FFE1EFD8"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -860,6 +860,15 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color rgb="FF5B9BD5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -900,15 +909,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color rgb="FF5B9BD5"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color rgb="FFACCCEA"/>
       </bottom>
       <diagonal/>
@@ -929,6 +929,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF5B9BD5"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF5B9BD5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -943,17 +954,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF5B9BD5"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF5B9BD5"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -962,43 +962,46 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1007,100 +1010,97 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1111,43 +1111,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1165,13 +1165,13 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1183,13 +1183,13 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1201,7 +1201,7 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1523,8 +1523,8 @@
   <sheetPr/>
   <dimension ref="B2:BK28"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="BE53" sqref="BE53"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="BA21" sqref="BA21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -4686,7 +4686,7 @@
         <v>12012</v>
       </c>
       <c r="BA21" s="7">
-        <v>11838</v>
+        <v>0</v>
       </c>
       <c r="BB21" s="22">
         <v>12196</v>
@@ -9898,7 +9898,7 @@
   <sheetPr/>
   <dimension ref="B2:BK28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="AW1" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="BE32" sqref="BE32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Atualização da analise completa
</commit_message>
<xml_diff>
--- a/Comparaçoes/BuscasLocais.xlsx
+++ b/Comparaçoes/BuscasLocais.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14925" windowHeight="12885" tabRatio="500"/>
+    <workbookView windowWidth="13725" windowHeight="12885" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="k = n|4" sheetId="1" r:id="rId1"/>
@@ -309,11 +309,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -342,8 +342,35 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF44546A"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -361,9 +388,42 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF44546A"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF44546A"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -375,52 +435,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color rgb="FF44546A"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color rgb="FF44546A"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF44546A"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -428,28 +442,14 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -469,37 +469,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF5B9BD5"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF4AF82"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF9BC2E6"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF70AD47"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF8EA9DB"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
+        <fgColor rgb="FFD9E1F2"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -511,67 +505,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFEBEBEB"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFE697"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB4C6E7"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFF2CA"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFED7D31"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEBEBEB"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFD964"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFBE3D5"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9E1F2"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4472C4"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC5DFB3"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -589,7 +541,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFBE3D5"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9BC2E6"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC5DFB3"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4AF82"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFED7D31"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4472C4"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -601,25 +589,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDDEBF7"/>
+        <fgColor rgb="FF70AD47"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFB4C6E7"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFD964"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FF5B9BD5"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBDD7EE"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -631,19 +625,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFBDD7EE"/>
+        <fgColor rgb="FFDDEBF7"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFF2CA"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE1EFD8"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8EA9DB"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
@@ -866,6 +866,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -890,6 +920,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFACCCEA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -907,30 +946,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFACCCEA"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color rgb="FF5B9BD5"/>
       </top>
@@ -939,30 +954,15 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -971,136 +971,136 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="23" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1111,43 +1111,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1165,13 +1165,13 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1183,13 +1183,13 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1201,7 +1201,7 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1523,7 +1523,7 @@
   <sheetPr/>
   <dimension ref="B2:BK28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="AR1" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="AR1" workbookViewId="0">
       <selection activeCell="BA21" sqref="BA21"/>
     </sheetView>
   </sheetViews>
@@ -5721,14 +5721,14 @@
   <sheetPr/>
   <dimension ref="B2:BK28"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="AV1" workbookViewId="0">
-      <selection activeCell="BF29" sqref="BF29"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="BB28" sqref="BB28:BC28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="2" width="9.14285714285714" style="9" customWidth="1"/>
-    <col min="3" max="3" width="19.5714285714286" style="9" customWidth="1"/>
+    <col min="3" max="3" width="5.3047619047619" style="9" customWidth="1"/>
     <col min="4" max="4" width="9.75238095238095" style="9" customWidth="1"/>
     <col min="5" max="5" width="10.5714285714286" style="9" customWidth="1"/>
     <col min="6" max="7" width="9.93333333333333" style="9" customWidth="1"/>
@@ -5736,13 +5736,13 @@
     <col min="9" max="14" width="9.14285714285714" style="9" customWidth="1"/>
     <col min="15" max="15" width="10.2857142857143" style="9" customWidth="1"/>
     <col min="16" max="23" width="9.14285714285714" style="9" customWidth="1"/>
-    <col min="24" max="24" width="17.0095238095238" style="9" customWidth="1"/>
+    <col min="24" max="24" width="6.73333333333333" style="9" customWidth="1"/>
     <col min="25" max="25" width="9.75238095238095" style="9" customWidth="1"/>
     <col min="26" max="26" width="10.5714285714286" style="9" customWidth="1"/>
     <col min="27" max="28" width="9.75238095238095" style="9" customWidth="1"/>
     <col min="29" max="30" width="9.57142857142857" style="9" customWidth="1"/>
     <col min="31" max="44" width="9.14285714285714" style="9" customWidth="1"/>
-    <col min="45" max="45" width="19.5714285714286" style="9" customWidth="1"/>
+    <col min="45" max="45" width="9.39047619047619" style="9" customWidth="1"/>
     <col min="46" max="49" width="10.8571428571429" style="9" customWidth="1"/>
     <col min="50" max="51" width="9.57142857142857" style="9" customWidth="1"/>
     <col min="52" max="16384" width="9.14285714285714" style="9" customWidth="1"/>
@@ -9898,14 +9898,14 @@
   <sheetPr/>
   <dimension ref="B2:BK28"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="BE32" sqref="BE32"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="AZ16" sqref="AZ16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="2" width="9.14285714285714" style="9" customWidth="1"/>
-    <col min="3" max="3" width="19.5714285714286" style="9" customWidth="1"/>
+    <col min="3" max="3" width="7.55238095238095" style="9" customWidth="1"/>
     <col min="4" max="4" width="9.75238095238095" style="9" customWidth="1"/>
     <col min="5" max="5" width="10.5714285714286" style="9" customWidth="1"/>
     <col min="6" max="7" width="9.75238095238095" style="9" customWidth="1"/>
@@ -9921,7 +9921,7 @@
     <col min="29" max="30" width="9.57142857142857" style="9" customWidth="1"/>
     <col min="31" max="43" width="9.14285714285714" style="9" customWidth="1"/>
     <col min="44" max="44" width="11.1428571428571" style="9" customWidth="1"/>
-    <col min="45" max="45" width="19.5714285714286" style="9" customWidth="1"/>
+    <col min="45" max="45" width="11.6285714285714" style="9" customWidth="1"/>
     <col min="46" max="49" width="10.8571428571429" style="9" customWidth="1"/>
     <col min="50" max="50" width="9.57142857142857" style="9" customWidth="1"/>
     <col min="51" max="51" width="8.76190476190476" style="9" customWidth="1"/>
@@ -14070,7 +14070,7 @@
   <sheetPr/>
   <dimension ref="B2:U71"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="K43" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" topLeftCell="K1" workbookViewId="0">
       <selection activeCell="R48" sqref="R48:U71"/>
     </sheetView>
   </sheetViews>

</xml_diff>